<commit_message>
Reestructuration of preprocessing, Add name to corpus excels
</commit_message>
<xml_diff>
--- a/corpus/test.xlsx
+++ b/corpus/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>class</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -451,11 +456,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>vayas muro andrea stella nervioso hacía bailaba pie derecho fernando alonso volaba asfalto shanghai rápido respondió tranquilidad jefe fórmula piloto volvió demostrar piloto mundo asturiano ofreció lección pilotaje inteligencia ganador ganó diez segundos ventaja kimi raikkonen doce lewis hamilton podio campeones carrera sebastian vettel cuarto jenson button quinto campeones mundo primeras posicionesveníamos advirtiendo alonso opciones victoria estrella ferrari coche competitivo trabajado duro piloto necesita dato preocupante felipe massa terminó sexto cuarenta segundos compañero ¿cuál realidadpues opiniones hechos evidente alonso preveían dispone coche jefe amo recuerdan asturiano disfruta valen dinero representante costar jefe jerez subió minardi cogía monoplaza consiguió renault dibujaba estrellas pista ofreció españoles deporte emocionarse sentirse orgullososdespués hamilton golpe tantas vettel títulos perdidos carrera desistió confiar genio asturiano pensaba sonrisas equivocaban ferrari esperaban optimistas presagiaban males eternos cuarto año dispone coche talento máscomenzó carrera tercero puso intentó meter coche hamilton llegaba vettel monstruo galletas neumáticos duros amenazando posiciones asturiano entró cambiar neumáticos medios vuelta comenzó carrera lucha hamilton kimi sebastian vuelta fernando adelantar di resta pérez button vettel hulkenberg pone líder tricampeón sonreír fernando gustándose parecía recta famoso drs sorprendió curva asturiano emocionó afición española esperaba sueño ferrari amo señor carrera hamilton raikkonen vettel intentando estrategia blandos funcionara alemán terminó cuarto estela hamilton sufría gomas medalla chocolate compañero mark webber rueda primeras vueltas pasan alonso luchar mundial terminado carreras ganó abandono malaisia líder destacado vettel kimi asturiano eterno capaz cantar himno letra miles chinos banderas españolas asturianas alonso vuelve jefe</t>
+          <t>hugo gonzález semifinal espaldanatación terminator titmus vence ledecky libera ira entrenadormichael phelps nado díasahmed hafnaoui tunecino años orgullo áfrica piscinaaustralia valquirias logran récord tokiode octavo cuarto metros hugo gonzález progresión espectacular arañar olímpica espalda prueba estrella estilos campeón europeo mayo contacto accedió séptimo semifinalistas llevará calle importante amortiguar presión mallorquín años rostro futuro natación española otoño mireia belmontela semifinal exigente dada calidad rivales rusos bandera olímpica klement kolesnikov yevgueni rylov contrario finales suele beneficioso obtener clasificación dadas referencias ofrecen sucedió mireia semifinales directas estilos riesgo desfondarse inicio impresión ofreció hugo gonzález verse paso reservas demuestra nadó cálculo síntoma madurez competitivael español necesitaba acercarse europeo budapest subirse peldaño podio tokio centésimas semifinales contrario sucede aquatic center nadado rápido tardes mañanas finales sucedió ganador semifinal gonzález favoritos kolesnikov pasó series irá seguro rápidohugo gonzález hijo padre español madre brasileña salto río compitió joven semifinales prueba administrar participación espalda series estilos aspira claridad medalla tratarse prueba abierta marcha nadadores michael phelps ryan lochte dejado estilos abiertos alternativas vimos oro chase kalisz acompañó marca mediocre</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Deportes_60.txt</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -464,11 +474,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>martín puente vigo junio número gallego carlos alcaraz cerrarán cima ranking mundial martín alcanzó dobles tenis silla común compañero amigo charly crack compartimos momentos us open taquillas sonrisa hicimos amistad volvimos coincidir recepción majestad felipe vi confiesa as deportista paralímpico año tachado sueños listaroland garros grand slam puertas dani caverzaschi aperitivo atracón triunfos ganó dobles us open francés nicolas peifer septiembre masters argentino gustavo fernández noviembre número dobles nivel individual coloca séptimo reto año ayudado confiar creer duda temporada servirá empujón próxima explica tenista desempolvar recuerdos roland garros torneo conduciendo car sant cugat vallés quería estrenar carné lució coche competición salió pedir boca semana flipé niño parque atracciones lados crecermartín lidiar presión privilegio jugando gloria alcance manejar presión abstraerse necesaria explorar límites argumenta deportista salvar numerosos obstáculos niño quería jugar celta admira aspas síndrome proteus cambió planes enfermedad rara provoca crecimiento óseo anormal terminó amputación pie izquierdo años levantar sábana shock pasar quirófano añosfue hermano antón estudia universidad sacramento california beca tenis descubrió tenis silla flechazo enamorando íbamos jugar club hermano hermana hacía pie frontón problemas físicos aumento primeras silla impresión esperaba semejante armatoste llamé transatlántico ruedas tenis silla ayudó olvidar operaciones noches hospital casualidad convertido vida pensé vivir juego desaparece silla mágico deporte explica niño prodigio años empezó competir conquistó título nacional número ranking mundial júnior consiguió diploma juegos río años joven modalidad tokio parís retos asoman hablar pronostica estudiante administración dirección empresaslos juegos igualdad tenis inclusión torneos atp confirma martín costado semanas asimilar año mágico quiero llegar número individual victoria llegar razónmartín puente jugó partido exhibición chile rafa nadal alejandro tabilo gustavo fernández experiencia ¡día histórico personas estadio retransmitido directo televisión nacional chile tenista paralímpicos redes año terminado fecha marcada rojo campeonato españa sevilla preparar australia comenzar fuerza</t>
+          <t>decisión gobierno central incrementar salario mínimo interprofesional años forma escalonada euros mantener reuniones llegar acuerdos empresas sindicatos valora mercado laboral provincia castellón noticia positiva subrayan fuentes ccoo provincia recordando sindicato reivindica smi salario resto países europeos comparamos interesa gobierno turnoa cifra aproximada ccoo confirman trabajadores trabajadoras verán beneficiados repunte empleados cobran únicamente salario mínimo cifrado euros recuerdan ugtdesde ccoo ugt explican incremento transmitirá tranquilidad sectores hostelería turismo carecer convenio colectivo regule condiciones laborales nivel empresas documento desapareció octubre vigentes convenios empresa empresa fija condiciones denuncia sindicatos incluyen salarios bajos representan miseria apunta secretario ugt castellón francisco sacaciaademás sector sindicatos sitúan punto mira trabajadores ganan vida limpieza hogares cuidadores personas mayores discapacitados sectorestambién establecimientos comerciales subraya sacacia carecen convenio colectivo aplican casos smi vigente momentosacacia siguiendo línea ccoo apunta ugt valora positivamente incremento queda corto defendemos salario mínimo euros salario cifra reivindica secretario ugt sindicato meses puso marcha campaña ponte mil exigir salario mínimo digno cubra necesidades ciudadanía acorde crecimiento económico productividad percibiendocabe destacar ministerio seguridad social provincia castellón cifró noviembre afiliados seguridad social dato disponible presente ejercicio engloba personas afiliadas régimen autónomos trabajadores mar minería carbón referimos número afiliados régimen cifra sitúa personas cierre noviembre trabajadores cotizan firmado contrato personas forma ilegal práctica seguirá manteniendo casos seguirán cobrando lamenta secretario ugtletra pequeña leyasimismo pese sacacia subraya necesidad leer letra pequeña leyes smi incrementó llegar euros indicaba cobraban salario mínimo beneficiarían subida alertan ugt incidiendo subidas salarios deberían negociables alusión gobierno palabra pese mantener encuentros sindicatos confederación española organizaciones empresariales ceoe cepymepor ccoo apuntan salarios aportaciones seguridad social recaudación vía irpf consumo consecuente repercusión dinamización economía ingresos vía indirectapor asegurado incremento euros economía crecerá euros cifra euros</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Politica_26.txt</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -477,11 +492,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>año carlos alcaraz explotó us open partido nivel mundial ganó ronda sets stefanos tsitsipas número ranking años exhibición fuerza tenis regaló espectadores arthur ashe gesta vuelta orbe vi golpear pelota fuerte griego perdió murciano temporada miami barcelonaalcaraz acumuló hitos precocidad hueco élite confianza actuación cuarto major alcanzó cuartos retiró lesión perdía augeraliassime disparó rendimiento circuito semifinales viena triunfo cuartos top matteo berrettini parís bercy jannik sinner ganar nextgen atp finals milán deshizo sebastian korda partido título sueño número mundo trabajaré allá ganar torneo objetivo seguiré enfocado ganar nextgen finals significa motivación cara año viene seguir entrenándome tope mejorando próximas atp finals objetivo chulo difícil diría imposible lucharemos trabajaremos lograrlo imaginaba diez meses clasificadosu objetivo top acabó curso número disgusto supuso jugar finales copa davis españa contraer covid justo comienzo ranking inicio caer ronda open australia sets berrettini ganó atp río janeiro torneo obtenido victoria atp ganó albert ramos años brasil levantó trofeo carrera umag julio entró top preparado entrar nivel advirtió prodigio palmar décimo carrera copa maestrospor debutó armada davis victoria rumano copil eliminatoria clasificación disputó marbella despegue semifinalista indian wells nadal cuerdas campeón español miami impuso ruud rival título liderato mundial us open tropiezo prematuro montecarlo korda triunfó metió top barcelona carreño madrid ganó masters frente zverev derrotado alemán cuartos roland garrosmiro ranking asombroso entreno ganar plazas importante advirtió caer octavos wimbledon sinner superó umag carlitos venía perder hamburgo musseti premio número jugó montreal cincinnati resultados discretos auguraban excelente desempeño us open tsitsipas acumula victorias títulos número joven historia excelente</t>
+          <t>cuba anunció retirada doctores brasil acusar presidente electo país jair bolsonaro exigir condiciones inaceptables mantener prestación servicios médicos aporta importantes ingresos gobierno cubanoel ejecutivo presidido miguel díazcanel tomado decisión continuar participando programa médicos ministerio salud comunicado ampliamente divulgado entidades medios estatales habanaen marco programa iniciado años doctores cubanos prestan atención médica brasil comunidades desfavorecidas remotas favelas río janeiro sao paulo poblaciones indígenas amazonasel presidente díazcanel pronunció decisión oficial twitter dignidad profunda sensibilidad profesionalidad entrega altruismo colaboradores cubanos prestado valioso servicio pueblo brasilactitudes dimensión humana respetadas defendidas somoscuba mandatario islael gobierno cubano atribuyó decisión retirar médicos declaraciones amenazantes despectivas bolsonaro prometió revisar contrato bilateral endurecer condiciones permanencia especialistas brasil asuma enerosalario integralel presidente electo brasileño tendencia ultraderechista criticado modelo actual programa médicos defendido continuidad modificaciones especialistas cubanos reciban salario integralhoy bolsonaro replicó gobierno cubano tuit recordó exigencias condicionamos continuidad programa médicos aplicación test capacidad salario integral profesionales cubanos destinado dictadura libertad traer familias infelizmente cuba aceptóla exportación servicios médicos importante fuente divisas cuba formación universitaria completamente gratuita año miles estudiantes licencian carrera medicina ejercer paísa cambio gobierno cubano embolsa salario perciben doctores países extranjeros comisión caso destinados brasil estima brasil paga dólares quedan efe médico cubano ejerce especialidad brasilrepatriacionesla fuente reveló comenzado repatriaciones doctores cuba proceso continuará próximas semanaspara destacar irreversibilidad decisión ministerio salud cubano remarcó comunicado directora ops organización panamericana salud líderes políticos brasileños fundaron defendieron iniciativatambién esbozó argumento doctores despachados brasil mantenido puesto salario cuba dólares mes alto comparación profesiones estatales insuficiente frente necesidades diarias islaprograma socialla participación cubana médicos realiza ops años funcionamiento profesionales isleños tratado millones pacientes brasileñosse teme programa aseste duro golpe frágil economía cuba cuya fuente divisas exportación servicios profesionales médicos recauda millones dólares anuales promediolos resultados económicos actividad superan ampliamente industria turismo registró ingresos millones dólares datos disponiblesen septiembre destitución presidenta dilma rousseff surgieron dudas continuidad doctores cubanos programa social brasileño finalmente cuba confirmó mantendríaen discursos ganar elecciones brasil bolsonaro anunciado giro política exterior acercarse eeuu cortar lazos medida venezuela cuba países gobiernos socialistas</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Politica_49.txt</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -490,11 +510,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>debut convertido importante eliminatoria difícil pelear unidos arengaba anabel media capitana española nuria párrizas mundo abriera miércoles frente yulia putintseva triunfo kazajistán bretaña martes permitía errores cálculos sencillos optar semifinales valía victoria finales billie king jean cup dejan margen error granadina entendía perfección saltar pista emirates arena glasgow paula badosa elena rybakina casos salida tromba incontestables toparse muros ceder putintseva origen ruso integrantes combinado superaba bolas partido rybakina campeona año wimbledon ranking salvaba nuria paula perder set tiraban garra cerrar puntos españa redondeó noche dobles badosa bolsova paso semifinales buscarán jueves posición grupo persiguiendo victoria bretañabadosa jugado selección año convocada causó baja lesión ganas estrenarse repitió dobles pese programada presencia motiva dejar jugar badosa españa decía previa piel cambio chip dejar atrás temporada agrio privó disputar wta finals necesitaba set mostraba totalmente liberada minutos viaje esencia derecha poderosísima ganadores impecable saque puntos ganados aces genialidades passing maravilloso tercer juego manga absorbía esencia selección suyaes jugadora rybakina ganadora grand slam jugamos sets feliz punto país nerviosa partido nuria perdido energía quiero país gusta representar gente declaraba paula victoria sonrisa brillante parcial contener elena implacable saque máximos kmh centímetros recuperó encajar break tercer juego grito reconquistaba terreno perdido fruto indicaciones anabel daba tableta empezaba reencontrarse resto reveses cortados bolas bajas red confianza vivido semanas volvía oportuno rotura juego definitivo rojo sienta bienpaula superaba muro impasible párrizas imprevisible putintseva ranking jugadora desquicia recogepelotas pase bolas gesticula constantemente queja cosa totalmente agrado set tiraba raqueta suelo dejarla pisoteaba terminaba energía llevarse manga tercero desfavorable golpeaba fuerza muslos asegurarse tiebreak daba puñetazo suelo celebración somete presión genera clima tenso rivales caso párrizas público afición kazaja mayoritaria español gradas jordi llegado expresamente barcelona bandera ruidosacon particular empeño nuria llevó set pasó terminó tiebreak sirvió resumen partido exposición virtudes defectos ambas jugadoras párrizas académica peligrosa podía entrar pista normalmente revés buscar derechas paralelas cogía renta importante putintseva anárquica sobrevivía dejadas bolas altas cara cruz tren inferior permite cubrir agilidad ángulos agarraba resistencia nuria agresiva ganadores conjunto superior saque puntos ganados resto mental importante martillo pilón iba recordando anabel zona selección</t>
+          <t>viernes firma iniciativa salud libre mercurio marco convenio minamata pide eliminación definitiva termómetros tensiómetros contengan mercurio pondrá producción importanción exportación instrumentos médicos incluyan elemento químico productos contienen pilas interruptores firma convención minamata conseguiremos proteger mundo devastadoras consecuencias mercurio salud afirma directora margaret chan elementos químicos preocupación salud pública dispersa permanece organismos años causando graves enfermedades discapacidad intelectual población expuesta continúa causar daño cerebral especialmente jóvenes desórdenes sistema nervioso inmunitario reproductor daños renales digestivoshace años expertos advertían anunciaban incremento emisiones metal negociaciones principios año países llegaron vinculante reducción emisiones finalmente suscribe viernespara conseguirlo convenio establece plan acción países firmantes eliminen formas perjudiciales mercurio reduzcan emisiones metal procedentes industria promuevan alternativas mercurio asequibles seguras protejan niños mujeres edad fértil mercurio plantea amenaza especial desarrollo niño útero exposición elemento químico tomen medidas mejorar salud bienestar trabajadores contacto mercurioaunque convención minamata permite sigan utilizando aparatos médicos medición mercurio circunstancias especiales organización mundial salud oms coalición internacional salud daño insisten dadas tremendas consecuencias exposición mercurio salud debería mantenerse fecha límitela oms trabajará gobiernos garantizar cumplan obligaciones virtud convenio especialmente áreas salud señala doctora maría neira directora oms salud pública ambiente requiere eliminación termómetros tensiómetros mercurio oms asociados sector salud comprometen eliminar mercurio antisépticos tópicos cosméticos aclarar piel quieren desarrollar medidas eliminar mercurio empastes productos dentales fomentar intercambio información investigación salud pública</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Salud_20.txt</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -503,11 +528,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>inicio declive serena williams existido tanta unanimidad hora señalar jugadora principal favorita campeona roland garros vitola iga swiatek pronúnciese sbiontec temporada torneo sábado confirmó pronósticos incontestable triunfo minutos coco gauff polaca reeditó título conquistado ocasión barrió estadounidense sofia kenin años doble campeona torneo nueve jugadoras logrado open grand slams racha victorias consecutivas periplo triunfal perdido sets instala nómina leyendas alcanzado registros parecidos superiores invencibilidad navratilova graf court evert venus williams mencionada serenaswiatek perdona ganar juego pierde vuelve pista sed venganza engulle rivales gauff finalista joven major sharapova wimbledon clijsters roland garros perdido manga campeonato vio admiradora nadal ganado torneos curso pasaba americana reprimir lágrimas podido tenistas siquiera inquietar número mundo afianza ventaja líder ranking saca puntos estonia kontaveitt paula badosa quinta jugadora años vencer parís cabeza serieespero llorar arrancó entrega trofeos merecemos equipo años esperaba ganar duro presión necesario llegar justo acordarse ucrania seguid fuertes guerra continúa recibir atronadora ovacióncon mínimo despiste quiebre inicio set swiatek saldría victoriosa celebró grada equipo familia futbolista bayer suena barça robert lewandowski porcentaje triunfos roland garros tercero historia gauff disputaba grand slam queda consuelo disputará dobles compatriota jessica pegula espero juguemos finales ganarte sonriendo llorar lamentaba podido competir agradecía apoyo público deportetras celebración triunfo iga swiatek philippe chatrier acogió dobles masculino impusieron marcelo arévalo salvador neerlandés jeanjulien rojer croata ivan dodig estadounidense austin krajicek arévalo rojer supieron sufrir set salvaron puntos partido triunfo pareja entra libros historia dobles puesto neerlandés rojer convierte ganador grand slam edad años nueve meses superando meses mike bryanrojer convertía jugador edad disputar grand slam dobles suma victoria torneo ganó wimbledon us open impuso feliciano marc lópez ambas rumano horia tecau pareja compañero marcelo arévalo grand slam palmarés fecha salvador sumaba títulos torneos año rojer única historia ganando roland garros jugador centroamérica gana grand slam</t>
+          <t>debut convertido importante eliminatoria difícil pelear unidos arengaba anabel media capitana española nuria párrizas mundo abriera miércoles frente yulia putintseva triunfo kazajistán bretaña martes permitía errores cálculos sencillos optar semifinales valía victoria finales billie king jean cup dejan margen error granadina entendía perfección saltar pista emirates arena glasgow paula badosa elena rybakina casos salida tromba incontestables toparse muros ceder putintseva origen ruso integrantes combinado superaba bolas partido rybakina campeona año wimbledon ranking salvaba nuria paula perder set tiraban garra cerrar puntos españa redondeó noche dobles badosa bolsova paso semifinales buscarán jueves posición grupo persiguiendo victoria bretañabadosa jugado selección año convocada causó baja lesión ganas estrenarse repitió dobles pese programada presencia motiva dejar jugar badosa españa decía previa piel cambio chip dejar atrás temporada agrio privó disputar wta finals necesitaba set mostraba totalmente liberada minutos viaje esencia derecha poderosísima ganadores impecable saque puntos ganados aces genialidades passing maravilloso tercer juego manga absorbía esencia selección suyaes jugadora rybakina ganadora grand slam jugamos sets feliz punto país nerviosa partido nuria perdido energía quiero país gusta representar gente declaraba paula victoria sonrisa brillante parcial contener elena implacable saque máximos kmh centímetros recuperó encajar break tercer juego grito reconquistaba terreno perdido fruto indicaciones anabel daba tableta empezaba reencontrarse resto reveses cortados bolas bajas red confianza vivido semanas volvía oportuno rotura juego definitivo rojo sienta bienpaula superaba muro impasible párrizas imprevisible putintseva ranking jugadora desquicia recogepelotas pase bolas gesticula constantemente queja cosa totalmente agrado set tiraba raqueta suelo dejarla pisoteaba terminaba energía llevarse manga tercero desfavorable golpeaba fuerza muslos asegurarse tiebreak daba puñetazo suelo celebración somete presión genera clima tenso rivales caso párrizas público afición kazaja mayoritaria español gradas jordi llegado expresamente barcelona bandera ruidosacon particular empeño nuria llevó set pasó terminó tiebreak sirvió resumen partido exposición virtudes defectos ambas jugadoras párrizas académica peligrosa podía entrar pista normalmente revés buscar derechas paralelas cogía renta importante putintseva anárquica sobrevivía dejadas bolas altas cara cruz tren inferior permite cubrir agilidad ángulos agarraba resistencia nuria agresiva ganadores conjunto superior saque puntos ganados resto mental importante martillo pilón iba recordando anabel zona selección</t>
         </is>
       </c>
       <c r="C6" t="n">
         <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Deportes_16.txt</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -516,11 +546,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>belleza ojo espectador millones ojos coches fórmula contemplan drástico adición cabina protección presenta red bull aeroscreen opiniones míalos coches fórmula cabina abierta argumentar mediados años mercedes demostró tipo monza tendencia tiempos cambian requisitos descartar movimiento modelo coche reconocer movimiento conocemos enorme movimiento duda ofenderá sensibilidades seguro gente molestará comparación encantarán minoría probablemente jurará verá carrera salva vida vale pena quiero estrellas fórmula vivos problema protecciones propuestas coches quedar debemos capaces cascos pilotos claridad esconderlos escudo jenson button pasó historia diciendo prefiere aspecto coche cubierta presentada red bull – fundamentando opinión carreras lanchas solía disfrutar niño rodeado niño ciencia ficción películas xwing fighter luke skywalker muestran máquinas equipadas cabina dosel dirijo mirada red bull daniel ricciardo pista sochi mañana viernes observarlo miré punta nariz divertida pegajosa sección abruptamente angular similar forma alain prost llegar sección plana encontrarme cabina escudo antidisturbios lewis hamilton montado superioren paso flujo aspecto uniforme lotus cabina envolvente fachada – veo superficies constreñidas norma regulaciones modernas fórmula creado frontal coche diseñada personas piense millones dólares gastan año traducen coches abultados pregunta acerca culpar aerodinámica resultado formas cambio producir vuelta hora reglas cambien exigir aspecto atractivo sección frontal coches motogp debería prohibir alerones pensamiento niño molestaba coches producción línea salían forma caja aburridos lejanos gloriosos coches conceptos salones automóvil ¿por podían diseño frescoeso parecido conceptos visto red bull ferrari mclaren acerca visión futuro construye supercoche feo ¿por debemos aceptar cosa fórmula especialmente oportunidad reglas recuerdo conversación peter stevens diseñador icónico mclaren acerca narices actuales fórmula calificarlas abominaciones visuales entraron funcionamiento sugirió aerodinámica olvidado enseñado arte vea oportunidad presentar diseño atrozestoy ciento ¿quién</t>
+          <t>conseller sanidad salud pública miguel mínguez asegurado martes hospital castellón colapso denunciaron lunes representantes trabajadores concentraron señal protesta centro sanitario referencia provinciatampoco comunidad valenciana reúnan circunstancias convocatoria huelga sanidad comunidad madridesta postura titular sanidad valenciano comparecencia sede consell castellón presentar presupuesto histórico departamentola visita mínguez producido justo trabajadores sanitarios sindicatos puesto grito cielo consideran discriminación reparto plazas hospital resto centros sanitarios valencianos departamentos salud quejas ve argumentadas consellerla conselleria disciminación recursos humanos infraerstructuras proporcionales responsable sanidad destaca esfuerzo efectuado personal plazas mayo provincia castellón mínguez puntualiza plazas médicos hospital adjudicaron médicosconcentraciones huelgapreguntado quejas sindicatos colapso mínguez alega instalen equipos dotarán personal deja puerta abierta hablar equipos directivos yen exista disminución personal solucionará diálogo gerencias coordinadores departamentos actualizar necesidades infraestruturas recursos humanos dichoel malestar profesionales abre posibilidad convoque huelga mínguez contempla comunidad valenciana actual reúne circunstancias comunidades exista convocatoria huelganosotros cerradas urgencias extrahospitalarias madrid comunidad valenciana único ampliar plazas abrir puestos atención continuada rebajar ratios atención primaria sip facultativo enfermería pediatríatenemos mejores ratios españarespecto inversión sanitaria castellón cuentas consell conseller destacó provincia castellón contará millones euros destinados mejora infraestructuras sanitariasparalelamente comparecencia realizada centro castellón trabajadores urgencias hospital concentraban puertas servicio denunciar precaridad falta personal atender pacientes sanitarios mostraban cartel reclamaron ¡urgencias dignas espera media sitúa ó</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Politica_19.txt</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -529,11 +564,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>open australia dejado sonrisas lágrimas ranking circuito wta tenistas sonríen australiana ashleigh barty checa barbora krejcikova polaca iga swiatek estadounidense danielle collins barty logra ampliar liderato krejcikova swiatek collins suben posiciones establecerse topsin jugadoras pesado open australia provocado sufran caída considerable ranking wta semana jugadoras simona halep petra kvitova habituales top años semana figuran puestos clasificación cabe destacar caída bianca andreescu campeona us open semana aparece puesto especialmente llamativas graves caídas clasificación campeonas open australia japonesa naomi osaka campeona estadounidense sofia kenin campeona osaka desploma clasificación defender puntos campeona semana pierde posiciones figurar puesto puntos impactante caída ranking sofia kenin verse sorprendida ronda madison keys cae puestos semana aparece puesto puntostambién cae clasificación checa karolina muchova compitió open australia alcanzar semifinales año provocado semana pierda puestos baje puesto ranking situación similar estadounidense jennifer brady finalista open australia podido participar lesión razón brady perdido posiciones clasificación salido top quedarse puntoslas hermanas williams topla ausencia serena williams open australia serias consecuencias tenista estadounidense ranking semana serena williams aparece puesto clasificación puntos abajo aparece hermana venus semana figura puesto caer posiciones jugar partido oficial torneo chicago mes agosto</t>
+          <t>autoridad europea seguridad alimentaria aesa alertado papel térmico utilizado recibos compra supermercados alimentos fuente exposición bisfenol bpa consumidoreslos expertos agencia llevado cabo estudio cuyos resultados provisionales concluyen dieta constituye grupos población fuente exposición sustanciaademás revela contacto pensaba lactantes niños adultos estima exposición media vía alimentaria llega dosis diaria tolerable fijada aesalos científicos concluido asimismo niños años expuestos bisfenol dieta consumo alimentos relación peso corporal superior edadesel informe revisión riesgo exposición bisfenol agencia llevado cabo ocasión analizan fuentes alimenticias tipo papel térmico aireel papel térmico utiliza resguardos bancarios representa fuente contacto importante bisfenol alimentación pudiendo suponer exposición grupos población señala comunicado agenciano obstante aesa matiza falta datos particular absorción sustancia piel hábitos manejo resguardos compra ofrecer estimación precisa exposición víael estudio forma proceso fases pretende analizar riesgo global ligado sustancia etapa posterior autoridad alimentaria organizará consulta pública evaluar riesgos potenciales salud humanael bisfenol sustancia química presente plástico policarbonato fabrican botellas resinas recubrir interior latas comida bebidadistintos estudios científicos concluyen niveles bajos concentración bpa asociado diabetes obesidad infertilidad cáncer mama próstata problemas cardiovasculares alteraciones desarrollo neurológico cerebral trastornos comportamiento</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Salud_33.txt</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -542,11 +582,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>acaban vacaciones madrid regresa entrenamientos descanso disfrutado jugadores convocados selecciones ancelotti seguirá grupo cuadro sesión carletto conformar once jueves citados nueve jugadores lunin lucas vázquez nacho vallejo mendy odriozola kroos ceballos mariano incorporarán benzema alabael delantero abandonar concentración francia noviembre aquejado desgarro muscular muslo izquierdo karim trabajando valdebebas disfruta isla reunión extra permiso único pisado ciudad deportiva blanca vallejo acudido ejercitarse sesiones castilla alaba amistosos andorra italia jugó selecciónlos mundialistas irán reincorporándose medida vayan eliminadas selecciones diez descanso volver alcancen semifinales jugar tercer cuarto puesto volver víspera partido espera madrid selección cae fase grupos croacia modric bélgica courtois hazard uruguay valverde corren peligro internacionales volverán torno eliminados octavos caigan cuartos equipo retomará liga viernes campo valladolid siguientes compromisos ligueros visitantes villarreal enero athletic enero medias intercalarán copa supercopa comenzará madrid dieciseisavos copa rey domicilio blancos exentos primeras eliminatorias participación supercopa verán caras enero supervivientes inferior categoría rival conocerá diciembrea enero ancelotti buscarán título temporada camino sextete supercopa españa obstáculo reválida título valencia medirá semifinales riad capital saudí alberga torneo madrid alcanza disputará título eneroel calendario guarda incógnitas copa supercopa principio agenda aparece partido bernabéu enero real sociedad calendario aguarda incógnitas copa supercopa torneo ko brinda par oportunidades volver bernabéu previsto octavos cuartos madrid queda emparejado equipo bola blancos sale coliseo blanco reabrir enero</t>
+          <t>argentina pendiente fallo juicio presunta corrupción política poderosa argentina cristina fernández kirchner sentencia conocerá martes diciembre filtración prensa mensajes jueces políticos opositores empresarios medios elevado tensión previa chat publicado domingo medios locales participantes debaten difundir versión falsa contrarrestar denuncia dádivas vinculada viaje pagado realizaron patagonia octubre presidente argentino alberto fernández anunciado cadena nacional solicitará justicia investiguen penalmente hechos relacionados viaje financiación consejo magistratura abra sumario jueces implicadosel kirchnerismo exhibe conversación supuestamente obtenida hackers radiografía precisa podredumbre lawfare judicatura fines políticos palabras ministro justicia martín soria macrismo cambio montaje objetivo salvar kirchner esperan martes sentencia negativa llamada causa vialidadlos mensajes involucran juez julián ercolini cargo instrucción investigación cristina kirchner colegas pablo yadarola carlos mahiques pablo cayssials fiscal ciudad aires juan bautista mahiques ministro seguridad ciudad aires marcelo dalessandro directivos grupo clarín chats publicados diario argentino portal web cohete luna hackeo línea teléfono celular implicados origen ilegal fuente impide puedan usados prueba justicialos participantes chat telegram muestran preocupados publicación diario página viaje pagado realizaron octubre avión privado bariloche alojarse par noches estancia multimillonario inglés joe lewis lago escondido lewis cercano expresidente mauricio macri estancia vieja conocida argentinos decisión empresario bloquear turistas ingresos lago intercambio involucrados analizan responder periodistas llaman confirmar viaje debaten distintas estrategias pasar viaje escapada conjunta pagaron bolsillopodríamos averiguar tema facturita comprobante pago lago escondido escucha mensaje voz juan bautista mahiques fiscal ciudad aires cayssals propone pagar avión quedaron casa amigo ercolini pregunta fácil facture lago escondido noches media pensión carajo inventar insiste ercolini mensajes filtrados coincide necesidad mantener llave fotos sacaron travesíalos participantes burlan critican periodistas contactan alardean responderles llamar directivos medios frenar difusión noticia principal blanco críticas policía seguridad aeroportuaria psa consideran origen filtración planilla viaje avión octubre tocará ministro nación disolver psa escribe dalessandro cargo cartera seguridad ciudad airesdesmentida clarínsegún medios publicaron noticia viaje financiado directivos grupo clarín versión conglomerado medios niega fuentes grupo clarín advierten contenidos chat totalmente truchos falsos adulterados procedencia ilegalel escándalo derivó doble denuncia consejo magistratura presunto desempeño funciones jueces fiscales presuntamente involucrados justicia bariloche supuesta violación deberes funcionario público admisión dádivas tráfico influenciasla filtración vuelto dividir argentina previas conozca sentencia juicio kirchner vicepresidenta acusada delitos asociación ilícita defraudación adjudicación centenar obras públicas provincia patagónica santa cruz mandatos presidenta kirchneristas sostienen mensajes evidencian connivencia judicial oposición vicepresidenta antikirchneristas operación espionaje ilegal orquestrada brazada ahogado sentenciala polémica creció llegar alto casa rosada alberto fernández convocó cadena nacional queda expuesta enorme contundencia corporaciones operan funcionarios jueces fiscales procurando favores casos buscan ventajas indebidas simplemente propician persecución enfrentan fernández pidió justicia investiguelos legisladores coalición gobernante frente pedido comunicado conjunto desempeño funciones comisión delitos graves escandalosas inconductas éticas confesas exigimos inmediata regularización institucional consejo magistratura paralizado accionar inocente corte suprema justicia renuncia funcionarios públicos involucrados seria profunda investigación señalan texto legisladores afirman público conocimiento magistrados fiscales manejan margen ley verlo escucharlo voz excede imaginadodesde alianza opositora juntos cambio provienen políticos involucrados voces media salido defender ministro seguridad porteño primeras presidenta propuesta republicana pro patricia bullrich filtración forma intentos desesperados kirchnerismo eludir justiciala hipótesis bullrich coincide dalessandro acusado redes kirchnerismo financiar impuestos operación tragicómica inteligencia salvar jefa kirchner equipo dalessandro contactado diario respondió consultasla filtración empeora imagen judicial argentina relación política juez federal prefiere mantener nombre reserva opinó sucedido gravísimo vergüenza impunidad manejan verduguean periodistas quedar jueces presidente cámara federal casación penal alejandro slokar máxima autoridad judicial corte suprema judicial vive crisis radical pidió tomar medidassuscríbase newsletter país américa reciba claves informativas actualidad región</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Politica_57.txt</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -555,11 +600,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>gol benfica minuto israel jornada fase grupos provocado psg encuadrado bayern octavos champions league parisinos enfrentaron barcelona real madrid cocos máxima competición continental eliminatoria durísima galtier sufrido consecuencias deberes instancia copa europael psg únicamente conseguido pasar enfrentamientos directos enfrentado clubes champions league eliminó chelsea justo año debacle gol demba ba stanford bridge pasó barcelona octavos venció bayern cuartos año resto chelsea barcelona city barcelona real madrid manchester united bayern city semifinal real madrid incapaz pasar tipo escenarios suelen favorecer ahoraun psgbayern remonta indudablemente champions inédita pandemia equipos enfrentaron lisboa única capitalinos historia coman canterano psg gol bayern sexta orejona tuchel miel labios jarro agua fría equipo actual khelaïfi liderara revolución mercado agosto precisamente abril psg bayern volvían enfrentarse eliminatoria apasionante lewandowski lesionado polaco fichado barça bayern sucumbió partido ida allianz arena exhibición neymar mbappé psg impuso partido trepidante puso tierra encuentro parque príncipesen parís neymar probablemente mejores partidos carrera psg consiguió marcar perdió bayern choupomoting jugador coman conjunto parisino autor insuficiente pochettino pasaron semifinales inferiores inspirado manchester city camerunés estrellas bayern nageslmann mostrándose intratable europa comienzo regular bundesliga domina antojocomo homogéneo psg domina ligue gas objetivo prioritario champions parisinos debacle absoluta edición champions cambiado empezando banquillo galtier sustituyó pochettino técnico francés avalado lille niza conseguido recuperar nivel messi neymar alternar distintos sistemas psg capaz jugar centrales defensas acumular jugadores imbatido temporada febrero buscará eliminar favoritos champions league fichado jugadores messi ramos donnarumma achraf salto cualitativo importante plantilla despachos luis campos conocido lille mónaco elegido asentar estabilidad parís portugués amigo mbappé fichó mercado soler fabián ruiz ekitike renato sanches vitinha jugadores línea refuerzan colectivo equipola ida disputará parque príncipes vuelta múnich escenario especialmente psg trae recuerdos cosechado champions falta llegarán neymar mbappé messi eliminatoria favoritos llevarse mundial eliminación prematura provocar bajón rendimiento aspecto psicológico meses doble enfrentamiento definitiva cruce apto cardiacos</t>
+          <t>acaban vacaciones madrid regresa entrenamientos descanso disfrutado jugadores convocados selecciones ancelotti seguirá grupo cuadro sesión carletto conformar once jueves citados nueve jugadores lunin lucas vázquez nacho vallejo mendy odriozola kroos ceballos mariano incorporarán benzema alabael delantero abandonar concentración francia noviembre aquejado desgarro muscular muslo izquierdo karim trabajando valdebebas disfruta isla reunión extra permiso único pisado ciudad deportiva blanca vallejo acudido ejercitarse sesiones castilla alaba amistosos andorra italia jugó selecciónlos mundialistas irán reincorporándose medida vayan eliminadas selecciones diez descanso volver alcancen semifinales jugar tercer cuarto puesto volver víspera partido espera madrid selección cae fase grupos croacia modric bélgica courtois hazard uruguay valverde corren peligro internacionales volverán torno eliminados octavos caigan cuartos equipo retomará liga viernes campo valladolid siguientes compromisos ligueros visitantes villarreal enero athletic enero medias intercalarán copa supercopa comenzará madrid dieciseisavos copa rey domicilio blancos exentos primeras eliminatorias participación supercopa verán caras enero supervivientes inferior categoría rival conocerá diciembrea enero ancelotti buscarán título temporada camino sextete supercopa españa obstáculo reválida título valencia medirá semifinales riad capital saudí alberga torneo madrid alcanza disputará título eneroel calendario guarda incógnitas copa supercopa principio agenda aparece partido bernabéu enero real sociedad calendario aguarda incógnitas copa supercopa torneo ko brinda par oportunidades volver bernabéu previsto octavos cuartos madrid queda emparejado equipo bola blancos sale coliseo blanco reabrir enero</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Deportes_22.txt</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -568,11 +618,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>salma paralluelo vivió montaña rusa emociones domingo civitas metropolitano aragonesa joyas cantera española fichó verano barcelona definitivamente pasión atletismo difícil decisión apostar deporte dando alegrías campeona mundo sub profesional años andadura azulgrana empezó altibajoslas lesiones impedido continuidad octubre levante debutar azulgrana noviembre marcó gol jugadora barcelona levante planas progresión importante llegando titular frente conjunto catalán alavés ganado confianza ausencia jugadoras importantes mariona hansen protagonismo domingo giráldez puso titular salió onces oficiales raro pasaba salieron calentar doce jugadoras crnogorcevic partía once salma retiró barcelona anunció aragonesa crnogorcevic saliese inicio hacía indicar salma lesionadola joven extremo salió banquillo lágrimas contener rabia emoción titular duelo altos vuelos estadio civitas metropolitano asisat oshoala intentaba consolar joven futbolista relato efecto minuto salma saltó campo descartando lesión minutos césped cuarto encuentro minutos recogió rechace lola gallardo penalti lanzó mariona quinto particular celebración podía oshoala minutos salma actuó posición nueve abrazo agradecimiento palabras banquillo aragonesa podía contener lágrimasha problema logístico entrar detalle cambio hora jonatan giráldez rueda prensa posterior ausencia salma once anunciar titular desveló razones jugado abierta banda derecha normalmente diestras juegan ana crnogorcevic caro hansen juegue pierna cambiada delantera cualidades izquierda talento descomunal puliendo salma vivió montaña rusa acabó victoria doblete demostración talento atesora</t>
+          <t>gol benfica minuto israel jornada fase grupos provocado psg encuadrado bayern octavos champions league parisinos enfrentaron barcelona real madrid cocos máxima competición continental eliminatoria durísima galtier sufrido consecuencias deberes instancia copa europael psg únicamente conseguido pasar enfrentamientos directos enfrentado clubes champions league eliminó chelsea justo año debacle gol demba ba stanford bridge pasó barcelona octavos venció bayern cuartos año resto chelsea barcelona city barcelona real madrid manchester united bayern city semifinal real madrid incapaz pasar tipo escenarios suelen favorecer ahoraun psgbayern remonta indudablemente champions inédita pandemia equipos enfrentaron lisboa única capitalinos historia coman canterano psg gol bayern sexta orejona tuchel miel labios jarro agua fría equipo actual khelaïfi liderara revolución mercado agosto precisamente abril psg bayern volvían enfrentarse eliminatoria apasionante lewandowski lesionado polaco fichado barça bayern sucumbió partido ida allianz arena exhibición neymar mbappé psg impuso partido trepidante puso tierra encuentro parque príncipesen parís neymar probablemente mejores partidos carrera psg consiguió marcar perdió bayern choupomoting jugador coman conjunto parisino autor insuficiente pochettino pasaron semifinales inferiores inspirado manchester city camerunés estrellas bayern nageslmann mostrándose intratable europa comienzo regular bundesliga domina antojocomo homogéneo psg domina ligue gas objetivo prioritario champions parisinos debacle absoluta edición champions cambiado empezando banquillo galtier sustituyó pochettino técnico francés avalado lille niza conseguido recuperar nivel messi neymar alternar distintos sistemas psg capaz jugar centrales defensas acumular jugadores imbatido temporada febrero buscará eliminar favoritos champions league fichado jugadores messi ramos donnarumma achraf salto cualitativo importante plantilla despachos luis campos conocido lille mónaco elegido asentar estabilidad parís portugués amigo mbappé fichó mercado soler fabián ruiz ekitike renato sanches vitinha jugadores línea refuerzan colectivo equipola ida disputará parque príncipes vuelta múnich escenario especialmente psg trae recuerdos cosechado champions falta llegarán neymar mbappé messi eliminatoria favoritos llevarse mundial eliminación prematura provocar bajón rendimiento aspecto psicológico meses doble enfrentamiento definitiva cruce apto cardiacos</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>0</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Deportes_24.txt</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -581,11 +636,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>barcelona nivel azulgrana volvieron demostrar europa candidatas lograr pleno títulos quieren puerta grande pleno victorias cuentan partidos temporada triunfos bayern demostración importantes bajas alexia mariona hansen equipo planeta pasaron bayern aguantó mitad acercamiento sucumbió geyse abrió marcador empezar golazos aitana pina fiesta camp nou espectadores batiendo récord fase gruposel barcelona salió azulgrana querían volver salir camp nou heroínas entrada coliseo azulgrana empezar aitana geyse ocasiones serios avisos bayern queria veía superado azulgrana cómodas crnogorcevic entrando derecha pina juntándose centro aitana dirigiendo orquesta geyse llegando bayern espacios hacía daño bühl remate lateral red ocasiones contadas notaba bávaras dinamita stanway evitar disparo activa aitana lados barcelona dominaba bayern esperaba ocasión canterana ocasión clarísima alto sendas llegadas área barcelona iba aprentando bayern intentando balón tramo aparecer grohs evitando gol olímpico mapi paradón aitana goles sensación barcelona merecía descansoen jugada rolfö internó izquierda cambió banda crnogorcevic asistió primeras geyse puso muralla alemana caía barcelona sabía straus dejar espacios barcelona cómodo quería media hora rolfö volvió internarse izquierda pase atrás metió aitana fondo red remate primeras premio merecido canterana motor equipo bayern intentaba asomar barcelona permitía guinda ′ pina sacó chistera golazo tiro área mandó escuadra camp nou fiesta giráldez empezó mover banquillo salma debutó champions bruna disfrutó camp nou barcelona quiso sangre tiro aitana oshoala gozó ocasiones nigeriana falta puntería bayern tiró toalla quería gol honra barcelona vuelve ganar camp nou muestra poderío fiesta azulgrana año pleno</t>
+          <t>fiscal superior galicia carlos varela reclamó martes elaboración plan gestión riesgos corrupción infracción conexas organismos entidades administraciones públicas gestionen dinero valores patrimonio público puedan adoptar medidas preventivas posibles riesgos corrupciónse evitar ocurran casos sobornos cohechos desfalcos públicos tráfico influencias varela comparecencia comisión administración públicas parlamento gallego insistió plan prevenir prácticas funcionarios públicos identificaría posibles responsables neutralizarpara propuso creación entidad funciones específicas prevención control problema prácticas relacionadas corrupción galicia consello prevención corrupción cpc funcionaría entidad administrativa independiente entidad fiscalizadora externa representa consello contasse perfilar eventual respuesta problema permitiendo creación grupo respectivos resultados apuntar caminos lógica preventiva permitan reducción número oportunidades práctica delitos insistiótodos grupos parlamentarios mostraron iniciativa consideraron apropiada actual situación política financiera numerosos casos corrupción administraciones públicas gallegas casos sonados operación campeón operación orquesta operación arena carioca otrasevitar reprochescarlos varela insistió combate criminalidad grave prácticas relacionadas corrupción centrar medios recursos sistema justicia penal evitar reproche digan rápidos juzgar condenar ladrón baratijas estafador esquina lentos juzgar defraudadores erario público violadores inocencia país generalmente respaldados profesionales especializados aliviar durar procesos paraíso prescripción indicóasí precisó corrupción extiende administración economía pasando ámbitos vida social espacio libre corrupción reclamó evitar prácticas administraciones púbicas deberían marcha planes prevención riegos corrupción frente soborno abuso información privilegiada tráfico influenciasla fiscalía superior galicia recalcó gestión riesgo corrupción protección salvaguarda intereses colectivos plan aplicaría actividad administración pública correspondiente integrantes órganos personal dirigente evitando desperdiciar recursos disponibledesde propuesta ocurrencia personal apuntar basa proceso metodológico análisis ámbito internacional forma grupo acción financiero internacional –gafi encarga analizar personas político ventajas terceros apuntó reino unido puso marcha prevention act evitar riesgos corrupción administraciones públicas portugal órgano consejo cuentaspor desarrollo plan encargar determinados funcionarios órganos semejantes implicaría coste adicional presupuestosun paso significativola paso significativo deberíamos dispuestos darlo evitar desviaciones distintas administraciones nacionalista tereixa paztambién socialista beatriz sestayo felicitó fiscal propuesta acogemos suma satisfacción proactivos medida erradicar prácticas corrupción apuntó reclamó medidas higiene democráticas actual coyuntura políticoeconómicapor popular paula prado mostrarse favorable medida criticó propuesta fiscal apareciera memoria fiscalía caso apuntó corrupción extendiendo ayuntamientos pequeños apostó erradicación leyes legislaciones actualizar queden libro concreten sentencias sanciones ejemplarizantes añadiólos grupos destacaron datos presentados memoria fiscalía nacionalistas incidieron documento demuestra tramas incendiarias socialistas agradecieron compromiso varela menores pidieron lucha delitos patrimoniales centre iglesias populares incidieron aumento delitos patrimonio asuntos violencia géneroprocesos tramitadosla fiscalía tramitó procedimientos penales año número delitos asociados volumen acusaciones aumentando ranking delitos seguridad colectiva situaron peldaño siguen delitos lesiones finalmente delitos patrimoniales justicia menores galicia tramitaron llevados juicio casos varela puntualizó delitos corregir dándole prioridad acciones pedagógicas inclusivassobre área personas discapacidad ministerio fiscal presentó año demandas incapacidad ambiente furtivismo tramitaron diligencias investigación penal furtivismo constituye actividad ilegal tolerada socialmente apuntó varelaen mediación familiar estadísticas reflejan tendencia alcista semestre derivados mediación asuntos semestre continuar ritmo crecimiento año terminar asuntos derivadospatrimonio culturalvarela robo códice calixtino puso mesa necesidad proteger patrimonio cultural galicia religioso enmarcó nacimiento proyecto iglesia seguracultura protegida evitar precisamente expoliación tipo bienes iniciativa participa xunta iglesia fiscalíafinalmente casos violencia género varela año registraron procedimientos sistema penal sustanciaron trámite juicios rápidos delito frecuente resultó delito maltrato familiar ocasional peso seguido maltrato familiar porcentaje</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Politica_29.txt</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -594,11 +654,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>real sociedad cita historia natalia arroyo viajado múnich difícil misión remontar partido ida conjunto donostiarra compitió gol lea schüller descanso suficiente bávaras llevaran pequeña ventaja reale arena derrota competitividad demostrada conjunto txuriurdin clave duelo siga abierto encuentro vuelta contagiar ilusión afición donostiarrauna pequeña ventaja contará conjunto natalia arroyo descanso bayern jugó domingo donostiarras sábado frente betis pudieron repetir triunfo jornada villarreal centrocampista portuguesa andreia jacinto autora empate amaiur sarriegi marcado temporada delantera suplente partido ida apunta titular liderará ataque fiel escudera nerea eizagirre empezado temporada nivelelene lete iris arnaiz reciente campeona mundo sub ana tejada completan equipo fuerte grupo precisamente central cree remontada muchísimas ganas ilusión afrontar partido múnich creemos posibilidades declaró entrevista as faltó encuentro ida gol faltó poquito acierto sacado conclusión marcarlas efectivas contundentes gracias seguramente podamos llevarnos eliminatoria ganas remontadaaunque conseguirlo deberán superar bayern schüller bühl principales bazas ofensivas anotar encuentro liga werder bremen conjunto bávaro marcha bundesliga puntos real sociedad partidos empate jornada frente eintracht frankfurt parten favoritas noruego alexander straus banquillo buscarán seguir sumando experiencia máxima competición europea temporada cayeron cuartos psg global factor sorpresa ilusión ganas dejar huella europa clasificándose fase grupos principales armas real sociedad seguir historia</t>
+          <t>agosto juegos río obtenía michael phelps relevos libre decimonovena medalla oro número metales periplo triunfal comenzado atenas transcurrido pekín londres sydney años tierna bisoñez acabó quinto mariposaen brasil nadador visto planeta volvía asombrar admirar regresando infierno personal lucha permanente oculta depresión debilidad inconfesable mundo máximamente competitivo llevado par detenciones conducir efectos alcohol foto pipa agua utilizadas fumar marihuana granjeó generalizado descrédito acreedor sanciones federativas cancelación contratos publicitarios acarició tentaciones suicidassu relación sentimental iniciada nicole johnson modelo miss california naufragaba reflotaba volvía naufragar desequilibrando causa efecto mundo michael víctimas éxito daña fracaso sentía marioneta dorada marioneta personaje creado bienintencionados empujaban buscar difícil decidió quería tales extremos londres decidió parar insoportable peso oro weight of gold título documental retirado abría íntimamente canalpero piscina cuyas brillantes aguas podían volverse oscuras rescatarlo catártico dramático taumatúrgico traumático vida tomaba influencia agua voluntario redentor vía reencuentro reconciliación resurrección michael sometió tratamiento antidepresivo resolvió problemas nicole contrajo matrimonio convirtió padre paces vida estabilizaba listo río años ¡hurraen principio previsto interviniese destinaba existían hombres estrictamente rápidos expedición estadounidense michael nadado trials mundo puso rendirle homenaje batalla elección compasiva michael nadó posta ganó medallas oro mariposa estilos libre estilos plata mariposa cerró historial olímpico agotamiento producido abundancia peso reparador medallas oro plata bronce the end</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>0</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Deportes_58.txt</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -607,11 +672,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>aficionados sorprenderán mirar clasificación euroliga armani milan clasificado victorias jornadas situación crítica equipo aspirante año reforzó nombres importantes funcionando queda euroliga realidad victorias puestos playoffs analizamos causas naufragio italiano acumula derrotas consecutivaslesiones encadenadasla realidad justos armani milán prácticamente podido plantilla completa euroliga lesión duda marcado shavon shields problemas aquiles jornada daño partido bayern vuelto jugar sufren ausencia meses kevin pangos deja tocado puesto base perdieron compromisos billy baron naz mitrou long stefano tonut juega jornada luigi datome podido jugar partidos euroliga recién llegado luwawucabarrot retirar partido baskonia fuerte golpe cabeza impidió regresar encuentro carrusel bajas importantes shields recambio natural equipo reinventarse semana continuidaddudas confección plantillafue verano intenso milán marcha sergio rodríguez malcolm delaney provocaba cambio estructural importante equipo italiano apostó fuerte kevin pangos debía romper cska johaness voigtmann salió rusia planificación funcionando dupla bases pangos mitrou long jugar equipo resolutiva juego interior deshaun thomas fichajes juega minutos partido voigtmann promedia discretos puntos partido brandon davies superado valoración partidos euroliga rendimiento discreto incorporaciones caché europa cromos plantilla estructuradas rotaciones roles ataque gente niccolo melli voigtmann hines hall versión problema reajustar minutos roles equilibrio complejoproblemas ataquees evidente ataque milán funciona soluciones probado messina hablamos equipo puntos mete partido euroliga cazoo baskonia presentan rating ofensivo competición puntos posesiones porcentaje triples porcentaje tiros equipo línea tiro libre rebote ofensivo aparece rebotes ofensivos capturas totales ataque posesiones fluidez problemas encontrar ventajas ataque messina ido cambiando rotaciones obligado lesiones buscando soluciones conseguido atascos provocado problemas espaciado abuso media distancia tramos falta soluciones ofensivas jugadores devon hall promediando tiros triples cartas tiro equipo italiano temporadael puesto basees punto clave baloncesto europeo armani milán dando clave partidos kevin pangos recambio garantías ausencia mitroulong pangos lesionado mitroulong asumir rol costando partidos anotaciones zalgiris frente fenerbahçe choque cazoo baskonia desastre tiros valoración bases ganar euroliga messina derrota buesa arena equipo acudirá mercado ficharon luwawu cabarrot desmentido negociado facundo campazzo mitroulong seguir asumiendo peso ofensivo equipo dudas puesto toma decisiones errática pistala defensa único salvablesorprendentemente equipo italiano presenta defensa euroliga rating defensivo puntos encajados posesiones exterior bajar datos asistencias forzar pérdidas rival equipo muestra cara defensiva dato paradojico preocupante atasco resuelve cambio actitud baskonia partido sufrieron rebote ofensivo concediendo tope temporada problema milán resumen cemento bloque sólido defensa soluciones ataqueel caso brandon daviesen capítulo fichajes brandon davies llamado incorporaciones rindiendo nivel esperado encuentro baskonia escarmiento messina jugar duelo fenerbahçe volvió liga italiana brilló cazoo baskonia puntos rebotes encuentros superado puntos choques graves problemas faltas limitado promedia ′ pista puntos rebotes brandon davies determinante vimos tramos barcelona justificando fuerte inversión económica armani milán él¿messinala realidad milán funciona banquillo institución europea ettore messina vemos equipo plano fantasía explosividad ofensiva jugadores años mike james sergio rodríguez kevin punter banquillo messina cómodoel equipo deprimido derrota baskonia semanas amagó dejar banquillo principal responsable equipo equipo juega siento responsable reunido equipo click único manejar situación italia euroliga seguimos jugando sacaré conclusiones iré señor armani diré necesario encontrar guía equipo perder efes llegado derrotas máshablamos técnico ascendencia enorme club responsabilidades director deportivo christos stavropoulos ¿se echar messina ¿se iría sucedió etapa real madrid capaz reconducir rumbo calendario llevará milán visitar oaka enfrentarse panathinaikos posteriormente recibir maccabi viajar belgrado enfrentarse estrella roja veremos cambia situación equipo italiano</t>
+          <t>británicos piensa brexit frente opina sondeo yougov cree alturas salir ue decisión equivocada sostiene decisión correcta encuesta reciente statista convencido brexit vida diaria servido disparar facturas cesta compra sondeo ipsosy pese recelo creciente votaron favor divorcio europa candidatos conservadores boca agua hablando oportunidades brexit prometido fieles presagio lanzado semana boris johnson partida significa brexit piensan equivocados demostrarhasta líder oposición laborista keir starmer defensor permanencia regurgitado lema rival quiero brexit funcione declarado intención reabrir heridas explorar opciones futuro ingreso mercado únicolos políticos quieren hablar tema dimisión johnson hito destino brexit escribe jonathan freedland the guardian autor salida reino unido ue caído proyecto desastroso seguir caminorecuerda freedland victoria referéndum apoyada falsedades marcado años gobierno boris johnson empezando ahorro millones libras semanales millones euros pintado famoso autobús rojo campaña vote leave realidad sirviendo desacreditar brexit sostiene columnista crecimiento lento facturas altas problemas constantes ausencia beneficios concretos saltan vista sigan usando palabras abstractas libertad soberaníadurante debate televisivo brexit convirtió arma arrojadiza candidatos rishi sunak desperdició oportunidad lanzarle liz truss pregunta incisiva noche arrepientes liberaldemócrata apoyado permanencia uela secretaria exterirores corrió cortina jactó haberle impulso brexit gobierno firmando acuerdos comerciales japón australia parecían impensables plantando cara ue negociación protocolo irlandalos candidatos conservadores profundamente brexiterosconsciente tirón ideológico brexit ala dura partido secretario tesoro rishi sunak marcó tempo debate candidatos conservadores cadena itv prometiendo revisión reforma derogación leyes transferidas ruptura bruselasgracias brexit reino unido siglo xxi nación soberana global defensora comercio libre control leyes regulaciones política comercial internacional anticipó sunak prometió sustitución actual ministerio oportunidades brexit llamado brexit delivery department departamento entrega brexit montasunak defendió salida ue referéndum dudó desempolvar remainer rival secretaria exteriores liz truss terminado explicar razones fondo conversión quiero hijas crezcan mundo necesiten visado permiso europa empresas puedan crecer costes barreras comerciolos defensores liz truss ministro brexit david frost arroparon candidata recordando firmeza hora impulsar unilateralmente ley protocolo irlanda frente postura blanca sunak advirtió frost hagas saltar aires negociaciones ueel veterano diputado bill cash apoyo domingo liz truss comparándola margaret thatcher determinación hora frente ue pidiendo brexiteros unan fuerzas candidatura atrás julio sabrán nombres finalistasla candidata predilecta bases penny mordaunt defendió expediente favor brexit campaña referéndum frente ofensiva mediática defensa derechos trans diputada kemi badenoch representante ala dura incondicionalmente favor brexit quinto discordia moderado tom tugendhat contrario salida ue muestra travestismo político reiteró compromiso exprimir oportunidades brexit llega ministro</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Politica_46.txt</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -620,11 +690,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>adiós eurobasket tropiezo mondelo equipo valencia medallas seguidas colgadas cuello pelear acabar mejores premundial australia año derrota bielorrusia pagado cara serbia cuartos rival querían enfrentar reconocía laia palau octava seleccióntodo distinto baloncesto cristina ouviña tiros libres falta segundos españa falló partido prórroga extra serbia anderson carrera vasic entonada jovanovic matando partido españa negada canasta minutos tiros libres ouviñala base anotó puntos españa partido inauguró marcador triple únicos lanzamientos puntos ndour españa metió descanso muñeca serbia llevado partido terreno puntos contacto marina maljkovic escatimó salida centímetros atragantaron selección costaba balones llegaran ndour pintura hispanosenegalesa ouviña anotaron tantos españa asaltopero hija boza guardaba as manga desparpajo anderson metió problemas faltas selección abrir cerrar ojos maite cazorla cometió minuto tiro libre serbia puso españa metido lleno trampa serbia rival afortunadamente tiro larga distancia descanso tierra tiradores puntería mitadraquel carrera despejó dudas ataque defensa robo culminó contraataque canasta aro puso selección min españa parecía comenzar carburar motor apagó minutos anotar serbia aprovechó reducir distancia astou arregló entuerto descansoen tercer cuarto serbia disfrutó ritmo jovanovic alero empató partido encestó triple equipo colocó españa vivía dejado contagiar caos rival salvó papeleta tiros libres ouviña cuarto jugarla selección dominaba rebote cometido demasiados errores pérdidas fallos tiro españa gozó renta puntos minutos acciones seguidas anderson acabaron ventaja serbia llevaba falta puso segundos bola españa ouviña tiros libres entró españa historia eurobasket</t>
+          <t>año carlos alcaraz explotó us open partido nivel mundial ganó ronda sets stefanos tsitsipas número ranking años exhibición fuerza tenis regaló espectadores arthur ashe gesta vuelta orbe vi golpear pelota fuerte griego perdió murciano temporada miami barcelonaalcaraz acumuló hitos precocidad hueco élite confianza actuación cuarto major alcanzó cuartos retiró lesión perdía augeraliassime disparó rendimiento circuito semifinales viena triunfo cuartos top matteo berrettini parís bercy jannik sinner ganar nextgen atp finals milán deshizo sebastian korda partido título sueño número mundo trabajaré allá ganar torneo objetivo seguiré enfocado ganar nextgen finals significa motivación cara año viene seguir entrenándome tope mejorando próximas atp finals objetivo chulo difícil diría imposible lucharemos trabajaremos lograrlo imaginaba diez meses clasificadosu objetivo top acabó curso número disgusto supuso jugar finales copa davis españa contraer covid justo comienzo ranking inicio caer ronda open australia sets berrettini ganó atp río janeiro torneo obtenido victoria atp ganó albert ramos años brasil levantó trofeo carrera umag julio entró top preparado entrar nivel advirtió prodigio palmar décimo carrera copa maestrospor debutó armada davis victoria rumano copil eliminatoria clasificación disputó marbella despegue semifinalista indian wells nadal cuerdas campeón español miami impuso ruud rival título liderato mundial us open tropiezo prematuro montecarlo korda triunfó metió top barcelona carreño madrid ganó masters frente zverev derrotado alemán cuartos roland garrosmiro ranking asombroso entreno ganar plazas importante advirtió caer octavos wimbledon sinner superó umag carlitos venía perder hamburgo musseti premio número jugó montreal cincinnati resultados discretos auguraban excelente desempeño us open tsitsipas acumula victorias títulos número joven historia excelente</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>0</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Deportes_14.txt</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -633,11 +708,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>discusión eterna baloncesto grande tiempos pelea encabezada leyendas michael jordan anillos campeón icono trascendió allá baloncesto chicago bulls lebron james elegido años carrera anillos legado gigante prefieren mj grandeza lbj jugador discusión fomenta nbahay apoyos fuertes candidatura lebron draymond green otrora enemigo finales cleveland cavalliers golden state warriors apoya pasó the shop programa produce james hbo equipo títere cabeza lebron grande punto vistalo justifica longevidad cima empezó seguía jugador nba importar pasase juego visto juego hombres hombres relató drayy sufrió carnes james michael jordan batió equipo jamás creado warriors curry klay thompson draymond green temporada tiempos victorias derrotas cayó finales nba cavs lebronademás finales green vitales discusión años agotador competir finales año año nueve seguidas jordan parar descansar lebron finales señalótambién apoya juego fijas habilidades jugado juego baloncesto lebron james quieren jordan entiendo forma controlar partido imposible parar confesó sustenta cree talento juego vendrán viejos realidad apple mejores ingenieros analizóuna unión hechos longevidad talento rendimiento alto discusión años locura sentenció estrella warriors dudas lebron james tiempos</t>
+          <t>vayas muro andrea stella nervioso hacía bailaba pie derecho fernando alonso volaba asfalto shanghai rápido respondió tranquilidad jefe fórmula piloto volvió demostrar piloto mundo asturiano ofreció lección pilotaje inteligencia ganador ganó diez segundos ventaja kimi raikkonen doce lewis hamilton podio campeones carrera sebastian vettel cuarto jenson button quinto campeones mundo primeras posicionesveníamos advirtiendo alonso opciones victoria estrella ferrari coche competitivo trabajado duro piloto necesita dato preocupante felipe massa terminó sexto cuarenta segundos compañero realidadpues opiniones hechos evidente alonso preveían dispone coche jefe amo recuerdan asturiano disfruta valen dinero representante costar jefe jerez subió minardi cogía monoplaza consiguió renault dibujaba estrellas pista ofreció españoles deporte emocionarse sentirse orgullososdespués hamilton golpe tantas vettel títulos perdidos carrera desistió confiar genio asturiano pensaba sonrisas equivocaban ferrari esperaban optimistas presagiaban males eternos cuarto año dispone coche talento máscomenzó carrera tercero puso intentó meter coche hamilton llegaba vettel monstruo galletas neumáticos duros amenazando posiciones asturiano entró cambiar neumáticos medios vuelta comenzó carrera lucha hamilton kimi sebastian vuelta fernando adelantar di resta pérez button vettel hulkenberg pone líder tricampeón sonreír fernando gustándose parecía recta famoso drs sorprendió curva asturiano emocionó afición española esperaba sueño ferrari amo señor carrera hamilton raikkonen vettel intentando estrategia blandos funcionara alemán terminó cuarto estela hamilton sufría gomas medalla chocolate compañero mark webber rueda primeras vueltas pasan alonso luchar mundial terminado carreras ganó abandono malaisia líder destacado vettel kimi asturiano eterno capaz cantar himno letra miles chinos banderas españolas asturianas alonso vuelve jefe</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>0</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Deportes_10.txt</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -646,11 +726,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>baloncesto silla ruedas deportes populares programa paralímpico disciplina nació objetivo rehabilitar soldados norteamericanos heridos ii guerra mundial rápidamente ganó popularidad tanta actualidad practica países juegos paralímpicos escenario deporte jugadores oportunidad ganar oro respectivos paísesreglas juegaaunque modalidad parezca deporte similar baloncesto pie reglas básicas comparte basket conocemos siguienteslos equipos constan doce jugadores máximo pistala cancha medidas canastas situadas alturael sistema puntuación exactamente puntos canastas logradas partido tiro libre encestado balones anotados línearealmente diferencia modalidad pie normaslos jugadores deberán botar pasar balón empujar silla ruedas vecesa jugador asigna puntuación habilidad funcional escala menor juego suma puntos deportistas cancha pasar categoríasel baloncesto paralímpico silla ruedas categorías nivel discapacidad jugadores máxima juegos paralímpicos plenaigualdad participantes selecciones enfrentan únicamente disciplinascategorías baloncesto silla ruedasbc jugadores parálisis cerebral utilizar manos pies ayudantebc bc capacidad funcionalbc jugadores parálisis cerebral discapacidad locomotriz extremidades disputar encuentros ayuda dispositivos especialesbc deportistas parálisis cerebral discapacidad extremidades capacidad funcional similar categoría bcla competición comenzará oficial agosto terminará septiembre jugará finaldel agosto partidos fase grupos edición grupo grupo bla ronda jugará septiembre</t>
+          <t>registro mundial trasplantes gestiona organización nacional trasplantes ont años colaboración organización mundial salud oms estima número trasplantes órganos sólidos efectuados mundo año representa aumento año trasplantesde riñón hígado corazón pulmón páncreas intestino único baja levemente año datos recogidos newsletter transplant publicación oficial comisión trasplantes consejo europasegún explicado europa press director organización nacional trasplantes ont rafael matesanz destacar aumento significativo trasplantes mundo añocuando visión global ocurriendo mundo ve realmente países creciendo inmensa mayoría tomado referencia sistema organizativo parecido español añadidoasí matesanz destaca crecimiento américa latina dato parado crecer españa empieza colaboración forma estructurada coordinadores programa alianza cooperación formación profesionales trasplantesel crecimiento donantes zona mundo zona mundo crecimiento añade concretamente publicación año efectuaron donantes órganos procedentes personas fallecidas aumento permitido trasplantes supone trasplantes año anteriorla publicación consejo europa incluye datos eeuu canadá australia países estancados cifras donación señala matesanz eeuu tasa donación permanece estable años oscila donantes millón personas canadá desciende puntos tasa donación sitúa australia eleva ligeramente alcanza donantes millón personasdel informe destacar fallos matesanz observa nivel mundial debería crecer velocidad creciendo realmente esfuerzos zonas mundo ritmo crecimiento debería destaca crecimiento donantes europa año crecido décimas pasando directiva europea donantes donantes millón personas significa crecido alegríasen futuro destacar evidencia países tomado enfoque modelo español copiado adoptado principales características creciendo mundo espera crecimiento países emergentes acaba producir principal fallo global</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Salud_25.txt</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -659,11 +744,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>max verstappen consiguió domingo octava victoria temporada fórmula cantidad triunfo logrado circuito américas encabeza lista favoritos helmut marko asesor deportivo red bull racingla victoria austin absolutamente mejores carreras visto max comenzó marko entrevista exclusiva motorsportcom países bajosal principio significativamente rápidos mercedes neumáticos medios hamilton pudimos convertir ventaja ganancias neumáticos duros mercedes realmente rápidospor marko alaba verstappen marcara diferencia fase complicada carrera ronda pits lograron undercut adelantar detención piloto campeón mundo sencillodespués parada max salió rápido resultado neumáticos evaporaron parada aprendió claramente max frenó deliberadamente curvas marko movimiento calificó gestióncomo resultado hamilton acercó max pusiera nervioso hamilton segundos max volvió acelerar vuelta mercedes vio posibilidad jugado nosotrosese juego recordó marko victoria verstappen fórmula circuit barcelonacatalunya apuntó viejas características presentes austinexactamente combinación gestión velocidad ahorro neumáticos demostró barcelona gusta comparar victoria aquellala comparación válida razón españa verstappen concentró puntos clave circuito austin mayo atacó sector texas enfocándose curva zona drs hamilton llegar curvas sverstappen formaun aspecto impresionó marko cooperación verstappen estrategia cabina dividiendo labor conducción ayudar planificación personas situadas muro boxeseso extraordinario modos pensábamos meter sergio pérez pits directamente hamilton pudiera continuar mensaje max radio miren háganlo demuestra queda capacidad pensar estrategia carrerasmarko aplauso extra verstappen sentía domingo sucedió pérez presentó malestar estomacal previo competenciano completamente forma desmayó ejercicios respiración líquido consiguió superarlo bajó coche victoria diría inestable pies choque silverstone compara austriaco años impacto fuerzas sufrido colisión lewis hamiltonlos esfuerzos verstappen recompensa puntos rival campeonato carreras concluir temporada</t>
+          <t>mireia belmonte campeona olímpica nataciónbelmonte acabó domingo julio cuarta estilos jueves julio luchar preliminares libre nadadoranacida badalona barcelona año mireia belmonte garcía presumir nadadoras mayores triunfos país campeona olímpica mundial europea normalmente compite categorías estilos mariposa librese mueve agua llevado alcanzar triunfos repasamoscuándo empezó participar jjoono presente juegos olímpicos tokio importante trayectoria debutó competición olímpica años jjoo pekín año posteriormente jjoo londres estrenó medallero olímpico platas mariposa libres imparable ganando campeonatos europeos mundialesen juegos años londres río janeiro brasil subió pódium campeona olímpica mariposa consiguiendo medalla bronce estilosen tokio disputa pruebas libre juegos protagonismo medallas piragüista saúl craviotto abanderada española ceremonia apertura juegos marcados pandemiaotros campeonatosmireia belmonte cosechado triunfos olímpicos causan sensación visto millones personas mundoasí destacar medallas campeonato mundial natación años diez medallas campeonato mundial natación piscina corta años referimos datos victorias cosechadas nivel europeo destacar trece medallas campeonato europeo natación años once medallas campeonato europeo natación piscina corta años</t>
         </is>
       </c>
       <c r="C18" t="n">
         <v>0</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Deportes_54.txt</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -672,11 +762,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>francia nicolas batum suspendido aire taponando balón prepelic puesta escena doncic argentina despedidas gasol scola imagen torneo baloncesto tokio francia sueñan salto batum prolongue llegue cielo selección vincent collet logre imposible madrugada viernes sábado ganar consecutivas unidos torneo oficial colgarse oro olímpico historia francia mandó vuelta casa unidos dongguan mundial china aparentes dificultades puntos fournier puntos rebotes gobert jornada fase grupos juegos fournier gobert repitieron actuación francia iluminada difícil pensar suficiente ahoraporque números team llegado saitama misión vengar derrotas francia limpiar nombre japón mundial cayó semifinal sorprendente grecia pese equipo campanillas fiasco atenas sensación chicos popovich llegaron dudas malhumorados japón extraña concentración vegas terminado entenderse jugamos países repiten equipo año año jugadores conocen campeonatos juntamos equipo menor consiguiendo lillard semifinal australiapopovich kerr team consciente desventaja verano vertebrar récord selecciones año bandera agarrarse líder define devin booker kevin durant años jugador washington echado team espalda ratitos apuro españa australia exhibido encontrado camino fino seda durant persigue tercer oro consecutivo convertiría leyenda juegos olímpicos puesto carmelo llegado cifra abriría puerta participación parís años vistalas apuestas volcadas favor unidos querido pegar pisotón acelerador francia necesita partido perfecto fournier gobert colo nivel semifinal luwawu jugador anónimo empezó romper eslovenia triple decisivo minuto aparezca noche larga francia viernes veremos avanzó scariolo oro reservado unidos</t>
+          <t>restos dictador francisco franco saldrán valle caídos periodo octubre consejo ministros aprobado viernes exhumación inhumación establece horquilla plazo previo avisar familia vicepresidenta gobierno funciones carmen calvo anunciado rueda posterior reunión gabinete socialista funciones tribunal supremo respaldo legal pretensiones ejecutivo cálculo moncloa octubreel presidente gobierno funciones pedro sánchez llevado asunto consejo ministros pese formado reunión preparatoria previa comisión secretarios subsecretarios presidencia potestad sánchez ejercido temase tercer sacar franco llegada psoe moncloa junio año pronunciamiento previo congreso modificación ley memoria histórica darle cobertura legal quiso ejecutarse pasadas navidades estableció fecha junio falta familia recursos tribunal supremo demorado cumplimiento promesa ocasión ordena inmediata viernes cierre temporal valle caídos finalización operaciónahora nietos dictador acudido constitucional paralizar in extremis traslado restos cementerio pardomingorrubio ejecutivo decidido ejecutar sentencia supremo manos libres actuar quierael gobierno semanas plazo razón fuentes consultadas coincidencia sentencia procés conocerá próxima semana cuyas consecuencias cataluña inquietan ejecutivo querido fijar fecha exacta preferido dejarlo abierto elegir adecuado función suceda cataluña fechas apuntadas fuentes gobierno posteriores comunicación sentencia convocatoria huelga comunidad prevista movilización electoradola decisión exhumar franco producirá campaña electoral oficialmente comienza noviembre partidos especialmente sánchez inmersos larga precampaña calvo defendido escogido deseo gobierno socialistas piensan traslado restos franco contribuye movilización electoradopara gobierno vicepresidenta supone satisfacción extraordinaria cerrar dignidad digno años referencia tumba franco enterradas víctimas bandos exhumación justificar apunte fecha concreta hará gobierno funciones disponga medios técnicos seguridad permitanse realizará arreglo criterios fijado gobierno resoluciones anteriores reiterado calvo procederá absoluto respeto restos familia avisará antelación discreción nietos bisnietos deciden celebrar ceremonia acorde preferencias religiosas adoptarán medidas necesarias seguridad restos mortales seguridad ciudadana orden público ejecutivo descarta restos puedan trasladar helicópteroel consejo ministros establece actuaciones exhumación traslado inhumación presenta ministra justicia dolores delgado condición notaria reino cámaras medios comunicación caso presentes explanada</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Politica_30.txt</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -685,11 +780,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>lamentablemente delegación mexicana participa juegos olímpicos tokio jornada resultados positivos competidores disciplinas escasos posibilidades medalla esfumaron quedaron camino competenciassin duda eliminación dolorosa méxico ocurrió tiro arco alejandra valencia cayó estadounidense mackenzie brown duelo máximo flecha desempate competidora barras estrellas terminó círculo central dejar arquera aztecapor clavados aranza vázquez logró colarse ronda trampolín metros individual femenil finalizar ronda preliminares octavo caso contrario compatriota aratxa muñoz lamentablemente erró saltos recibió calificación cero dejándola competenciala selección mexicana beisbol debutó juegos olímpicos desafortunadamente bateo escaso novena verda derrotados república dominicana pizarra arranque atletismo tokio méxico ventana oportunidades pies edgar rivera originario agua prieta sonora terminó participación quedar octavo grupo preliminatoriootra esperanzas país competencias julio dafne navarro gimnasia trampolín calificó resultado óptimo competencia medallas mexicana terminó lugarmientras boxeo rogelio romero eliminado cuartos peso semipesado sucumbir frente arlen lópez cuba cartones mexicano termina participación justa veraniegaeste contenido vídeo disponible zona geográficacarlos ortiz convirtió esperanza medalla méxico finalizar boxeo clasificación tarjetas estadounidense xander schauffele compatriota abraham ancer ubicado posición</t>
+          <t>vitaminas lociones champús tratamientos cosméticos utilizados tratar alopecia efectividad médica frenan caída cabello asegurado coordinador unidad tricología hospital ramón cajal madrid sergio vañó jornada trastornose problema médico necesita valoración adecuado tratamiento combatirlo cien causas origina pérdida pelo terapia frene definitivamente problema métodos técnicas médicas ayudan retrasar tipos alopecia tratamientos factores crecimiento farmacológicos asegurado especialista demostrado efectivos perfil seguridadahora múltiples factores originan alopecia vañó recordado comunes hormonales provocan alopecia androgenética producidos cambios ritmo vida originan alopecia efluvio telógena autoinmunes ocasionan conocida alopecia areataéstas formas frecuentes causas caída pelo trastornos alimentarios déficit hierro alteraciones tiroides provocadas determinados medicamentos enfermedades sistémicas señalado vañótodos proseguido factores afectan importante calidad vida pacientes demostrado alopecia enfermedades cutáneas procesos afecta calidad vida personasademás experto informado mujeres padecen cáncer plantean someterse tratamientos quimioterapia evitar caída pelo darle nivel médico institucional importancia proceso pacientes pasan apostilladodicho vañó explicado principales líneas investigación médica enfermedad centrado medicina regenerativa factores crecimiento células madre obstante reconocido diez años marcha aplicación prácticapor dermatólogo participado curso actualización tricología organizado hospital ramón cajal insistido importancia personas sufren caídas severas cabello acudan especialista farmacéutico centro cosmético médicos capaces retrasar eficazmente alopecialos pacientes problema médico piensan cosmético acuden centros belleza realidad alopecia enfermedad hipertensión diabetes requiere valoración adecuado tratamiento médico zanjado</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Salud_39.txt</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -698,11 +798,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>presidente comité olímpico español coe alejandro blanco valorado miércoles decisión federación tiro arco volver juego plaza olímpica asegurado respeta normas pone federación conceder billete juegos tokio aplazados encuentro telemático ufedega unión federaciones deportivas gallegas comité olímpico español blanco interpelado presidente federación gallega tiro arco decisión tomado deportista gallego miguel alvariño ganarse billete tokioespaña plaza tokio asegurada verano mano pablo acha clasificatorios juegos olímpicos arquero gallego adjudicó volverá disputarse billete presidente coe distinguió hora clasificación jjoo clases deportes equipo ypor individuales diferencias casos deportista gana plaza juegos acudir gana país representa tiro arco ganado deportista plaza país pablo acha federación plaza jjoo pongo serie condiciones razonó blanco recordó potestad tomar decisión requisitos clasificarse tokio federación deportivacorrespondiente plaza país coe presenten equipos potestad entrar decisiones tome federaciónademás alejandro blanco deseo gobierno acelere desescalada deportistas puedan regresar entrenamientos hice peticiones corresponde debemosser iguales desescalada responsable coe trasladado ufedega comunicado puedes argumentar razonablemente futbolista entrenar piragüista tenista judoca ejemplos puedan pedido gobierno acelere desescalada</t>
+          <t>vicepresidenta congreso diputados celia villalobos cargado diario mundo publicar portada foto móvil alfredo pérez rubalcaba cuya pantalla leerse mensaje privado referente eventual futuro alberto ruizgallardónen programa radio nacional villalobos afirmado cosa presentable periódico refleja dedos señor pérez rubalcaba móvil mensaje privado llega serestá hagan foto rubalcaba actitud móvil absolutamente privado mensaje privado posiblemente brete respetarlo agregado ministra sanidad aznarvillalobos supervisando fotógrafos foto barbanchovillalobos supervisando fotógrafos foto barbanchovillalobos equiparado violación privacidad reporteros gráficos fotografiar papeles anotaciones realizadas mariano rajoy responder portavoces grupos intervinieron congreso cámara respetar intimidad personasla portavoz popular soraya sáenz santamaría dirigió fotógrafos entender tomando imágenes papeles rajoy villalobos pidió reporteros gráficos mostraran material capturado accedieron pese obligados tratarse espacio público imagen villalobos comprobando cámaras reporteros publicada mundo edición diciembrele diciendo fotógrafos favor saquéis cámara pedazo teleobjetivos papel escrito mano señor rajoy respetar concluido vicepresidenta cámaraa pregunta juan ramón lucas equipararse frases cazadas micrófonos indiscretos villalobos respondido hombre oculta mujer muerta mujeres equivocar añadido mujer twitter facebook periodista masculino ingenioso dedica artículos tivalenciano defiende privacidad rubalcabapor secretaria política internacional cooperación psoe elena valenciano defendido privacidad móvil rubalcaba debería consentir hagan fotos leer perfectamente mensaje textoen declaraciones telemadrid valenciano referido foto publicada mundo aparece móvil ministro interior mensaje texto leer informadora ayto madrid gallardón defensavalenciano señalado problema haga foto móvil privado publique página periódico mensaje privadosobre persona informa rubalcaba mensaje futuro político alcalde madrid valenciano idea apuntado alguien psoe pp periodista definitiva gente caso relevante valenciano rubalcaba informan buscado información</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Politica_17.txt</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -711,11 +816,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>proceso selección equipo nacional arco adaptado arrancaba febrero deportistas participantes distintas categoríasopen recurvo open compuesto vi vi temporada clasificatorio consta pruebas tirándose dobles rounds obtendremos promedio deportistas postre determinará clasificación representar federación citas internacionales temporada desafortunadamente crisis covid permitió concluir proceso selección aplazar temporalmente clasificatorios previsto celebrarse marzo fecha declaró oficialmente alarmaen resultados obtenidos deportistas participaban proceso selección suspendiera clasificatorio cabe destacar rendimiento mostrado arquero open recurvo josé manuel marín batía récord españa categoría pruebas clasificatorias celebradas andaluz alcanzaba puntos clasificatorio volviendo repetir puntuación doble prueba clasificatoria volverlo batir rounds clasificatorios prueba puntosen josé manuel único deportista cumpliría promedio mínimo referencia formar equipo nacional arco adaptado modalidad subvención completaotros deportistas promedio guillermo rodríguez open compuesto daniel martín vi adrián orjales vi cumplen momentos promedio copagoa destacar línea ascendente carmen rubio deportista open compuesto recuperarse desafortunada grave lesión sufría temporada progresión manuel sánchez reclasificación open compuestoen clasificatorios open compuesto participando jovencísimo adrián martínez duda experiencia sirviendo enormemente cara futuro experimentado fernando barredo mostrándose regular puntuaciones promedio copagoworld archery europe declaró recientemente suspenso actividad julio aplazando pruebas clasificatorias jjpp tokio previstas temporada campeonato europa arco adaptado previsto abril olbia italia copa europa arco adaptado celebrarse principio junio nove mesto república checa esfuerzos federación europea volcarán celebre temporada informaciones respectofinalmente reseñar comités olímpico paralímpico internacionales tomaron recientemente decisión aplazar jjoo jjpp celebrarán finalmente verano federaciones internacionales tomar decisión futuro calendario internacional reste temporada adaptándose restricciones marquen nivel salud públicaante enorme incertidumbre genera situación calendario previsión plantear rfeta mera especulación único conseguiría generar incertidumbre asumir caso sistemas selección puedan sufrir cambios fuere objetivo rfeta garantizar participación equipos mejores condiciones posibles pruebas referencia año</t>
+          <t>jefe ejecutivo josé maría aznar asegurado futuro país necesita coaliciones radicales estabilidad institucional levanten mañanas ejercicio voluntad propósito insultar españael presidente gobierno pp refirió situación postelectoral cataluña semanas escuchando exceso palabras verbos radicalesaznar consideraciones intervención tradicional cena navidad pp madrid celebró hotel afueras capitalademás recordó imagen secretario psoe josé luis rodríguez zapatero sonriendo complacidamente balcón palacio sant jaume jefe independentistas catalanes referencia líder erc josep luis carod roviraesa imagen verse toma posesión pasquall maragall presidente generalitat pacto socialistas recordó quieren independencia españa antipática sienten cómodos quieren marchartambién lamentó palabras maragall riesgos drama situación subrayó levanten mañanas ejercicio voluntad propósito insultar españafrente pp seguir defendiendo convivencia solidaridad futuro progreso todosno sacar radicales pongan tranquilidad moderación sosiego firmeza encontrar comportamiento partido pensando interés país añadiócenarato rajoy posan cocineros restaurante madrid cenaron efepara aznar españa necesita gritos radicales tensar cuerdas organizar drama continuidad histórica estabilidad institucional políticas reforma seguir progresocon coaliciones radicales juicio gobierna ayuntamiento comunidad autónoma españa necesita radicalismo unidad garantiza pp candidato presidencia gobierno mariano rajoyun pacto cree nadiepor rajoy acusó presidente generalitat pasqual maragall apostar modelo financiación cataluña arreglar problemas generado firmando pacto cree psoe pp avalarárajoy subrayó gana elecciones acción política centrará impulsar españa unida solidaria caben modelos económicos sociales apuesten diferencias territorios propuestas cambios constitución estatutos pactados plan ibarretxerajoy determinación lograr presidencia gobierno pidió esfuerzo dedicación militantes lograr meta gracias aznar base partido cohesionado unido proyecto españa ideas llevarlo término</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Politica_25.txt</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -724,11 +834,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>permíteme dato explicarlo técnicos presupuesto corea sur tiro arco millones euros calcula rubén montes director deportivo federación española tiro arco acaba despejar incógnita ¿eso ¿el dinero ¿un montón dinero acabar amamos deporte incertidumbrevamos hechos corea sur ganado oros disputa juegos tokio lunes equipos categoría masculina camino pleno victorias consiguió juegos río país tirador capaz romper racha tiro arco suele abierto sorpresas atrás categoría femenina pierden equipos dejado escapar triunfo individual dream team baloncesto mantiene récord parecidoel arco flechas elementos deporte nacional país asiático indudable ¿cómo conseguido dominio abrumador tradición sitio escuelas primaria institutos universidades equipo tiro arco digo quiero excepción cantera arqueros inagotable cuentan estructura potente liga profesional clubes profesionales sueldos euros anuales media mejores prácticamente millonariosrecrear escenarioel presupuesto federación guinda pastel dinero compre permite tiradores dediquen exclusivamente entrenar mejores instalaciones juegos recreado seúl recinto olímpico construido idéntico tokio acostumbradísimos ambiente analiza montes recuerda coreanos cayeron mundial categorías chicos imbatibles chicas llevan ganando oro interrupción reconoce técnico analiza lanzamientos asiáticos concluye distinto descubierto truco inventado nadade kisik lee seleccionador coreano entrenador unidos corea sur utiliza técnica eficiente analiza biomecánica tiros centenares arqueros profesionales entrenar compiten semana rivales nivel ventaja difícil revertir finaliza montes espera competición queda llegue alegría españolaeste martes tifón permite daniel castro empezará cuadro individual masculino rival coreano kim woojin logra alcanzar cuartos derrotarle complicado realmente complicado montón dinero acabar amamos deporte incertidumbre</t>
+          <t>comité investiga asalto capitolio enero presentó pruebas martes presidente estadounidense donald trump planeó instigar seguidores acudir sede congreso círculo cercano reunió grupos ultra participarontrump escribió tuit envió mensaje conservan archivos nacionales suficiente comité demostrar trump consejeros interesados alentar masasel llamamiento líder republicano avanzaba iba discurso mañana pedía llegar multitudes previstas instaba gente dirigirse capitolio certificando votos condujeron investidura demócrata joe bidenla audiencia puerta abierta reflejó grupos ultraderechistas oath keepers proud boys lideraron protesta coordinado gente confianza trump contacto ellosdías asesor seguridad nacional michael flynn participara reunión despacho oval analizó revertir resultado elecciones fotografiado capitolio miembros destacados oath keepersasimismo colaborador roger stone usó chat encriptado coordinar esfuerzos escrutinio cierre urnas llamado amigos stone participaban miembros ambas organizacionesla audiencia martes séptima comité centró vínculos disparatada reunión diciembre despacho oval trump publicó tuit avanzaba iba protesta enero washington animaba acudir iba salvajeen encuentro insultos acusaciones deslealtad trump dictar decreto abogada sidney powell poderes incautar máquinas votación volver recuento papeletas precisó legislador demócrata jamie raskin miembro comitéfinalmente ganó común entiendo siquiera mala idea idea terrible país powell pat cipollone abogado casa blanca luchó esfuerzos presidente revertir resultado eleccionesel comité obstante descartó martes trump manipulado ignorar asesores cercanos creer fraude electorales hombre años niño impresionable mundo país responsable acciones decisiones acceso información detallada específica mostraba elección robo legisladora liz cheney republicanos forman comité enfrentada mandatarioinstigación armaspor criticó siguiera denuncias mensajes interpretados llamamiento protesta armas extremistas hablaron abiertamente internet acudir armados capitaluno stephen ayres entró capitolio aferraba palabra trump intervención martes convencido elección fraude presidente republicano iba gente protesta enerolos mensajes circulaban redes sociales mayoría naturaleza violenta hablaban celebrar boda roja recordó raskin martes sirve hablar clave masacrelas reuniones casa blanca trump siguiera variadas diciembre comité participaron once republicanos presionó vicepresidente mike pence ayudara darle vuelta resultadosel comité promete revelaciones próximas audiencias reveló cheney trump intentó llamar testigo declarado rechazó responder advirtió abogado tentativa</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Politica_53.txt</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -737,11 +852,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>tíos arcos flechas sonaba viejo cuento mitología cualquiera héroes pegados artilugio ¿el tiro arco gente españa sabía deporte relacionaban robin hood películas… explica juan carlos holgado cáceres miembro tridente antonio vázquez aller asturias alfonso menéndez presentes podio competición ponerse lanzar clavaron flechas dios cupido indiferenciaen diarios aparecían opciones medalla llegué tiro arco ponía ¡demoledor recuerda holgado lanzar flechas llevaba cupido dorada amor enamorar oro finlandia agosto subían vall dhebron olimpo elevado antonio rebollo arquero español excelencia arqueros españoles entrenador ucraniano victor sydoruklos arqueros españoles entrenador ucraniano victor sydoruk eduard omedesel flechazo antonio vázquez sangre fría sensible prisas flecha lanzar impacto amarillo puntos victoriosos marcador ¿nervios miré reloj marcador simplemente pendiente gente chillaba oía sofrológico importante mariano espinosa explica rebollo inauguración difícil disparó flecha fuego caído llegar pebetero gente había…¡la liado asegura asturiano enero sponsor retiró patrocinio falta resultados ¡ellos perdieron añade pícara sonrisa vázquez contaba único objetivo pasar ronda dinamarca ronda liberamos asegurado beca año claves supimos jugar viento señala alfonso menéndez actualidad gerente club natación santa olaya gijón tantos flechazos gente encaprichó trío cuya cortado telediario amor repentino antonio look ideal celebridad abundante revolucionado pelo afro asustónos hicimos famosos golpe pelo afro decidí cortármelo pasar desapercibidoantonio vázquezyo reservado sentía agobiado anónimos fama futbolistas llegué pueblo asturias tardé hora recorrer metros casa peluquería gente agasajaba llegué peluquería dije barbero quitara pelo quería pasar desapercibido dudando ¡al salir tardé minuto volver casa camino explica partiéndose risa antonio vázquez entrenador federación catalana tiro arco monitor club olesa montserrat divina historia sobrehumano surgida flechas lanzadas años razón diarias crudeza dureza intransigente método soviético ucraniano victor sydoruk entrenador cincuentón vuelta coronel ejército urss campeón mundo tiro arco dejar lucha grecorromana lesión rodilla devoto teorías charles darwinholgado vázquez entreno competiciónholgado vázquez entreno competición pep moratalos quedamos juegos pura selección natural únicos lesionamos entrenamientos durísimos hacíamos sesiones nocturna cenar mandó golpe casa valían explica vázquez cascarrabias frecuente reparos sydoruk volcar rabia sentía ilustra anécdota holgadoyo quería campeonato regional madrid victor dejaba acabar cogió pechera llegamos manos puso doble entrenamiento desobediente guerra fría duro trato costó acostumbrarse cultura entendía pudiera utilizar instalación hora ocupada obsesión llegar españa pegó patada rabia piedra motivo rompió dedo pie mes escayolado disciplina ganar meses momentos tensión desgaste conllevaba familia caracteres superamos relata holgado director deportes federación internacional deporte universitariome emociona hablar victor sydoruk vive situación difícil ucraniaalfonso menéndezotra anécdota sucedió piscina natación formaba preparación física antonio sabía nadar victor ven enseñaré ¿sabes ¡le tiró agua alfonso rápido enseñarle método sydoruk supervivencia explica mondándose risa holgado hijo españoles nacido alemania trasladado años cáceres sentimiento sydoruk gratitud aspereza ternura hombre parco seco encajamos emociona recordar justo medalla victor ucraniano situación pasando suerte relación estrecha boda destaca voz quebrada alfonso menéndez sydoruk presidente federación tiro arco ucrania años energía admirable resalta holgadoalfonso menéndez foto actual oro barcelona medalla oro real orden mérito deportivo orden olímpicaalfonso menéndez foto actual oro barcelona medalla oro real orden mérito deportivo orden olímpica sergio vegasepultada dinamarca ronda cumplido expediente aguardaba relamiéndose favoritísimo oro equipo unificado nombre competían rusia resto países urss bálticos desintegración imperio soviético suerte echada abundante acumulado oyeron holgado vázquez menéndez susurrar mente arrebato patriótico sydorukya año rusos podéis perder sesiones castigo tema personal podíamos perder equipo rusia barcelona contento explica risas juan carlos semifinales tridente español despidió reino unido finlandia menéndez supimos jugar vientonosotros usábamos condones resto atletas villa ¡victor controladosjuan carlos holgadonuestra medalla explica puntuaciones hicimos sorpresa marcábamos entrenamientos pienso principal punto fuerte caracteres complementábamos virtud compensaba defecto extrovertido antonio introvertido alfonso punto compitiendo lanzaba miraba puntuación valoraba viento innovador equipo adaptara circunstancias destaca holgadojuan carlos holgado foto reciente orojuan carlos holgado foto reciente oroy vázquez menéndez holgado llevaron oro moldeado entrenamientos extenuantes convergencia caracteres concentración… abstinencia dormimos villa olímpica comimos entrenamos dormimos barcelona vivimos ambiente villa victor controlados decía villa dormir estadística quinto sexto juegos utilizan preservativos atleta ¡habría usaría vimos exclama carcajadas juan carlos holgado vieron afrodita lanzaron dorada flecha amor cupido españa gente tiro arco deporte medallistas olímpicos concluye holgado imprevistos héroes equipo español tiro arco bonita casualidad barcelona tiro arcocon gente miguel alvariño medalla olímpica ahoralo equipo español tiro arco barcelona aislado continuidad pudieron volver subir podio competición recortes plan ado alegrías juegos permanece única medalla olímpica españa deporte plata mundial victoria canadá josé ignacio catalán juan sancho antonio cerra único metal campeonato mundosin destaca figura gallego miguel alvariño junio alzó campeón europa tiro arco recurvo aupó número ránking mundial competición daniel castro gallego cuarto españa llevó plata equipos alvariño castro burgalés pablo acha predecesor alvariño prueba individual ganar título continental éxitos vienen creciendo abajo delegación española trajo medallas mundial juvenilelías cuesta trabajando seleccionador nacional haciéndose nombre miguel alvariño trabajado europeo logrado resultados arqueros golpe medalla olímpica destaca antonio vázquez metido tiro arco español entrenador federación catalana</t>
+          <t>baloncesto silla ruedas deportes populares programa paralímpico disciplina nació objetivo rehabilitar soldados norteamericanos heridos ii guerra mundial rápidamente ganó popularidad tanta actualidad practica países juegos paralímpicos escenario deporte jugadores oportunidad ganar oro respectivos paísesreglas juegaaunque modalidad parezca deporte similar baloncesto pie reglas básicas comparte basket conocemos siguienteslos equipos constan doce jugadores máximo pistala cancha medidas canastas situadas alturael sistema puntuación exactamente puntos canastas logradas partido tiro libre encestado balones anotados línearealmente diferencia modalidad pie normaslos jugadores deberán botar pasar balón empujar silla ruedas vecesa jugador asigna puntuación habilidad funcional escala menor juego suma puntos deportistas cancha pasar categoríasel baloncesto paralímpico silla ruedas categorías nivel discapacidad jugadores máxima juegos paralímpicos plenaigualdad participantes selecciones enfrentan únicamente disciplinascategorías baloncesto silla ruedasbc jugadores parálisis cerebral utilizar manos pies ayudantebc bc capacidad funcionalbc jugadores parálisis cerebral discapacidad locomotriz extremidades disputar encuentros ayuda dispositivos especialesbc deportistas parálisis cerebral discapacidad extremidades capacidad funcional similar categoría bcla competición comenzará oficial agosto terminará septiembre jugará finaldel agosto partidos fase grupos edición grupo grupo bla ronda jugará septiembre</t>
         </is>
       </c>
       <c r="C24" t="n">
         <v>0</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Deportes_38.txt</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -750,11 +870,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>sirenita michelle alonso santa cruz tenerife conquistó piscina oro metros braza categoría discapacidad intelectual registrando récord mundo prueba estrella corona londres revalidó río tokio demostrado reina indiscutible oros juegos incontestable canaria daba decimoséptima medalla españa sincera esperaba oro plata sabía rivales siento soñando sonar despertador medallas paralímpicas especial significado conseguirla tokio confesóeste oro redondear juegos papel protagonista nadadora elegida ricardo ten abanderada equipo español ceremonia inauguración vio desparpajo estadio nacional tablas michelle ejerció abanderada clausura ríounos problemas espalda lanzaron piscina años apuntaba maneras maneras recibieron mejores pensó marcharse volver problemas comunicación encajaba resto compañeras burlas tornaron situación insostenible ademi josé luis guadalupe alias guada mentor entrenador padre natacióny sirenita voz empezó hablar alto brazada metro recorrido ganaba confianza dejaba atrás rechazo compañeras daban discapacidad intelectual tokio deslumbrando carrera cimentada esfuerzo brilla base medallas sonríe disfruta países favoritos puesto loca sushi anime manga cultura japonesa pisa tokio últimaademás rostro michelle desconocido público nipón años protagonizó documental cadena nipona wowow michelle reina aguas mares resistan sirenita</t>
+          <t>inicio declive serena williams existido tanta unanimidad hora señalar jugadora principal favorita campeona roland garros vitola iga swiatek pronúnciese sbiontec temporada torneo sábado confirmó pronósticos incontestable triunfo minutos coco gauff polaca reeditó título conquistado ocasión barrió estadounidense sofia kenin años doble campeona torneo nueve jugadoras logrado open grand slams racha victorias consecutivas periplo triunfal perdido sets instala nómina leyendas alcanzado registros parecidos superiores invencibilidad navratilova graf court evert venus williams mencionada serenaswiatek perdona ganar juego pierde vuelve pista sed venganza engulle rivales gauff finalista joven major sharapova wimbledon clijsters roland garros perdido manga campeonato vio admiradora nadal ganado torneos curso pasaba americana reprimir lágrimas podido tenistas siquiera inquietar número mundo afianza ventaja líder ranking saca puntos estonia kontaveitt paula badosa quinta jugadora años vencer parís cabeza serieespero llorar arrancó entrega trofeos merecemos equipo años esperaba ganar duro presión necesario llegar justo acordarse ucrania seguid fuertes guerra continúa recibir atronadora ovacióncon mínimo despiste quiebre inicio set swiatek saldría victoriosa celebró grada equipo familia futbolista bayer suena barça robert lewandowski porcentaje triunfos roland garros tercero historia gauff disputaba grand slam queda consuelo disputará dobles compatriota jessica pegula espero juguemos finales ganarte sonriendo llorar lamentaba podido competir agradecía apoyo público deportetras celebración triunfo iga swiatek philippe chatrier acogió dobles masculino impusieron marcelo arévalo salvador neerlandés jeanjulien rojer croata ivan dodig estadounidense austin krajicek arévalo rojer supieron sufrir set salvaron puntos partido triunfo pareja entra libros historia dobles puesto neerlandés rojer convierte ganador grand slam edad años nueve meses superando meses mike bryanrojer convertía jugador edad disputar grand slam dobles suma victoria torneo ganó wimbledon us open impuso feliciano marc lópez ambas rumano horia tecau pareja compañero marcelo arévalo grand slam palmarés fecha salvador sumaba títulos torneos año rojer única historia ganando roland garros jugador centroamérica gana grand slam</t>
         </is>
       </c>
       <c r="C25" t="n">
         <v>0</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Deportes_18.txt</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -763,11 +888,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>mireia belmonte campeona olímpica nataciónbelmonte acabó domingo julio cuarta estilos jueves julio luchar preliminares libre ¿quién nadadoranacida badalona barcelona año mireia belmonte garcía presumir nadadoras mayores triunfos país campeona olímpica mundial europea normalmente compite categorías estilos mariposa librese mueve agua llevado alcanzar triunfos repasamos¿cuándo empezó participar jjoono presente juegos olímpicos tokio importante trayectoria debutó competición olímpica años jjoo pekín año posteriormente jjoo londres estrenó medallero olímpico platas mariposa libres imparable ganando campeonatos europeos mundialesen juegos años londres río janeiro brasil subió pódium campeona olímpica mariposa consiguiendo medalla bronce estilosen tokio disputa pruebas libre juegos protagonismo medallas piragüista saúl craviotto abanderada española ceremonia apertura juegos marcados pandemiaotros campeonatosmireia belmonte cosechado triunfos olímpicos causan sensación visto millones personas mundoasí destacar medallas campeonato mundial natación años diez medallas campeonato mundial natación piscina corta años referimos datos victorias cosechadas nivel europeo destacar trece medallas campeonato europeo natación años once medallas campeonato europeo natación piscina corta años</t>
+          <t>secretario psoe josé luis rodríguez zapatero anunciado programa electoral socialista comicios año incluirá propuesta modelo financiación comunidades autónomas adaptado proceso descentralización añosel líder socialista anuncio conferencia prensa sede federal psoe informar reunión comisión ejecutiva partido análisis significado año socialistasexplicó psoe apuesta desarrollo autonómico implica apuesta reforma estatutos autonomía marco proceso solidaridad regiones convivencia ciudadanos cohesión territorialfinanciacióninformó programa electoral contendrá propuesta modelo financiación autonómica recordó respaldamos parlamento modelo impulsó gobierno pp subrayó apuesta desarrollo autonómico desarrollo llegado rincones españadestacó propondrá modelo adecúe proceso descentralización vivido años modelo diálogo consenso fuerzas políticas gobiernos autonómicos marca ley orgánica financiación comunidades autónomas espíritu constitucióngobierno pprodríguez zapatero análisis acción gobierno pp resume diciembre alta crispación política evidenció despedida presidente gobierno josé maría aznar congreso semana pasadaafirmó año acaba fuertes tensiones territoriales ponen manifiesto gobierno pp transmitir mensaje confianza esperanza estabilidad españoles transmite mensaje incertidumbres temores crispaciónel equipo electoralpara superar situación zapatero ejecutiva socialista aprobado marcha inmediatamente parón navideño campaña programa cuya elaboración trabajará presidente castillala mancha josé bono presidentes autonómicos cuyos nombres reveló zapatero pidió felipe gonzález irá listas socialistasfrente opinan debate electoral cohesión territorial zapatero psoe centrará políticas sociales advirtió partido elaboración constitución modelo territorial defendimos gobernando trece añosvamos seguir impulsando autonomías líder socialista mostró convencimiento ciudadanos garantiza convivencia unidad respeto diversidad sitio capacidad diálogosubrayó apuesta mensaje positivo confianza creer constitución estatutos frente lanzan temores peligros riesgos absurdo modelo autonómico cerrado resumió planes reforma senado participación autonómica ue adecuación estatutos cambios registrados años</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Politica_28.txt</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -776,11 +906,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>david popovici bate récord libre natación destroza estigma bañadores prohibidosel rumano años establece marca segundos centésimas rápido logrado césar cielo bañador enterizo impermeablecaeleb dressel nadador rápido mundo bañador textil campeón mundial campeón olímpico naturalmente tratándose velocista unidos años apogeo junio mundiales budapest decidió retirarse competición alegando razones médicas especificadas justo constatar disputaría metros libre flaco pómulos salientes mirada brillante años largos semifinal segundos llamaba david popovicisi dressel huyó visión futuro inhóspito pareció razones faltaron futuro nado libre pertenecía tallo estatura inesperado extraño origen rumano previsible progresión sábado piscina foro itálico sede campeonatos europa natación popovici confirmó trayectoria devastadora anuncian marcas años ian thorpe convirtió campeón mundial prematuro tiempos años surgía nadador libre autoritario muchacho vida entrenándose club bucarest principales corrientes natación élite destrozó segundos récord mundial césar cielo enquistado memoria infausta bañadores flotantes poliuretanoexactamente siglo johnny weissmüller batiera plusmarca destino reservó círculo perfectamente irónico popovici convirtió hombre joven batir récord prueba legendaria natación localización carga simbólica piscina foro itálico viejos pinos escenario estableció récord precedente años atrás mundiales roma julio embutido mono goma ayudaba deslizarse superficie empleando fuerza sostenerle ocupaba tecnología césar cielo tocó pared gritó victorioso gloria brasil arena fabricante bañadores marca segundos acababa nacer parecía grabada piedra hombre rompiera debería nadar llevara incorporado artefacto flotador gamaprohibidos bañadores impermeables natación alumbró sobria espectacular armados bermuda tela agua fluía freno caeleb dressel australianos kyle chalmers cameron mcevoy intentaron éxito aproximarse territorio inhumano cielo dressel bajó segundos mundiales convirtieron hito rayo esperanza peregrinos avanzaban cumbre helada habitó cieloel salvajepopovici años mundiales carecía memoria complejos sintió inferior pecho desnudo cubierta entrepierna bermuda tela luciendo multitud pecho insinuante esternón desafiado húngaro kristof milak mariposista transformado librista debió encontrar aliciente sacan salvaje ganar oro budapest mes milak nadaba izquierda empujó terreno adrenalinamilak salió francés maxime grousset mandó prueba viraje segundos popovici tocó pared posición sesenta centésimas parcial cielo regreso inaudito popovici avanzó cuchillo agua ofrecer resistencia ofrecer superficie rozamiento rotando tronco clavando manos equilibrio perfecto falta metros traspasaba umbral ritmo récord mundo constituyen mayores hazañas historia deporte señal ominosa unidos australia potencias nado libre camino juegos parís</t>
+          <t>proceso selección equipo nacional arco adaptado arrancaba febrero deportistas participantes distintas categoríasopen recurvo open compuesto vi vi temporada clasificatorio consta pruebas tirándose dobles rounds obtendremos promedio deportistas postre determinará clasificación representar federación citas internacionales temporada desafortunadamente crisis covid permitió concluir proceso selección aplazar temporalmente clasificatorios previsto celebrarse marzo fecha declaró oficialmente alarmaen resultados obtenidos deportistas participaban proceso selección suspendiera clasificatorio cabe destacar rendimiento mostrado arquero open recurvo josé manuel marín batía récord españa categoría pruebas clasificatorias celebradas andaluz alcanzaba puntos clasificatorio volviendo repetir puntuación doble prueba clasificatoria volverlo batir rounds clasificatorios prueba puntosen josé manuel único deportista cumpliría promedio mínimo referencia formar equipo nacional arco adaptado modalidad subvención completaotros deportistas promedio guillermo rodríguez open compuesto daniel martín vi adrián orjales vi cumplen momentos promedio copagoa destacar línea ascendente carmen rubio deportista open compuesto recuperarse desafortunada grave lesión sufría temporada progresión manuel sánchez reclasificación open compuestoen clasificatorios open compuesto participando jovencísimo adrián martínez duda experiencia sirviendo enormemente cara futuro experimentado fernando barredo mostrándose regular puntuaciones promedio copagoworld archery europe declaró recientemente suspenso actividad julio aplazando pruebas clasificatorias jjpp tokio previstas temporada campeonato europa arco adaptado previsto abril olbia italia copa europa arco adaptado celebrarse principio junio nove mesto república checa esfuerzos federación europea volcarán celebre temporada informaciones respectofinalmente reseñar comités olímpico paralímpico internacionales tomaron recientemente decisión aplazar jjoo jjpp celebrarán finalmente verano federaciones internacionales tomar decisión futuro calendario internacional reste temporada adaptándose restricciones marquen nivel salud públicaante enorme incertidumbre genera situación calendario previsión plantear rfeta mera especulación único conseguiría generar incertidumbre asumir caso sistemas selección puedan sufrir cambios fuere objetivo rfeta garantizar participación equipos mejores condiciones posibles pruebas referencia año</t>
         </is>
       </c>
       <c r="C27" t="n">
         <v>0</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Deportes_46.txt</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -789,11 +924,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>agosto juegos río obtenía michael phelps relevos libre decimonovena medalla oro número metales periplo triunfal comenzado atenas transcurrido pekín londres sydney años tierna bisoñez acabó quinto mariposaen brasil nadador visto planeta volvía asombrar admirar regresando infierno personal lucha permanente oculta depresión debilidad inconfesable mundo máximamente competitivo llevado par detenciones conducir efectos alcohol foto pipa agua utilizadas fumar marihuana granjeó generalizado descrédito acreedor sanciones federativas cancelación contratos publicitarios acarició tentaciones suicidassu relación sentimental iniciada nicole johnson modelo miss california naufragaba reflotaba volvía naufragar desequilibrando causa efecto mundo michael víctimas éxito daña fracaso sentía marioneta dorada marioneta personaje creado bienintencionados empujaban buscar difícil decidió quería tales extremos londres decidió parar insoportable peso oro weight of gold título documental retirado abría íntimamente canalpero piscina cuyas brillantes aguas podían volverse oscuras rescatarlo catártico dramático taumatúrgico traumático vida tomaba influencia agua voluntario redentor vía reencuentro reconciliación resurrección michael sometió tratamiento antidepresivo resolvió problemas nicole contrajo matrimonio convirtió padre paces vida estabilizaba listo río años ¡hurraen principio previsto interviniese destinaba existían hombres estrictamente rápidos expedición estadounidense michael nadado trials mundo puso rendirle homenaje batalla elección compasiva michael nadó posta ganó medallas oro mariposa estilos libre estilos plata mariposa cerró historial olímpico agotamiento producido abundancia peso reparador medallas oro plata bronce the end</t>
+          <t>caminar pandillero recomiendo policía anda tatuado voz queda eva mujer años habitante montreal populosa colonia área metropolitana san salvador gobierno nayib bukele instauró régimen excepción salvador meses habitantes montreal histórico bastión mara salvatrucha ms miedo pandilleros cambio temen policía ejército sitiado multitud comunidades paísaquí policías soldados absoluto cualquiera cae vuelto pandilla insiste eva sentada viejo sillón pequeña sala casa observa reojo puerta vigilando escuche conversación eva pide revelar nombre completo seguridad acompañan esposo madre hijos pequeños vecinas reunido contar vive lugarhasta años entrar montreal desconocido temeridad dimensionarlo vendetta ms barrio controlaba colonia terminó asesinato personas murieron quemadas microbús transporte colectivo regresaban trabajarahora calles colonia ven pandilleros atuendos holgados tatuajes rostro armas cinto ve caminando mujeres comprando pequeña tienda regresan traer hijos escuela patrullas policías soldados rostro cubierto pasean escaneando mirada transeúntes detienen hombre joven pasahace meses llevaron yerno jorge erazo años joven trabajador estudiante tercer año licenciatura administración empresas papá llamaba conductor buseta quemaron pandilleros ″ ana vecinas reunidas salalo sucede montreal único salvador meses régimen excepción mara salvatrucha estructura criminal grande país languidece medidas presidente bukele cuestionadas autoritarismo personas detenidas miles denuncias arrestos ilegales casos torturas desplazamiento forzado causado policía ejército asesinatos prisiones gobierno país centroamericano acerca objetivo vencer pandillas costa suspensión libertades derechos constitucionales violaciones derechos humanos informe amnistía internacional publicado principios junio sitio decretado bukele desembocado violaciones masivas derechos humanos detenciones arbitrarias miércoles human rights watch hrw organización salvadoreña cristosal previsto presentar informe conjunto documenta graves abusos incluyendo desapariciones forzadas torturas malos tratosentre septiembre noviembre país habló empresarios transporte colectivo líderes mercados investigadores policiales fiscal antipandillas visitó comunidades área metropolitana san salvador históricamente controladas ms analizar resultados mediano plazo régimen excepción apunta ms huesos miembros policía ejército ocupado vacío dedican denuncias cometer delitosaunque aplicar ecuación comunidades país resultado desplazamiento ms perdido fuerza medida actividades vitales extorsión control territorial capacidad reclutamiento integrantes vinieron policías soldados capturaron mundo vinieron camiones quisieran dejar llevaron pandilleros llevaron montón gente inocente continúa evasegún lugareños consultados reportaje montreal sufrido éxodo pandilleros huyeron autoridad habitantes vínculos pandillas huir país policía amenazara encarcelarlos colaboraban ofrecían informacióny miedo desaparecido montreal comunidades visitadas periódico vecinos siguen obedeciendo normas establecidas pandillas recibir visitas familiares vengan zonas pandilla contraria hablar policías soplón vea ahorita pandilla ojos oídos lados salir cárcel explica anael marzo bukele emprendió embestida grande gobierno lanzado pandillas ms barrio medida práctica significado sistemática violación derechos humanos organizaciones humanitarias impuesta estructuras criminales masacraran personas semana supuestamente consecuencia ruptura pacto secreto gobierno mantenía investigaciones periodísticas ejecutivo niega secretoaquella matanza significó golpe administración bukele jactaba mundo control pandillas gobierno salvadoreño logrado organismos nacionales internacionales comité tortura onu señalado graves violaciones derechos humanos régimen excepción bukele gabinete desechan argumentando país eventos públicos masivos reciente concierto bad bunny medida despliegue policías militares cercar territorios ciudades país operativo empezó sábado municipio soyapango área metropolitana san salvador principios abril presidente número pandilleros ascendía encarceladoslas prácticas negociación embestida pandillas gobierno bukele salvador mandato expresidente francisco flores gobiernos dedicado reprimir negociar grupos logrado fortalecerlos expertos tema coinciden diferencia radical concentración control sistema justicia persona presidenteun pandilleros salir salir sed venganzados empresarios transporte colectivo aceptaron hablar país explicar drástica reducción cobro extorsión sector explicaron condición proteger identidad mediados década años noventa cubren rutas circulan área metropolitana san salvador pertenecen organizaciones gremiales transportistas país llevan década pagando extorsión pandillas ms barrio pago extorsión mes pague empresarios decirlo empezó régimen excepción pago prosigue coinciden meses extorsión transporte colectivo reducido calculan datos difieren expresados representante mesa nacional transporte calculó reducción agosto pasadoes mentira dejado pagar rutas pagamos dólares euros mensuales ms asegura empresarios muestra teléfono conversaciones whatsapp coordina pandillero entrega extorsión fe compañeros siguen pagando siguen pagando añadedatos mesa nacional transporte señalan transportistas pagaron millones dólares pandillas año crisis pandemia covid obligó cerrar economía país monto redujo millonesambos empresarios aseguraron transportistas dejado pagar extorsión razones principales pandillas perdido capacidad cobrarla menor control territorio pagar considerado delito empresario ruta ab acusado testaferro pandilla seguía pagando extorsión policía tomó financista víctima extorsión delito relata continúan pagando miedo pandilleros salgan prisión salir salir sed venganza afirma unoaunque ms diversificado fuentes ingresos incursionando droga lavado dinero extorsión principal fuente financiación vital práctica ms punto tratado negociaciones gobiernos país década negociaciones pandilla dejado matar extorsionarmiembros fuerza aramada salvador patrullan comubnidades reparto guadalupe campanera municipio soyapangomiembros fuerza aramada salvador patrullan comubnidades reparto guadalupe campanera municipio soyapangovíctor peñaun informe organización crisis group publicado estimó monto global extorsión salvador rondaba millones dólares año equivalente producto interno bruto pib enorme cantidad pandillas salvador siguen mafia pobresotro sectores extorsión reducida drásticamente comercio informal mercados país consultó líderes principales gremiales vendedores centro san salvador corazón comercio informal capital recorridos mercados ciudad conversaciones vendedores mayoría dejado pagar atrevo extorsión bajado comparación régimen excepción asegura líderes vendedores consultadosun estudio naciones unidas publicado junio señala vendedores ambulantes repartidores productos pagaban millones dólares concepto peaje pandillas noviembre entrevista noticiero local ministro justicia seguridad gustavo villatoro extorsión reducido nivel nacionalla bestia herida muerteun investigador policía fiscal investiga diez años negocios ms salvador aceptaron hablar principios noviembre país condición anonimato coinciden capacidad reclutamiento control territorial economía criminal pandilla punto críticola bestia herida muerte ahorita señal diga cambiar investigador policial bestia agente formas nombrar ms usada pandilleros investigador dedica años combatirla ms perdido capacidad controlar territorio reclutar miembrosahorita comiendo mierda extorsionar robar controlar negocios lavan dinero empresa formal rato ms quebrada fiscal hundimiento costando salvador profundos retrocesos libertades derechos bukele ganando guerra denuncias costa violar ley</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Politica_58.txt</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -802,11 +942,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>premio italia convirtió montaña emociones marcar drásticamente campeonato pilotos incidente max verstappen lewis hamilton ocasión diferencia sucedido silverstone quedaron eliminadoslos compases competencia destellos emociones arrancada clímax daniel ricciardo largó atacó interior verstappen arrebatarle plaza hamilton puso neerlandés ligero toque obligó salir circuito chicane permitió avance lando norris plaza dejando red bull coches casa wokingel virtual safety car apareció rápidamente consecuencia alfa romeo antonio giovinazzi cruzado golpeado posterior ferrari carlos sainz italiano ubicado primeras posiciones esperanza aspirar puntos carrera condenada finalizar ° frontal parrilla acciones valtteri bottas iniciaba remontada giro escandinavo mercedes zona puntos largado posterior cambio unidad potenciadaniel ricciardo pits giro colocando neumático duro verstappen siguiéndole vuelta posterior red bull perdió segundos detención falla pistolas cambio neumáticosal hamilton adelantó pista norris plaza líder campeonato regresó circuito mclaren británico perdido pitsa arrancar neumático duro hamilton entró colocar vuelta parada lenta segundos perder ritmo líderesal salir boxes empezó drama competencia campeón mundo extendió movimiento exterior curva arrinconar verstappen neerlandés cedió transitó chicana historia cambió neumáticos izquierdos tocó bordillos elevó monoplaza red bull desencadenar choque contendientes títuloel neumático trasero derecho rbb pasó halo mercedes finalmente posarse frontal obligar salida safety carde inmediato charles leclerc carlos sainz sergio pérez george russell valtteri bottas pilotos aprovecharon cumplir detención colocando duro excepción finlandés mercedes apostó cierrela carrera reinició giro ricciardo liderato seguido leclerc norris pérez sainz bottas británico mclaren atacó inmediato ferrari monegasco establecer casa wokingpérez desaprovechó sorpresa llevado leclerc atacó tomar posiciónsin adelantamiento mexicano vio ensombrecido salirse circuito concretar rebase recortar chicana acción considerada comisarios ilegal otorgaron sanción segundos finalbottas superó monegasco quitarle cuarto puesto enfocarse duelo directo mexicano red bull finlandés ataque giros logró mantener posición enfoque mantener mínima diferencia mexicano espera castigo segundos cruzar metanorris pidió mclaren dejarle atacar ricciardo boxes negaron posibilidad significaba equipo escuadra gp canadá australiano cruzó meta ventaja segundos norris bottas cerrando podio leclerc llevó cuarta plaza pérez finalizó quinto sanción aplicada justo ferrari sainz</t>
+          <t>posibilidad corregir genes defectuosos técnica sencilla predecesoras convertido hito científico opinión revista science tecnología denominada crispr utilizada éxito laboratorio ratones adultos patología genética logra resultados esperanzadoresla publicación eligió crispr hallazgo importante año termina recoge número investigaciones independientes idéntico resultado cortapega genético logrado mejorar atrofia muscular ratones afectados distrofia duchennela distrofia duchenne enfermedad degenerativa afecta varones nacidos vivos causa rápido deterioro sufren pacientes media suelen verse postrados silla ruedas años vida defecto gen codifica proteína esencial funcionamiento músculosesa proteína distrofina codificada gen compuesto regiones exones piezas puzle funciona cadena producción distrofina pone marcha gen cromosoma distrofia duchenne afecta varones doble copia mujeres garantiza cromosoma disponen copia intacta gen distrofinahasta llevado cabo intentos reparar gen distintos métodos terapia génica publica revista science ratones esperanzadoresutilizando virus adenoasociado taxi herramientas corte genético gen defectuoso animales equipos científicos logrado resultados similareslos investigadores universidades duke harvard texas eeuu lograron eliminar exones defectuosos ratones distrofia concretamente necesidad sustituirlo copia corregida simplemente borrado pieza defectuosa lograr producción distrofina animales versión reducida funcional gen recuperaron parcialmente función muscularen opinión lluis montoliu centro nacional biotecnología trabajos interesantes abren puerta futuras aplicaciones clínicas pacientescomo explica diario experimentos similares células realizados vivo novedad relevancia aclara pasocomo aclara virus adenoasociados sirve vehículo transporte vector tijeras genéticas exon mutado local inyección pata sistémica viajen organismohasta técnica crispr funciona especie cortapega genético reemplazar regiones genéticas mutadas probado únicamente líneas celulares éxito animales vivos adultos cuya enfermedad genética causado daños muscularesen trabajos dirigido christopher nelson universidad duke inyectaron pata abdomen virus adenoasociados lograr llegar exon borrarlo relatan artículo inyecciones locales lograron restaurar nivel distrofina mejoría músculos pata animal caso inyección abdomen pruebas posteriores mostraron mejoría músculos cardiaco pulmonar estructuras ven afectadas falta producción distrofina relacionadas mortalidad prematura lso afectados duchenneen caso chengzu long universidad texas southwestern emplearon virus patógeno humano adenovirus denominado aav llegar herramientas crispr exon caso probaron óvulos espermatozoides lograron ratones libres mutación casos posteriormente repitieron prueba grupo ratones duchenne nacer ocasión inyección genética aplicada directamente músculos logró mejorías significativas animales persistieron meses terapiaa resultados tercer idénticamente positivos autores cautos traducción hallazgos humanos posibilidad crispr corregir defectos embriones humanos generado enorme controversia ética recientemente explica charles gersbach coautor estudio declaraciones transmitidas universidad aplicación tejidos adultos afectada debate estudios demuestran posibilidad queda reconoce</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Salud_15.txt</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -815,11 +960,16 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>hugo gonzález semifinal espaldanatación terminator titmus vence ledecky libera ira entrenadormichael phelps nado díasahmed hafnaoui tunecino años orgullo áfrica piscinaaustralia valquirias logran récord tokiode octavo cuarto metros hugo gonzález progresión espectacular arañar olímpica espalda prueba estrella estilos campeón europeo mayo contacto accedió séptimo semifinalistas llevará calle importante amortiguar presión mallorquín años rostro futuro natación española otoño mireia belmontela semifinal exigente dada calidad rivales rusos bandera olímpica klement kolesnikov yevgueni rylov contrario finales suele beneficioso obtener clasificación dadas referencias ofrecen sucedió mireia semifinales directas estilos riesgo desfondarse inicio impresión ofreció hugo gonzález verse paso reservas demuestra nadó cálculo síntoma madurez competitivael español necesitaba acercarse europeo budapest subirse peldaño podio tokio centésimas semifinales contrario sucede aquatic center nadado rápido tardes mañanas finales sucedió ganador semifinal gonzález favoritos kolesnikov pasó series irá seguro rápidohugo gonzález hijo padre español madre brasileña salto río compitió joven semifinales prueba administrar participación espalda series estilos aspira claridad medalla tratarse prueba abierta marcha nadadores michael phelps ryan lochte dejado estilos abiertos alternativas vimos oro chase kalisz acompañó marca mediocre</t>
+          <t>pasa desapercibido frente problemas salud vih importante amenaza salud pública europa demuestra informe elaborado conjunto centro europeo prevención control enfermedades ecdc oficina europea organización mundial salud omsla fotografía arroja informe cambia función continente aumentando número personas viven vih diagnosticar restringe foco unión europea situación esperanzadoraa pasa desapercibido frente problemas salud vih importante amenaza salud pública europa demuestra informe elaborado conjunto centro europeo prevención control enfermedades ecdc oficina europea organización mundial salud omsla fotografía arroja informe cambia función continente aumentando número personas viven vih diagnosticar restringe foco unión europea situación esperanzadoraen cambio fronteras ue tendencia global invierte muestran datos década diagnósticos ligeramente frecuentes infecciones significa cantidad personas vive vih saberlo disminuido años estima personas vih ue diagnosticarsi realizan test forma regular personas riesgo generarse periodo infección diagnóstico beneficia persona posibilidades desarrollar enfermedad grave muerte diagnostica salud pública personas seropositivas transmitir vih parejas sexuales saberlo subrayado ammonen informe indica mitad diagnósticos vih realizados recuento células cd menor células milímetro cúbico sangre diagnóstico indica llevaban años conviviendo infecciónhay necesidad crucial aumentar testeo detección señala informe reclama estrategias mejorar diagnóstico concienciar población necesidad someterse pruebasen vías transmisión datos informe relaciones hombres mantienen sexo hombres vía común transmisión unión europea transmisión heterosexual drogas inyectables frecuente regióndurante décadas diagnosticado millones casos región europea oms unión europeaen años transmisión heterosexual disminuido considerablemente unión europea occidente años especialmente mujeres número casos debidos relaciones sexuales hombres determinados países ue occidente transmisión drogas inyectables disminuido constantemente alta europa</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Salud_10.txt</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -828,11 +978,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>neerlandés disfrutó cerrar batalla campeonaot anticipada dominio mitad temporada permitió corona pilotos premio japónesto contrasta título infarto abu dhabi terminó circunstancias controvertidas manejo fia reinicio coche seguridad carreraverstappen forma terminó lucha título lewis hamilton podía frente tensión duelo apretado tiempoen declaraciones the guardian puedes drama año seguro saludable equipo equipospero medida prepara calendario carreras verstappen consciente estrés tensiones pilotos posibilidades aumentarcuando preguntó preparado vuelta esquina verstappen preocupación complicaciones desafío necesitaba preparado mayores dificultadessi preparado dejarlo ¿no quiero corredores amamos carreraspor bonito temporada año bonito temporada año duro años año año pasadopero ocurre realmente fórmula debería bienel rival cercano verstappen charles leclerc coincidió opción preparado temporadas intensas avecinancreo preparados temporadas largas espero apretada lucha preparado carreras lucha larga esperoaunque red bull dominado año superado desventaja peso rb verstappen cree diferencia oposición mantenga gente entendiendo coches equipos acercaránsabemos invierno seguir empujando seguir tratando encontrar rendimiento rendimiento entender posiblemente neumáticos neumáticos cambiar año gestionar</t>
+          <t>hablado consumo alcohol vinculación cáncer estudio viene constatar relación concretando riesgo ingesta bebe embarazo probabilidad cáncer mama aumenta comparación mujeres optan bebidas alcohólicasel estudio cuyos datos publicado revista journal of the national cancer institute establecido vínculo ingesta alcohol cáncer mama riesgo problema enfermedad benigna mama independientemente consumo alcohólico realice gestaciónestudios previos demostrado alcohol consumido año afecta riesgo cáncer mama mujer datos relación ingesta bebidas alcohólicas periodo menstruación mujer embarazo enfermedad tejido mamario particularmente susceptible agentes carcinógenos espacio temporalying liu escuela medicina universidad washington st louis unidos colegas analizaron datos enfermeras edades años historia médica reproductiva estilo vida gracias cuestionarios estudio salud enfermeras ii nhsiise obtuvieron datos consumo alcohol periodos edad preguntando participantes número bebidas alcohólicas consumían edades años excluir mujeres cumplían criterios estudio predeterminados incluyó análisis mujeres embarazo términoentre mujeres seleccionadas investigación registraron casos cáncer mama casos bbd periodo estudio confirmados médicos revisaron información historias clínicas pacienteel consumo alcohol mujer embarazo asoció riesgo cáncer mama bbd proliferativa independientemente bebida hubera tomado embarazo datos indicaron relación dependiente dosis significa alcohol toma mujer probabilidad desarrollar cáncer mama tomar gramos alcohol vinculó aumento riesgo cáncer mujeres tomaron gramos diarios alcohol unidades vaso vino riesgo investigadores informan beber alcohol embarazo asoció riesgo cáncer mama bbd constató retrasar maternidad hijos vincula probabilidad alta desarrollar tumorla consistencia patrones asociación alcohol riesgo bbd proliferativa cáncer mama apoya hipótesis ingesta alcohol especialmente embarazo probable tejido mama etapa vulnerable jugar papel importante etiología cáncer mama concluyen investigadores</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Salud_27.txt</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -841,11 +996,16 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>preguntas grupo parlamentario socialista sesión control gobierno miércoles pedir explicaciones escándalos corrupción afectan pp protagonismo ministros rafael catalá juan ignacio zoido caso lezo iniciará ofensiva portavoz antonio hernando quen preguntará presidente gobierno piensa recuperar confianza ciudadanos sucesión casos corrupción afectan pp ministro catalá protagonismo preguntas portavoz adjunta isabel rodríguez abordará gobierno pensado maniobras fiscalía obstaculizar determinadas causas judiciales corrupción denuncias fiscales presiones jefe anticorrupción manuel moix caso lezo diputado rafael simancas exigirá explique vínculos implicados operación lezo intercambió mensajes sms ignacio gonzález operación lezo diputado felipe sicilia preguntará ministro interior juan ignacio zoido secretario seguridad justificado suficientemente reunión hermano ignacio gonzález comparecencia número interior arremetió prensa oposición cuestionar actuaciónotras preguntas dirigirán ministro hacienda portavoz economía pedro saura preguntará cristobal montoro pensando amnistía fiscal beneficiosa lucha corrupción sabido implicados operación lezo apuntado amnistía fiscal diputada soraya rodríguez reclamará valoración revelaciones relacionadas actuaciones irregulares rodrigo rato interpelación urgente ministro justicia ofensiva corrupción afecta pp grupo socialista presentará sesión control interpelación urgente ministro justicia responsabilidades políticas piensa asumir consecuencia maniobras producido seno ministerio fiscal dirigidas obstaculizar determinadas causas judiciales corrupción actuaciones ministro relación causasesta interpelación dará paso pleno mayo moción grupo socialista reclamará reprobación destitución ministro justicia fiscal fiscal anticorrupción</t>
+          <t>adiós eurobasket tropiezo mondelo equipo valencia medallas seguidas colgadas cuello pelear acabar mejores premundial australia año derrota bielorrusia pagado cara serbia cuartos rival querían enfrentar reconocía laia palau octava seleccióntodo distinto baloncesto cristina ouviña tiros libres falta segundos españa falló partido prórroga extra serbia anderson carrera vasic entonada jovanovic matando partido españa negada canasta minutos tiros libres ouviñala base anotó puntos españa partido inauguró marcador triple únicos lanzamientos puntos ndour españa metió descanso muñeca serbia llevado partido terreno puntos contacto marina maljkovic escatimó salida centímetros atragantaron selección costaba balones llegaran ndour pintura hispanosenegalesa ouviña anotaron tantos españa asaltopero hija boza guardaba as manga desparpajo anderson metió problemas faltas selección abrir cerrar ojos maite cazorla cometió minuto tiro libre serbia puso españa metido lleno trampa serbia rival afortunadamente tiro larga distancia descanso tierra tiradores puntería mitadraquel carrera despejó dudas ataque defensa robo culminó contraataque canasta aro puso selección min españa parecía comenzar carburar motor apagó minutos anotar serbia aprovechó reducir distancia astou arregló entuerto descansoen tercer cuarto serbia disfrutó ritmo jovanovic alero empató partido encestó triple equipo colocó españa vivía dejado contagiar caos rival salvó papeleta tiros libres ouviña cuarto jugarla selección dominaba rebote cometido demasiados errores pérdidas fallos tiro españa gozó renta puntos minutos acciones seguidas anderson acabaron ventaja serbia llevaba falta puso segundos bola españa ouviña tiros libres entró españa historia eurobasket</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Deportes_34.txt</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -854,11 +1014,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>vicepresidenta congreso diputados celia villalobos cargado diario mundo publicar portada foto móvil alfredo pérez rubalcaba cuya pantalla leerse mensaje privado referente eventual futuro alberto ruizgallardónen programa radio nacional villalobos afirmado cosa presentable periódico refleja dedos señor pérez rubalcaba móvil mensaje privado llega serestá hagan foto rubalcaba actitud móvil absolutamente privado mensaje privado posiblemente brete respetarlo agregado ministra sanidad aznarvillalobos supervisando fotógrafos foto barbanchovillalobos supervisando fotógrafos foto barbanchovillalobos equiparado violación privacidad reporteros gráficos fotografiar papeles anotaciones realizadas mariano rajoy responder portavoces grupos intervinieron congreso cámara respetar intimidad personasla portavoz popular soraya sáenz santamaría dirigió fotógrafos entender tomando imágenes papeles rajoy villalobos pidió reporteros gráficos mostraran material capturado accedieron pese obligados tratarse espacio público imagen villalobos comprobando cámaras reporteros publicada mundo edición diciembrele diciendo fotógrafos favor saquéis cámara pedazo teleobjetivos papel escrito mano señor rajoy respetar concluido vicepresidenta cámaraa pregunta juan ramón lucas equipararse frases cazadas micrófonos indiscretos villalobos respondido hombre oculta mujer muerta mujeres equivocar añadido mujer twitter facebook periodista masculino ingenioso dedica artículos tivalenciano defiende privacidad rubalcabapor secretaria política internacional cooperación psoe elena valenciano defendido privacidad móvil rubalcaba debería consentir hagan fotos leer perfectamente mensaje textoen declaraciones telemadrid valenciano referido foto publicada mundo aparece móvil ministro interior mensaje texto leer informadora ayto madrid gallardón defensavalenciano señalado problema haga foto móvil privado publique página periódico mensaje privadosobre persona informa rubalcaba mensaje futuro político alcalde madrid valenciano idea apuntado alguien psoe pp periodista definitiva gente caso relevante valenciano rubalcaba informan buscado información</t>
+          <t>falta global presupuestos catalunya govern dando muestras querer encarrilarlo psc comú podem relegar junts entente anuncios realizados línea acuerdos adelantados líder comunes jéssica albiach jueves atadas medidas socioeconómicas cargo cuentas suman mesa tercer sector revalorizar índice renta suficiencia catalunya irscentre medidas concretadas formación morada albiach resaltado rne govern comprometería extender bonificación transporte público catalunya año requiere implicación gobierno central puesto medida vigente diciembre cofinanciada generalitat gobierno central anunció octubre presentó anteproyecto presupuestos generales ampliará bonificación españa coste millones euros anuncio albiach adecuar previsión ejecutivo pedro sánchez territorio catalánla bonificación vigente expira diciembre gobierno anunció intención extenderla caso catalunya extensión bonificación transporte público año coste aproximado millones euros sufragada generalitat autoridad transporte metropolitano atmel president govern pere aragonès reúne palau jefe oposición salvador illapero albiach explicado conseguido compromiso ejecutivo erc extender gratuidad transporte público comunidad catalana menores años medida implantada usuarios barcelona título transporte coste millones euros ampliación territorio catalán supondría millón euros tercer comunes anunciado govern ampliará rango usuarios título tjove años costaría millones euroslos comunes acordado govern extender catalunya gratuidad transporte jóvenes años extender tjove añoslos comunes aseguran compromisos cerrados marco negociaciones aprobar presupuestos señalan ámbito movilidad debería margen incluir medidas incluir beneficiarios gratuidad transporte discapacitados colectivo menor catalunya cuyo coste rondaría millones euros calculan advierten queda acordar govern cerrado presupuestos remarcan carpeta sanidad clave definitivo cuentasjordi turull albert batet reunión jxcat bruselasademás medidas deberán contar visto psc potencial socio govern viene mostrando afinidad negociar junts elevara precio apoyo propuesta fiscal alejada voluntad ejecutivo pere aragonès principio debería problema socialistas dieran beneplácito puesto sujetas concurso gobierno centralen caso salvador illa ven presionados prisas govern cerrar presupuestos semana socialistas comunes ven inviable formaciones ven margen zanjar pacto permita aragonès aprobar anteproyecto ley consell executiu principios semana viene</t>
         </is>
       </c>
       <c r="C33" t="n">
         <v>2</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Politica_20.txt</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -867,11 +1032,16 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ministerio sanidad política social decidido destituir secretaria plan nacional sida teresa robledo cuyo nombramiento produjo año organizaciones conocido noticia medios comunicación manifiestan sorpresa decisiónfuentes departamento dirige trinidad jiménez explicado agencia efe robledo seguirá trabajando ministerio puesto funcionaria funcionesla noticia recibida sorpresa principales organizaciones dedicadas atención pacientes vih reconocido haberse enterado destitución medios comunicaciónno sabíamos reconoce elmundoes santiago pérez avilés presidente cesida noticia impacto colectivo esperaba reconoce juanse fernández portavoz grupo tratamientos vih gttambos coinciden decisión llega diciembre mundial vih importantes reuniones ong plan nacional comunidades autónomas explica pérez aviléspara representante gtt principales preocupaciones secretaria plan permanezca descabezada nombre sustituto robledo tema peliagudo años baile personas estabilidad costó encontrar persona adecuada reconoce fernándezel nombramiento teresa robledo produjo enero ministra sanidad elena salgado sustitución maría val díez plan cabeza añaden gttcuriosamente utilizan palabra dialogante valorar robledo frente plan muestran satisfechos llevado cabo codo codo organizaciones colectivos vih entendemos sanidad comunicado oficialmente motivos apunta presidente cesidasu perfildesde robledo licenciada medicina cirugía universidad complutense madrid trabajado ministerio sanidad desempeñado carrera profesional diversos puestos relacionados ámbito salud públicadesde nombramiento responsable área prevención subdirección promoción salud epidemiología dirección salud públicarobledo miembro grupo promoción salud sociedad española medicina familia comunitaria semfyc comité español interdisciplinario prevención cardiovascularrobledo inaugurado octubre ix jornadas estatales vihsida organizadas cruz roja española infecciones vih registran españa relaciones sexuales protegidas carácter heterosexual homosexual bisexual</t>
+          <t>líder partido populista austriaco fpö protagonista llamado ibizagate heinzchristian strache vuelve política partido nombre responde tradición formación vicepresidente austria strache obligado marcharse fpö escándalo provocado vídeo indicios corruptelas anunció viena regreso vida pública movimiento equipo hc strache alianza austria formación pretende concurrir elecciones regionales viena mes octubreel equipo hc strache asume ideario principios políticos fpö modeló notable éxito centrará fortalecimiento intereses regionales nacionales austria venos contrapeso globalización mundo control alternativa progresivo desarraigo sociedad política incapaz defender intereses respuesta preocupaciones presentación proyectola caída strache produjo año raíz difusión vídeo negociaba contratos sugería líneas financiación ilegal partido supuesta oligarca rusa imágenes tomaron mayo ibiza isla pasa años vacaciones escándalo supuso grabación abrió fractura coalición gobierno populares övp líder canciller sebastian kurz puso cortafuego escándalo perder cuestión confianza votos fpö austria manos equipo tecnócratas celebración elecciones kurz ganó legislatura eligió socio gobierno verdesstrache anunció retirada política octubre año intentos volver intermitentes previo formación movimiento strache fundó partido alianza austria daö grupo políticos disidentes fpö formación puerto añada siglas sello personallas circunstancias distintas pandemia coronavirus servir abono populismo comparecencia prensa strache apelado precisamente miedo votantes perder riesgo caer pobreza decisión gobierno cerrar fronteras correcta decisión reiniciar actividad económica llegado apoyos previstos afectados insuficientes subrayóstrache concurrirá partido madre línea pasos dados líder histórico populismo derechas austríaco fallecido jörg heider fundador fpö heider llevó fpö gobierno intrigas internas partido provocaron salida fundó alianza futuro austria bzöel anuncio regreso strache política provocado tipo reacciones incluida burla especialmente nombre elegido movimiento aspira posicionarse política nacional equipo strache recuerda equipo stronach tuiteó periodista orf armin wolf aludiendo proyecto político corta duración magnate negocios frank stronach austria strache nuevamente pletórico periodista julia ortner fascinante</t>
         </is>
       </c>
       <c r="C34" t="n">
         <v>2</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Politica_54.txt</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -880,11 +1050,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>conseller sanidad salud pública miguel mínguez asegurado martes hospital castellón colapso denunciaron lunes representantes trabajadores concentraron señal protesta centro sanitario referencia provinciatampoco comunidad valenciana reúnan circunstancias convocatoria huelga sanidad comunidad madridesta postura titular sanidad valenciano comparecencia sede consell castellón presentar presupuesto histórico departamentola visita mínguez producido justo trabajadores sanitarios sindicatos puesto grito cielo consideran discriminación reparto plazas hospital resto centros sanitarios valencianos departamentos salud quejas ve argumentadas consellerla conselleria disciminación recursos humanos infraerstructuras proporcionales responsable sanidad destaca esfuerzo efectuado personal plazas mayo provincia castellón mínguez puntualiza plazas médicos hospital adjudicaron médicosconcentraciones huelgapreguntado quejas sindicatos colapso mínguez alega instalen equipos dotarán personal deja puerta abierta hablar equipos directivos yen exista disminución personal solucionará diálogo gerencias coordinadores departamentos actualizar necesidades infraestruturas recursos humanos dichoel malestar profesionales abre posibilidad convoque huelga mínguez contempla comunidad valenciana actual reúne circunstancias comunidades exista convocatoria huelganosotros cerradas urgencias extrahospitalarias madrid comunidad valenciana único ampliar plazas abrir puestos atención continuada rebajar ratios atención primaria sip facultativo enfermería pediatríatenemos mejores ratios españarespecto inversión sanitaria castellón cuentas consell conseller destacó provincia castellón contará millones euros destinados mejora infraestructuras sanitariasparalelamente comparecencia realizada centro castellón trabajadores urgencias hospital concentraban puertas servicio denunciar precaridad falta personal atender pacientes sanitarios mostraban cartel reclamaron ¡urgencias dignas espera media sitúa ó</t>
+          <t>año vuelto demostrar oncología española envidiar países entorno mirar ojos estadounidense congreso cáncer mundo celebrado semana chicago resumir participación española pieza imposible abundante individual cooperación grupos internacionalesla sesión plenaria recoge estudios importantes presentados congreso contó participación española estudio estadounidense evaluó positivamente beneficio añadir bevacizumab quimioterapia aumentar supervivencia global cáncer cuello útero avanzado españa único país europeo aportó pacientes estudio estadounidense cambia práctica clínica entrada estudio envergadura pone relieve duda alta calidad investigación clínica española subrayó principal investigadora nacional oncóloga hospital vall dhebron ana oakninmás allá hall fama asco presencia española fructífera variada grupo español investigación cáncer mama geicam presentado trabajos conclusiones interesantes explica elmundoes miguel martín coordinador trabajos concluido sobrepeso extremo factor pronóstico cáncer mama efecto tratamiento apunta oncólogo mujeres obesas diagnosticadas enfermedad priorizar perder peso rápido posibleotro geicam basado multitudinario proyecto álamo analiza pacientes cáncer mama concluye afectadas enfermedad pariente grado sufrido datos conocían apunta martínla conjunción investigación básica clínica cabo españa protagonismo chicago mano director programa investigación traslacional centro nacional investigaciones oncológicas cnio manuel hidalgo investigadora equipo elena garralda presentado estudio pacientes secuenciado completamente exoma genes decidir tratamientos funcionar acorde mutaciones observadas acotadas posibles terapias utilizaron llamados ratones avatar introducen muestras tumor humano probar fármacos pacientes reduciendo posibilidades fracaso toxicidades pacientes españoles hospital madrid conseguido supervivencias importantes tipo tumores hablando resume hidalgo periódico descanso congreso participantes benefició ratones dispuestos probar fármaco enviado publicación revista alto impactorafael rosell espada oncología española desplazado chicago experto cáncer pulmón presentado diversos estudios quimioterapia seleccionada mutaciones tumor vía eficaz aumentar supervivencia cánceres letales comunicación oral presentada congreso oncólogo catalán demostrado pacientes hora empezar tratamiento responden independencia estadio tumor trabajos grupo investigación cáncer pulmón logrado aumentar supervivencia meses grupo enfermospor colaboración cancer therapeutics innovation group ctig rosell caído bondades secuenciación genómica completa hallazgos positivos demuestran reajusta tumor poquísimo inicio tratamiento personalizado desvelar alteraciones genómicas conocidas mutación egfr</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Salud_37.txt</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -893,11 +1068,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>falta global presupuestos catalunya govern dando muestras querer encarrilarlo psc comú podem relegar junts entente anuncios realizados línea acuerdos adelantados líder comunes jéssica albiach jueves atadas medidas socioeconómicas cargo cuentas suman mesa tercer sector revalorizar índice renta suficiencia catalunya irscentre medidas concretadas formación morada albiach resaltado rne govern comprometería extender bonificación transporte público catalunya año requiere implicación gobierno central puesto medida vigente diciembre cofinanciada generalitat gobierno central anunció octubre presentó anteproyecto presupuestos generales ampliará bonificación españa coste millones euros anuncio albiach adecuar previsión ejecutivo pedro sánchez territorio catalánla bonificación vigente expira diciembre gobierno anunció intención extenderla caso catalunya extensión bonificación transporte público año coste aproximado millones euros sufragada generalitat autoridad transporte metropolitano atmel president govern pere aragonès reúne palau jefe oposición salvador illapero albiach explicado conseguido compromiso ejecutivo erc extender gratuidad transporte público comunidad catalana menores años medida implantada usuarios barcelona título transporte coste millones euros ampliación territorio catalán supondría millón euros tercer comunes anunciado govern ampliará rango usuarios título tjove años costaría millones euroslos comunes acordado govern extender catalunya gratuidad transporte jóvenes años extender tjove añoslos comunes aseguran compromisos cerrados marco negociaciones aprobar presupuestos señalan ámbito movilidad debería margen incluir medidas incluir beneficiarios gratuidad transporte discapacitados colectivo menor catalunya cuyo coste rondaría millones euros calculan advierten queda acordar govern cerrado presupuestos remarcan carpeta sanidad clave definitivo cuentasjordi turull albert batet reunión jxcat bruselasademás medidas deberán contar visto psc potencial socio govern viene mostrando afinidad negociar junts elevara precio apoyo propuesta fiscal alejada voluntad ejecutivo pere aragonès principio debería problema socialistas dieran beneplácito puesto sujetas concurso gobierno centralen caso salvador illa ven presionados prisas govern cerrar presupuestos semana socialistas comunes ven inviable formaciones ven margen zanjar pacto permita aragonès aprobar anteproyecto ley consell executiu principios semana viene</t>
+          <t>política española tablero juego mesa estrategia movimiento inocente importante composición mesa congreso presidente cámara baja compuesta presidente vicepresidentes secretarios cargo importante legislatura recaído diputado grupo sustenta gobierno albert rivera oposición pp ocupe cargo recaiga oposición ciudadanos suma petición psoeel presidente ciudadanos reunión mantuvo moncloa mariano rajoy salió satisfecho entorno mostró favorable presida gobierno presida cortes equilibrio expuso circunstancia sana razonable conversaciones rivera mantenido rajoy sánchez acordaron partidos comiencen negociaciones constitución mesa caso ciudadanos personas designadas josé manuel villegas vicesecretario jefe gabinete rivera miguel gutiérrez delegado formación madrid diputado circunscripciónciudadanos suma psoe petición presidente congreso persona forme partido lidere ejecutivo transmitió pedro sánchez rajoy reunión mantuvieron semana moncloa líder socialista barrió casa razonable presidiera congreso fuerza política rivera explícito fuentes dirección aseguraron planteen objeto buscar máxima pluralidad ocurrido reflejo situación actual dialogaren ciudadanos consideran cambio color sillón presidencia congreso importante evitar paralización rechazo reformas partido prioritarias pacto educación ley electoral reforma administración pública supresión diputaciones financiación autonómicasegún reglamento congreso mesa corresponde gobierno interior organización parlamentario calificación escritos parlamentarios decisión admisibilidad tramitaciónen mente ciudadanos reproducir sucedido murcia gobierna pp psoe preside asamblea regional gracias socialistas ciudadanosla formación mesa muesca intuir futuros movimientos cara alianzas formar gobierno pp descarta opción partido presida cámara baja gesto políticotambién suceder alianza formaciones izquierda otorgara presidencia congreso psoe gobernar sillones existiría opción revocar nombramiento cámara baja evitar partido mandara ejecutivo</t>
         </is>
       </c>
       <c r="C36" t="n">
         <v>2</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Politica_24.txt</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -906,11 +1086,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>junts per catalunya entregado miércoles govern generalitat reunión presupuestos documento demandas negociar cuentas generalitat anunciaron semanas bases negociación presupuesto propuesta seria rigurosa pensada sesgo ideológico necesidades país apuntado secretario formación jordi turull atención medios insistimos fiscalidad justa añadido líder jxcatla formación articulado propuesta ejes –desarrollo económico derechos cohesión social equidad seguridad catalán lengua cultura medios comunicación equilibrio territorial soberanía nacional– medidas destacadas ámbito fiscalidad educación seguridad medidas paliar inflación fiscalidadasí junts aboga deflactar irpf tramos paliar efectos inflación desbocada revisar reducir impuesto sucesiones forma progresiva vuelva niveles bonificación adquisiciones debidas muerte familiar grado padres hermanos hijossi deflacta irpf aumento fiscal encubierto ingresos adicionales administraciones inflación acabará año subidas salariales llegarán nivel contabilizamos subida media piden media organizaciones sindicales puedes saltar tramo deflacta perder adquisitivo apuntan fuentes jxcatninguna medida élites conjunto familias paísjunts apuesta bajar irpf tramo rentas bajas tributen catalunya territorios incrementar mínimos personales familiares irpf inflación medida protección fiscal sucesión empresas familiares permitir continuidad llegando bonificar toca mínimo exento personal familiar acabas pagando impuestos comunidades previsto añaden fuentes consultadasal incluye propuesta fiscal modificación impuesto patrimonio barajado posibilidad subir mínimo exento niveles euros actuales personas lleguen extranjero pagar patrimonio acumulado llegar catalunya compromiso permanencia adquisición vivienda circunstancias similares formación facilitar descartado punto afecta ciudadanos pedimos luna aseguran junts medida élites conjunto familias país sostienen formaciónescuela concertada actualización módulosotras propuestas destacadas ámbito educación jxcat pide actualizar incrementar precio módulos escuela concertada revertir presupuestariamente infrafinanciación escuela concertada perjuicio escuela pública pública preparada quite escuela concertada favor mejorar escuela pública fraguando problema concertada prejuicios ideológicos lamentan posconvergentes incluyen garantizar universalidad gratuidad concertación plazas seguridad ocupaciones delincuencialesen materia seguridad formación reclama crear unidad mossos desquadra especializada ocupaciones delincuenciales materia partido viene insistiendo semanas extitulares justícia drets socials lourdes ciuró violant cervera impulsado cambios código civil catalán vecinos administraciones locales pudieran denunciar casos propietarios casos tenedores actúan sanidaden materia sanidad apuesta incremento presupuestario millones euros años destinar presupuesto sanidad reforzar atención primaria incrementar partidas destinadas salud mental avanzar agència integrada social sanitària previsto exconseller josep maria argimon exconsellera cervera asimismo pide compromiso avanzar dilaciones proyecto hard rock aprobar plan desarrollo urbanístico acabe año previsto ejecuten inversiones necesarias creación incaoli institut català loli completar despliegue fibra óptica territorio catalán propuesta seria rigurosa pensada sesgo ideológico necesidades jordi turullsecretario junts per catalunyaen apartado reclama departamentos govern trabaje mentalidad trabaje reducir dependencia figura propuesta incremento millones euros fomento impulso catalánno líneas rojas aceptan medidas advierten junts asegura jugarán dilatar tiempos negociación govern pere aragonès acelerado negociación grupos reunió psc perfila socio probable ritmo espera ejecutivo catalán comunes peso parlament reunido ocasiones govern apoyo concurso socialistas posconvergentes insuficiente</t>
+          <t>martín puente vigo junio número gallego carlos alcaraz cerrarán cima ranking mundial martín alcanzó dobles tenis silla común compañero amigo charly crack compartimos momentos us open taquillas sonrisa hicimos amistad volvimos coincidir recepción majestad felipe vi confiesa as deportista paralímpico año tachado sueños listaroland garros grand slam puertas dani caverzaschi aperitivo atracón triunfos ganó dobles us open francés nicolas peifer septiembre masters argentino gustavo fernández noviembre número dobles nivel individual coloca séptimo reto año ayudado confiar creer duda temporada servirá empujón próxima explica tenista desempolvar recuerdos roland garros torneo conduciendo car sant cugat vallés quería estrenar carné lució coche competición salió pedir boca semana flipé niño parque atracciones lados crecermartín lidiar presión privilegio jugando gloria alcance manejar presión abstraerse necesaria explorar límites argumenta deportista salvar numerosos obstáculos niño quería jugar celta admira aspas síndrome proteus cambió planes enfermedad rara provoca crecimiento óseo anormal terminó amputación pie izquierdo años levantar sábana shock pasar quirófano añosfue hermano antón estudia universidad sacramento california beca tenis descubrió tenis silla flechazo enamorando íbamos jugar club hermano hermana hacía pie frontón problemas físicos aumento primeras silla impresión esperaba semejante armatoste llamé transatlántico ruedas tenis silla ayudó olvidar operaciones noches hospital casualidad convertido vida pensé vivir juego desaparece silla mágico deporte explica niño prodigio años empezó competir conquistó título nacional número ranking mundial júnior consiguió diploma juegos río años joven modalidad tokio parís retos asoman hablar pronostica estudiante administración dirección empresaslos juegos igualdad tenis inclusión torneos atp confirma martín costado semanas asimilar año mágico quiero llegar número individual victoria llegar razónmartín puente jugó partido exhibición chile rafa nadal alejandro tabilo gustavo fernández experiencia ¡día histórico personas estadio retransmitido directo televisión nacional chile tenista paralímpicos redes año terminado fecha marcada rojo campeonato españa sevilla preparar australia comenzar fuerza</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Deportes_12.txt</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -919,11 +1104,16 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>pedro sánchez juega elecciones domingo celebran meses victoria primarias psoe autoridad partido fase construcción ¿resistiría precario liderazgo debacle histórica urnas socialistas superados cómputo global votos fuerza hegemónica izquierda incapaces recuperar feudos históricos arrebató pp extremadura castillala mancha probablemente psoe cosechó elecciones municipales celebradas años resultado historia votos sánchez siquiera soñar rozar listón irrupción fuerza ciudadanos partidos cuño existían salvando distancias elecciones generales locales autonómicas suelen primar rostros siglas barómetro centro investigaciones sociológicas cis daba psoe intención voto comicios legislativos salvar cara sáncheznecesitaría arrebatar pp extremadura castillala mancha comunidades autónomas manos socialistas única excepción estaúltima legislaturay conservar principado asturias único territorio andalucía gobierna psoe escenario –es perder asturias josé antonio monago maría dolores cospedal siguieran mando extremadura castillala mancha respectivamente–sería sinónimo cataclismo situación castillala mancha resulta especialmente endiablada cospedal sondeo cis perdería mayoría absoluta comunidad obtendría escaños socialista emiliano garcíapage lograría décimas populares intención voto ¿quién tomaría iniciativa formar gobierno comunidad cospedal investida presidenta apoyo ciudadanos escaños partido albert riverarespaldaría pp inclinaría psoe aire futuro político extremadura gobernada años pp apoyo natura iu cis otorga socialistas guillermo fernández vara horquilla escaños alejados marcan umbral mayoría absoluta psoe alcanzar cota apoyo cis lograría diputados populares quedarían puertas objetivo voto parlamentarios barómetro concede ciudadanospedro sánchez miedo quede rajoy asturias dibuja igualmente complejo mosaico apoyos cruzados determinante papel ciudadanos psoe gobierna principado volvería ganar elecciones gobernar respaldo formación lidera pablo iglesias –el presidente asturiano javier fernández ve simpatía podemos– pp hacerse ejecutivo autonómico lograra respaldo ciudadanos foro asturias partido creado exministro popular francisco álvarez cascos recientes elecciones andaluzas mérito pírrica victoria socialista susana díaz protagonizó deliberadamente campaña medida injerencias ferraz domingo miradas clavadas sánchez mérito psoe salva muebles reforzando precario liderazgo secretario partido losresultados calamitosos dudan tardarían alzarse voces reclamaran cabeza caso primarias convocadas julio contar probablemente aspirante</t>
+          <t>parlamento indonesia aprobó martes polémica reforma código penal retroceder nación sudeste asiático millones habitantes décadas derechos alcanzados materias libertades sexual religiosa expresión reforma amplia historia archipiélago mundo islas incluye artículos prohíbe sexo extramarital cohabitación parejas casadas apostasía difamación dirigentes recorte libertades promovido presidente joko widodo llega país mandatario recibieran amplio reconocimiento internacional organización cumbre celebró noviembre baliel código aplicará indonesios extranjeros aprobado apoyo partidos políticos temores legislación ahuyente turistas paradisíacas costas tropicales perjudique inversiones decenas ong grupos civiles salido calles denunciar cambios informa prensa localhan años espera declaró viceministro derecho derechos humanos edward omar sharief cámara representantes votase unanimidad favor código penal entrará vigor permitir redacten reglamentos aplicación presidente comisión parlamentaria encargada revisión texto bambang wuryanto código antiguo vestigio dominación colonial holandesa cabidaentre cláusulas morales criticadas figuran pena año prisión practicar sexo matrimonio cualquiera formas castigo meses cárcel parejas viven juntas casarse indonesia país población musulmana grande planeta tradición liberal prohíbe adulterio relaciones prematrimoniales velo hiyab obligatorio escuelasalbert aries portavoz ministerio justicia declarado denunciar padre cónyuge hijo presuntos infractores regulaciones morales objetivo proteger institución matrimonio valores indonesios protege intimidad comunidad niega terceros derecho denunciar asunto jueces nombre moralidad afirmóactivistas sostienen carteles manifestación código penal indonesia martes yakarta carteles lee rechazad reforma código penal código penal amordaza libertad prensa activistas sostienen carteles manifestación código penal indonesia martes yakarta carteles lee rechazad reforma código penal código penal amordaza libertad prensaslamet riyadi apúnete país seguir actualidad leer límitesgrupos favor derechos humanos afirman leyes afectan forma desproporcionada mujeres personas lgtbi minorías étnicas país phil robertson director adjunto asia organización proderechos humanos human rights watch denunciado twitter paso indonesia propone avanzar senda desastre violación derechos penalizar relaciones sexuales matrimonio escandalosa propuesta código penal viola normas internacionales derechos privacidad dañará gravemente paísotros cambios legales críticos socavan libertades civiles democracia planeta condena meses años rejas atentar dignidad presidente vicepresidente insultar instituciones ilegalización apostasía pena años cárcel propagar noticias falsas prohibición difundir opiniones contrarias ideología organizar protestas notificación previaen respuesta críticas vienen resonando semana ministro derecho derechos humanos yasonna laoly expuso martes legisladores fácil país multicultural multiétnico elaborar código penal acomodar interesesel gobierno indonesio llevaba décadas discutiendo revisión código penal enormes protestas anunciarse reelección joko widodo vencedor comicios presidenciales abril detuvieron aprobación norma legisladores tratado suavizar disposiciones widodo instado parlamento aprobar proyecto ley año caldee clima político cara elecciones presidenciales previstas principios martes periódicos nacionales condenado editoriales leyes diario koran tempo sostiene código tintes autoritarios jakarta post expresa profunda preocupación futura aplicación textodesde industria turística mostrado rechazo ley llega economía turismo empieza recuperarse pandemia maulana yusran subsecretario asociación turística país código totalmente contraproducente lamenta gobierno cerrado ojos cita reuters estallido crisis sanitaria indonesia especialmente isla bali intentado atraer nómadas digitales establezcan costas ofreciendo visado flexible espera alcancen niveles turismo anteriores pandemia millones visitantes bali</t>
         </is>
       </c>
       <c r="C38" t="n">
         <v>2</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Politica_55.txt</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -932,11 +1122,16 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>psoe mantiene intención voto pp bajaría punto mes barómetro noviembre centro investigaciones sociológicas cis público viernes sondeo concluye partido socialista socio mayoritario gobierno coalición ganaría hipotéticas elecciones generales apoyos octubre principal partido oposición liderado alberto núñez feijóo reuniría papeletas punto resultados socialistas aumentan puntos distancia populares unidas socio psoe ejecutivo lograría votos punto mes vox recupera punto ciudadanos baja levemente formación independentista erc rasca décima sondeo pregunta principal responsable ruptura delas negociaciones gobierno populares renovación consejo judicial tribunal constitucional encuestados apuntan pp frente señala psoeel campo sondeo analiza información entrevistas noviembre error muestral barómetro pp rompiera negociaciones gobierno renovar judicial años caducado límite tribunal supremo imposibilidad nombramientos funciones pregunta encuestados principal responsable naufragio conversaciones renovación órgano gobierno jueces tribunal constitucional cuya designación encallada disyuntiva señala pp responsable ruptura frente apunta psoe encuestas coincidieron anuncio presidente gobierno pedro sánchez reforma código penal suprimirá delito sedición motivo alegó partido feijóo romper negociación renovación judicial polémica política posteriorla posición pp psoe principales fuerzas políticas país mantiene línea similar barómetro tendencias voto municipales incluía estimación comicios generales calculaba distancia puntos formaciones barómetro noviembre pregunta preparación personal líderes pedro sánchez alberto núñez feijóo respuestas sitúan plano similar presidente gobierno saque ventaja líder oposición encuestados ve líder socialista preparado preparado frente dirigente popular preparado preparado mes barómetro evaluado popularidad aceptación líderes visible choque exlíder pablo iglesias ministra yolanda díaz precisamente díaz vicepresidenta líder unidas gobierno coalición política encuestados puntuación siguen presidente gobierno pedro sánchez líder pp alberto núñez feijóo líder país íñigo errejón alcanza inés arrimadas ciudadanos valorado santiago abascal principales preocupaciones ciudadanas crisis económica problema nombrado seguido paro sanidad problemas políticos ocupan cuarto ―un citan― educación sitúa quinto puesto comportamiento políticos citado pregunta encuestados problemas afectan personalmente mantienen puestos crisis económica sanidad paro educación continuación entran incertidumbres relacionadas calidad cambio climático inseguridad ciudadana</t>
+          <t>décadas figurado lista principales enemigos salud consumo demonizado apuntalado larga lista riesgos dejado crecer estrategias combatirlas grasas empezando redimidas cienciavarias investigaciones recientes señalado hora quitarles estigma dañinas constatación tipos grasa tomar aceite oliva cuyas propiedades cardiosaludables ratificadas ingerir conocidos ácidos grasos trans presentes alimentos procesados cuyos riesgos probados evidencias grasas principales culpables epidemia enfermedades cardiovascularesla relación aparentemente lógica consumo grasa alimentaria acumulación grasa corporal tambaleado señalaba diario meses josé maría ordovás director laboratorio nutrición genómica usdahuman nutrition research center on aging universidad tufts eeuu principales expertos áreacoincidía punto vista semanas dariush mozaffarian codirector programa epidemiología cardiovascular universidad harvard visita centro nacional investigaciones cardiovasculares señalaba empezó colesterol sangre único parámetro evaluar calidad dieta llevó recomendación reducir grasas dieta error dieta depende mides colesterol fotografía reducidaesta semana comentario publicado revista bmj firmado cardiólogo británico aseem malhotra une argumentario sugiriendo suprimir mantra asocia grasa saturada enfermedad cardiovascularpara malhotra historia culpable señalar dedo duda azúcar industria añade productosel miedo grasa señala cardiólogo llevó considerable reducción presencia productos procesados problema ejemplifica quitas grasa comida industria alimentaria compensó falta reemplazando grasa saturada azúcares añadidosla evidencia científica actual añade demostrando azúcar factor riesgo independiente desarrollar síndrome metabólico personas llegan hospital infarto concentraciones colesterol totalmente normales subraya malhotra seguidamente pregunta replantearse colesterol realmente problemala obsesión colesterol llevado sobremedicación millones personas comenta cardiólogo reflexiona demostrado adoptar dieta mediterránea ataque corazón efectivo tomar estatina reducir mortalidad</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Salud_18.txt</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -945,11 +1140,16 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>política española tablero juego mesa estrategia movimiento inocente importante composición mesa congreso presidente cámara baja compuesta presidente vicepresidentes secretarios cargo importante legislatura recaído diputado grupo sustenta gobierno albert rivera oposición pp ocupe cargo recaiga oposición ciudadanos suma petición psoeel presidente ciudadanos reunión mantuvo moncloa mariano rajoy salió satisfecho entorno mostró favorable presida gobierno presida cortes equilibrio expuso circunstancia sana razonable conversaciones rivera mantenido rajoy sánchez acordaron partidos comiencen negociaciones constitución mesa caso ciudadanos personas designadas josé manuel villegas vicesecretario jefe gabinete rivera miguel gutiérrez delegado formación madrid diputado circunscripciónciudadanos suma psoe petición presidente congreso persona forme partido lidere ejecutivo transmitió pedro sánchez rajoy reunión mantuvieron semana moncloa líder socialista barrió casa razonable presidiera congreso fuerza política rivera explícito fuentes dirección aseguraron planteen objeto buscar máxima pluralidad ocurrido reflejo situación actual dialogaren ciudadanos consideran cambio color sillón presidencia congreso importante evitar paralización rechazo reformas partido prioritarias pacto educación ley electoral reforma administración pública supresión diputaciones financiación autonómicasegún reglamento congreso mesa corresponde gobierno interior organización parlamentario calificación escritos parlamentarios decisión admisibilidad tramitaciónen mente ciudadanos reproducir sucedido murcia gobierna pp psoe preside asamblea regional gracias socialistas ciudadanosla formación mesa muesca intuir futuros movimientos cara alianzas formar gobierno pp descarta opción partido presida cámara baja gesto políticotambién suceder alianza formaciones izquierda otorgara presidencia congreso psoe gobernar sillones existiría opción revocar nombramiento cámara baja evitar partido mandara ejecutivo</t>
+          <t>ministerio sanidad política social decidido destituir secretaria plan nacional sida teresa robledo cuyo nombramiento produjo año organizaciones conocido noticia medios comunicación manifiestan sorpresa decisiónfuentes departamento dirige trinidad jiménez explicado agencia efe robledo seguirá trabajando ministerio puesto funcionaria funcionesla noticia recibida sorpresa principales organizaciones dedicadas atención pacientes vih reconocido haberse enterado destitución medios comunicaciónno sabíamos reconoce elmundoes santiago pérez avilés presidente cesida noticia impacto colectivo esperaba reconoce juanse fernández portavoz grupo tratamientos vih gttambos coinciden decisión llega diciembre mundial vih importantes reuniones ong plan nacional comunidades autónomas explica pérez aviléspara representante gtt principales preocupaciones secretaria plan permanezca descabezada nombre sustituto robledo tema peliagudo años baile personas estabilidad costó encontrar persona adecuada reconoce fernándezel nombramiento teresa robledo produjo enero ministra sanidad elena salgado sustitución maría val díez plan cabeza añaden gttcuriosamente utilizan palabra dialogante valorar robledo frente plan muestran satisfechos llevado cabo codo codo organizaciones colectivos vih entendemos sanidad comunicado oficialmente motivos apunta presidente cesidasu perfildesde robledo licenciada medicina cirugía universidad complutense madrid trabajado ministerio sanidad desempeñado carrera profesional diversos puestos relacionados ámbito salud públicadesde nombramiento responsable área prevención subdirección promoción salud epidemiología dirección salud públicarobledo miembro grupo promoción salud sociedad española medicina familia comunitaria semfyc comité español interdisciplinario prevención cardiovascularrobledo inaugurado octubre ix jornadas estatales vihsida organizadas cruz roja española infecciones vih registran españa relaciones sexuales protegidas carácter heterosexual homosexual bisexual</t>
         </is>
       </c>
       <c r="C40" t="n">
         <v>2</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Politica_18.txt</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -958,11 +1158,16 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>jefe ejecutivo josé maría aznar asegurado futuro país necesita coaliciones radicales estabilidad institucional levanten mañanas ejercicio voluntad propósito insultar españael presidente gobierno pp refirió situación postelectoral cataluña semanas escuchando exceso palabras verbos radicalesaznar consideraciones intervención tradicional cena navidad pp madrid celebró hotel afueras capitalademás recordó imagen secretario psoe josé luis rodríguez zapatero sonriendo complacidamente balcón palacio sant jaume jefe independentistas catalanes referencia líder erc josep luis carod roviraesa imagen verse toma posesión pasquall maragall presidente generalitat pacto socialistas recordó quieren independencia españa antipática sienten cómodos quieren marchartambién lamentó palabras maragall riesgos drama situación subrayó levanten mañanas ejercicio voluntad propósito insultar españafrente pp seguir defendiendo convivencia solidaridad futuro progreso todosno sacar radicales pongan tranquilidad moderación sosiego firmeza encontrar comportamiento partido pensando interés país añadiócenarato rajoy posan cocineros restaurante madrid cenaron efepara aznar españa necesita gritos radicales tensar cuerdas organizar drama continuidad histórica estabilidad institucional políticas reforma seguir progresocon coaliciones radicales juicio gobierna ayuntamiento comunidad autónoma españa necesita radicalismo unidad garantiza pp candidato presidencia gobierno mariano rajoyun pacto cree nadiepor rajoy acusó presidente generalitat pasqual maragall apostar modelo financiación cataluña arreglar problemas generado firmando pacto cree psoe pp avalarárajoy subrayó gana elecciones acción política centrará impulsar españa unida solidaria caben modelos económicos sociales apuesten diferencias territorios propuestas cambios constitución estatutos pactados plan ibarretxerajoy determinación lograr presidencia gobierno pidió esfuerzo dedicación militantes lograr meta gracias aznar base partido cohesionado unido proyecto españa ideas llevarlo término</t>
+          <t>usos toxina botulínica seborrea psoriasis moléculas descubiertas capaces combatir cáncer piel dermatólogos ponen hallazgos científicos candentes año congreso nacional academia española dermatología venereología celebrando valencialos destacados relacionados tumores cutáneos interés encontrar medicamentos consigan tratar pacientes efectos secundarios forma rápida abarcando extensión moléculas vismodegib imiquimod diclofenacola terapia fotodinámica ingenol mebutato confirma carlos guillén jefe dermatología instituto valenciano oncología ivo presentada congreso anual sociedad americana oncología clínica asco labrolizumab capaz respuestas claras personas melanoma metastásico suerte mayoría melanomas detectan precoces curan problema extirpaciónen información filtros solares curvas cáncer piel melanoma melanoma dejado crecer señala joseph malvehy coordinador unidad melanoma hospital clínic barcelona década problema triplica estimamos españoles melanoma vida mayores años desarrolla carcinoma tipo cáncer piel melanomamalvehy liderado puesta marcha encuesta nacional hábitos solares presentado resultados definitivos especialista adelanta datos obtenidos parecen confirmar hipótesis españoles conscientes efectos exceso exposición solar cambian hábitos siguen saliendo centrales aplicándose crema protectora insuficiente playa minutos etc fallando encuestados asumían lunares iba dermatólogo población riesgo desarrollar melanoma acuden especialistatan importante investigación prevención reglas sencillas razón cumplen deseable aficiones expuestos radiaciones solares año deberían ropa adecuada gorros sombreros manga larga crema protección solar olvidar rayos ultravioleta tipo altos inviernolas personas oficinas necesitan filtro año basta protejan piel expuesta recomienda malvehy ideal extender capa miligramos centímetro cuadrado piel seca media hora exposición solar bañoen fotoprotectores orales remarca doctor refuerzan sustituyen protección solar componentes sumplementos alimenticios antioxidantes vitaminas carotenoides realmente protegen quemaduras complemento habituales recomendaciones aconsejamos pacientes riesgo</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Salud_36.txt</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -971,11 +1176,16 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>decisión gobierno central incrementar salario mínimo interprofesional años forma escalonada euros mantener reuniones llegar acuerdos empresas sindicatos valora mercado laboral provincia castellón noticia positiva subrayan fuentes ccoo provincia recordando sindicato reivindica smi salario resto países europeos comparamos interesa gobierno turnoa cifra aproximada ccoo confirman trabajadores trabajadoras verán beneficiados repunte empleados cobran únicamente salario mínimo cifrado euros recuerdan ugtdesde ccoo ugt explican incremento transmitirá tranquilidad sectores hostelería turismo carecer convenio colectivo regule condiciones laborales nivel empresas documento desapareció octubre vigentes convenios empresa empresa fija condiciones denuncia sindicatos incluyen salarios bajos representan miseria apunta secretario ugt castellón francisco sacaciaademás sector sindicatos sitúan punto mira trabajadores ganan vida limpieza hogares cuidadores personas mayores discapacitados sectorestambién establecimientos comerciales subraya sacacia carecen convenio colectivo aplican casos smi vigente momentosacacia siguiendo línea ccoo apunta ugt valora positivamente incremento queda corto defendemos salario mínimo euros salario cifra reivindica secretario ugt sindicato meses puso marcha campaña ponte mil exigir salario mínimo digno cubra necesidades ciudadanía acorde crecimiento económico productividad percibiendocabe destacar ministerio seguridad social provincia castellón cifró noviembre afiliados seguridad social dato disponible presente ejercicio engloba personas afiliadas régimen autónomos trabajadores mar minería carbón referimos número afiliados régimen cifra sitúa personas cierre noviembre trabajadores cotizan firmado contrato personas forma ilegal práctica seguirá manteniendo casos seguirán cobrando lamenta secretario ugtletra pequeña leyasimismo pese sacacia subraya necesidad leer letra pequeña leyes smi incrementó llegar euros indicaba cobraban salario mínimo beneficiarían subida alertan ugt incidiendo subidas salarios deberían negociables alusión gobierno palabra pese mantener encuentros sindicatos confederación española organizaciones empresariales ceoe cepymepor ccoo apuntan salarios aportaciones seguridad social recaudación vía irpf consumo consecuente repercusión dinamización economía ingresos vía indirectapor asegurado incremento euros economía crecerá euros cifra euros</t>
+          <t>organización mundial salud oms actualizado listado principales causas muerte mundo mantienen enfermedades transmisibles patologías coronarias accidentes cerebrovasculares enfermedad pulmonar obstructiva crónica epoc top ten aparece diabetes sale tuberculosiseste organismo naciones unidas utilizado datos relativos año estiman murieron mundo millones personas enfermedades transmisibles responsables fallecimientos millones años representaban muertes millonesla causa muerte siguen enfermedades cardiovasculares mataron millones personas representaron fallecimientos millones cardiopatía isquémica millones accidente cerebrovasculara ambas dolencias siguen ranking infecciones vías respiratorias inferiores causantes millones muertes enfermedad pulmonar obstructiva crónica epoc millones enfermedades diarreicas millones vihsida millones cánceres tráquea bronquios pulmón millones diabetes mellitus millones accidentes tráfico millones nacimientos prematuros peso nacer millonesprecisamente oms destaca top ten sale tuberculosis obstante principales causas muerte provocando millón fallecimientos informe destacan causas muerte variar países altos bajos ingresos países ricos enfermedades transmisibles representan muertes países bajos ingresos representan ganan protagonismo enfermedades infecciosas vihsida enfermedades diarreicas malaria tuberculosis representan tercio muertes paísestambién diferencias edad fallecidos países ingresos altos muertes producen personas años muertes niños menores años países bajos ingresos muertes producen años personas años máslas complicaciones derivadas parto prematuro asfixia lesiones nacer encuentran principales causas muerte cobrando vida recién nacidos lactantesen oms pone relieve millones niños murieron cumplir años países bajos medianos ingresos complicaciones nacer neumonía enfermedades diarreicas malaria importante causa muerte edades especialmente áfrica subsahariana causa muertes menores años fallecimientos franja edad produjo vida</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Salud_29.txt</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -984,11 +1194,16 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>pspv eupv compromís pedido domingo alcaldesa valencia rita barberá dé explicaciones supuestos regalos valorados euros recibidos feria valencia aclare razón presentesasí solicitado grupos oposición raíz información publicada diario mundo fiscalía investiga marco diligencias gestión feria valencia regalos presuntamente entregados dirigentes pp alcaldesa fuentes recibido distintos complementos marcas lujoel portavoz socialista ayuntamiento joan calabuig advertido barberá fiscalía deja excusas seguir eludiendo asumir responsabilidad gestión feria valencia ¿en calidad recibía regalos institución ferial preguntado edil considerado inadmisible barberá pretenda eludir responsabilidades gestión entidades relacionadas consistorio aflorado presuntos casos corrupciónha incidido negativa pp aprobar pleno moción retirar cargos imputados cobra información aparece publicada miedo acaben imputados casos salpican ayuntamientoasí incidido regalos investiga fiscalía euros únicos procedencia dudosa recibe alcaldesa señalada reiteradas ocasiones receptora regalos lujo empresas entidades públicas emarsa investigada agujero contable millones eurosregalos álvaro pérez bigotes cabecilla trama gürtel valencia alcaldesa conversación telefónica interceptada policía curso investigación año aseguraba tienda louis vuitton comprándole bolso alcaldesa agregado calabuigcómplice necesariaen caso joan calabuig apuntado deriva feria valencia lamentable vuelto exigir barberá asuma responsabilidad política preside patronato nombra miembros comité ejecutivo miembros patronato visto ocupa cargo únicamente recibir regalos lujo criticadocon actitud barberá cómplice necesaria hundiendo feria valencia incapaz vigilar gestión evitar escándalo presuntos sobrecostes millonarios despilfarro agregadopor diputado eupv cortes víctor tormo señalado pp arruinado saqueado arcas generalitat feria valencia caso gobierno sale luz atraco arcas públicas regalos lujo alcaldesa regalos aceptó gustosamente valencianos engrosaban lista desempleados viendo peligrar casa dificultades llegar mes indicado tormo barberá debería dimitir inmediatamente obstante precisado esperamos decencia personajes esperamos justiciaasimismo compromís portavoz ayuntamiento joan ribó exigido explicaciones rita barberá presuntos regalos recibidos años dirección presidencia feria cometieron irregularidades investiga fiscalía anticorrupción informe elaborado intervención generalitat valencianaribó recordado barberá preside patronato feria valencia alcaldesa valencia figura estatutos entidad derecho público estatutos recogen operación comercial financiera supere euros aprobada patronatotodos conocemos predilección barberá firmas lujo desplazarse coche oficial rodeada escoltas vacaciones particulares gerencia feria valencia conocía gustos agasajaron bolsos pañuelos complementos comprados milla oro entregaban coche oficial pagado valencianos apuntadopor compromís exige barberá explique razón regalos preguntado barberá servirían patronato preside aprobará operaciones comerciales crédito euros</t>
+          <t>hungría asume enero presidencia rotativa consejo unión europea incorporación bloque comunitario forma convertirá tercer país bloque comunista cumplir rol siguiendo eslovenia república checasu debut anfitrión marcado fuerte polémica internacional flamante ley medios aprobada diciembredurante meses hungría hará cargo agenda consejo presidirá reuniones entrada vigor tratado lisboa presidencia ostenta mayoría políticas definen bruselas oportunidad clave mostrarse país tratar instalar temas agenda política internacionalla prioridad clave economía ministro exteriores jános martonyi fijado elementos esenciales coordinación políticas económicas enviar mercados financieros mensaje calma informa efeuno principales desafíos económico buscando aprobar sistema reforzado sanciones países déficit desequilibrios excesivos concluir negociaciones fondo rescate permanente países insolventes eurozonasumado continuará debate futuro presupuesto ue maneras país ocupará privilegiado negociaciones frenar crisis deuda eurozona eurootra prioridad presidencia húngara avanzar estrategia europea afrontar inclusión gitanos encaminar negociaciones integración croacia uehungría principales impulsores incorporación vecino gracias relaciones bilaterales budapest asumido firmar presidencia documento adhesión hará cerrar negociacionesen ámbito energético fomentar seguridad suministro países europa central dependen medida rusia ámbito expertoen febrero celebrará cumbre dedicada energía hungría esperanzas cerrar decisiones estratégicasademás país acogerá mayo cumbre países asociación oriental fortalecer relaciones ue repúblicas soviéticas ucrania bielorrusia moldavia georgia armenia azerbaiyán</t>
         </is>
       </c>
       <c r="C43" t="n">
         <v>2</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Politica_47.txt</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -997,11 +1212,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>secretario psoe josé luis rodríguez zapatero anunciado programa electoral socialista comicios año incluirá propuesta modelo financiación comunidades autónomas adaptado proceso descentralización añosel líder socialista anuncio conferencia prensa sede federal psoe informar reunión comisión ejecutiva partido análisis significado año socialistasexplicó psoe apuesta desarrollo autonómico implica apuesta reforma estatutos autonomía marco proceso solidaridad regiones convivencia ciudadanos cohesión territorialfinanciacióninformó programa electoral contendrá propuesta modelo financiación autonómica recordó respaldamos parlamento modelo impulsó gobierno pp subrayó apuesta desarrollo autonómico desarrollo llegado rincones españadestacó propondrá modelo adecúe proceso descentralización vivido años modelo diálogo consenso fuerzas políticas gobiernos autonómicos marca ley orgánica financiación comunidades autónomas espíritu constitucióngobierno pprodríguez zapatero análisis acción gobierno pp resume diciembre alta crispación política evidenció despedida presidente gobierno josé maría aznar congreso semana pasadaafirmó año acaba fuertes tensiones territoriales ponen manifiesto gobierno pp transmitir mensaje confianza esperanza estabilidad españoles transmite mensaje incertidumbres temores crispaciónel equipo electoralpara superar situación zapatero ejecutiva socialista aprobado marcha inmediatamente parón navideño campaña programa cuya elaboración trabajará presidente castillala mancha josé bono presidentes autonómicos cuyos nombres reveló zapatero pidió felipe gonzález irá listas socialistasfrente opinan debate electoral cohesión territorial zapatero psoe centrará políticas sociales advirtió partido elaboración constitución modelo territorial defendimos gobernando trece añosvamos seguir impulsando autonomías líder socialista mostró convencimiento ciudadanos garantiza convivencia unidad respeto diversidad sitio capacidad diálogosubrayó apuesta mensaje positivo confianza creer constitución estatutos frente lanzan temores peligros riesgos absurdo modelo autonómico cerrado resumió planes reforma senado participación autonómica ue adecuación estatutos cambios registrados años</t>
+          <t>neerlandés disfrutó cerrar batalla campeonaot anticipada dominio mitad temporada permitió corona pilotos premio japónesto contrasta título infarto abu dhabi terminó circunstancias controvertidas manejo fia reinicio coche seguridad carreraverstappen forma terminó lucha título lewis hamilton podía frente tensión duelo apretado tiempoen declaraciones the guardian puedes drama año seguro saludable equipo equipospero medida prepara calendario carreras verstappen consciente estrés tensiones pilotos posibilidades aumentarcuando preguntó preparado vuelta esquina verstappen preocupación complicaciones desafío necesitaba preparado mayores dificultadessi preparado dejarlo quiero corredores amamos carreraspor bonito temporada año bonito temporada año duro años año año pasadopero ocurre realmente fórmula debería bienel rival cercano verstappen charles leclerc coincidió opción preparado temporadas intensas avecinancreo preparados temporadas largas espero apretada lucha preparado carreras lucha larga esperoaunque red bull dominado año superado desventaja peso rb verstappen cree diferencia oposición mantenga gente entendiendo coches equipos acercaránsabemos invierno seguir empujando seguir tratando encontrar rendimiento rendimiento entender posiblemente neumáticos neumáticos cambiar año gestionar</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Deportes_8.txt</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -1010,11 +1230,16 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>fiscal superior galicia carlos varela reclamó martes elaboración plan gestión riesgos corrupción infracción conexas organismos entidades administraciones públicas gestionen dinero valores patrimonio público puedan adoptar medidas preventivas posibles riesgos corrupciónse evitar ocurran casos sobornos cohechos desfalcos públicos tráfico influencias varela comparecencia comisión administración públicas parlamento gallego insistió plan prevenir prácticas funcionarios públicos identificaría posibles responsables neutralizarpara propuso creación entidad funciones específicas prevención control problema prácticas relacionadas corrupción galicia consello prevención corrupción cpc funcionaría entidad administrativa independiente entidad fiscalizadora externa representa consello contasse perfilar eventual respuesta problema permitiendo creación grupo respectivos resultados apuntar caminos lógica preventiva permitan reducción número oportunidades práctica delitos insistiótodos grupos parlamentarios mostraron iniciativa consideraron apropiada actual situación política financiera numerosos casos corrupción administraciones públicas gallegas casos sonados operación campeón operación orquesta operación arena carioca otrasevitar reprochescarlos varela insistió combate criminalidad grave prácticas relacionadas corrupción centrar medios recursos sistema justicia penal evitar reproche digan rápidos juzgar condenar ladrón baratijas estafador esquina lentos juzgar defraudadores erario público violadores inocencia país generalmente respaldados profesionales especializados aliviar durar procesos paraíso prescripción indicóasí precisó corrupción extiende administración economía pasando ámbitos vida social espacio libre corrupción reclamó evitar prácticas administraciones púbicas deberían marcha planes prevención riegos corrupción frente soborno abuso información privilegiada tráfico influenciasla fiscalía superior galicia recalcó gestión riesgo corrupción protección salvaguarda intereses colectivos plan aplicaría actividad administración pública correspondiente integrantes órganos personal dirigente evitando desperdiciar recursos disponibledesde propuesta ocurrencia personal apuntar basa proceso metodológico análisis ámbito internacional forma grupo acción financiero internacional –gafi encarga analizar personas político ventajas terceros apuntó reino unido puso marcha prevention act evitar riesgos corrupción administraciones públicas portugal órgano consejo cuentaspor desarrollo plan encargar determinados funcionarios órganos semejantes implicaría coste adicional presupuestosun paso significativola paso significativo deberíamos dispuestos darlo evitar desviaciones distintas administraciones nacionalista tereixa paztambién socialista beatriz sestayo felicitó fiscal propuesta acogemos suma satisfacción proactivos medida erradicar prácticas corrupción apuntó reclamó medidas higiene democráticas actual coyuntura políticoeconómicapor popular paula prado mostrarse favorable medida criticó propuesta fiscal apareciera memoria fiscalía caso apuntó corrupción extendiendo ayuntamientos pequeños apostó erradicación leyes legislaciones actualizar queden libro concreten sentencias sanciones ejemplarizantes añadiólos grupos destacaron datos presentados memoria fiscalía nacionalistas incidieron documento demuestra tramas incendiarias socialistas agradecieron compromiso varela menores pidieron lucha delitos patrimoniales centre iglesias populares incidieron aumento delitos patrimonio asuntos violencia géneroprocesos tramitadosla fiscalía tramitó procedimientos penales año número delitos asociados volumen acusaciones aumentando ranking delitos seguridad colectiva situaron peldaño siguen delitos lesiones finalmente delitos patrimoniales justicia menores galicia tramitaron llevados juicio casos varela puntualizó delitos corregir dándole prioridad acciones pedagógicas inclusivassobre área personas discapacidad ministerio fiscal presentó año demandas incapacidad ambiente furtivismo tramitaron diligencias investigación penal furtivismo constituye actividad ilegal tolerada socialmente apuntó varelaen mediación familiar estadísticas reflejan tendencia alcista semestre derivados mediación asuntos semestre continuar ritmo crecimiento año terminar asuntos derivadospatrimonio culturalvarela robo códice calixtino puso mesa necesidad proteger patrimonio cultural galicia religioso enmarcó nacimiento proyecto iglesia seguracultura protegida evitar precisamente expoliación tipo bienes iniciativa participa xunta iglesia fiscalíafinalmente casos violencia género varela año registraron procedimientos sistema penal sustanciaron trámite juicios rápidos delito frecuente resultó delito maltrato familiar ocasional peso seguido maltrato familiar porcentaje</t>
+          <t>método imágenes estructura cromosomas dibujando cuadro real forma rara científicos consejo biotecnología ciencias biológicas investigación bbsrc reino unido colaboración universidad cambridge reino unido instituto weizmann israel producido modelos muestran precisión compleja forma pliegan interior adnla forma utiliza describir cromosomas instantánea complejidad doctor peter fraser instituto barbraham financia bbsrc imagen cromosoma mancha forma adn familiar imagen microscópica cromosoma realidad muestra estructura produce transitoriamente células punto punto dividirse mayoría células organismo termina dividiendo cromosomas parecen forma cromosomas células forma imposible crear imágenes precisas estructura investigadorel equipo fraser desarrollado método visualizar forma consiste miles mediciones moleculares cromosomas células individuales utilizando tecnología secuenciación adn combinación pequeñas mediciones potentes ordenadores creado retrato tridimensional cromosomas tecnología gracias financiación bbsrc consejo investigación médica mrc wellcome trust reino unido imágenes únicas muestran estructura cromosoma camino adn permite mapear genes específicos características importantes modelos comenzado desentrañar principios básicos estructura cromosomas papel funcionamiento genoma fraseresta investigación publicada revista nature pone adn contexto célula transmitiendo belleza complejidad genoma mamíferos eficaz muestra estructura cromosomas forma adn interior pliega íntimamente relacionadas cantidad genes expresan consecuencias directas salud envejecimiento enfermedaddouglas kell directivo bbsrc sentencia comprensión estructura cromosómica limitado imágenes borrosas diagramas conocida ven división celular imágenes verdaderas ayudarán entender parecen cromosomas mayoría células cuerpo intrincados pliegues ayudan desentrañar cromosomas interactúan controlan funciones genoma</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Salud_24.txt</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1023,11 +1248,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>restos dictador francisco franco saldrán valle caídos periodo octubre consejo ministros aprobado viernes exhumación inhumación establece horquilla plazo previo avisar familia vicepresidenta gobierno funciones carmen calvo anunciado rueda posterior reunión gabinete socialista funciones tribunal supremo respaldo legal pretensiones ejecutivo cálculo moncloa octubreel presidente gobierno funciones pedro sánchez llevado asunto consejo ministros pese formado reunión preparatoria previa comisión secretarios subsecretarios presidencia potestad sánchez ejercido temase tercer sacar franco llegada psoe moncloa junio año pronunciamiento previo congreso modificación ley memoria histórica darle cobertura legal quiso ejecutarse pasadas navidades estableció fecha junio falta familia recursos tribunal supremo demorado cumplimiento promesa ocasión ordena inmediata viernes cierre temporal valle caídos finalización operaciónahora nietos dictador acudido constitucional paralizar in extremis traslado restos cementerio pardomingorrubio ejecutivo decidido ejecutar sentencia supremo manos libres actuar quierael gobierno semanas plazo razón fuentes consultadas coincidencia sentencia procés conocerá próxima semana cuyas consecuencias cataluña inquietan ejecutivo querido fijar fecha exacta preferido dejarlo abierto elegir adecuado función suceda cataluña fechas apuntadas fuentes gobierno posteriores comunicación sentencia convocatoria huelga comunidad prevista movilización electoradola decisión exhumar franco producirá campaña electoral oficialmente comienza noviembre partidos especialmente sánchez inmersos larga precampaña calvo defendido escogido deseo gobierno socialistas piensan traslado restos franco contribuye movilización electoradopara gobierno vicepresidenta supone satisfacción extraordinaria cerrar dignidad digno años referencia tumba franco enterradas víctimas bandos exhumación justificar apunte fecha concreta hará gobierno funciones disponga medios técnicos seguridad permitanse realizará arreglo criterios fijado gobierno resoluciones anteriores reiterado calvo procederá absoluto respeto restos familia avisará antelación discreción nietos bisnietos deciden celebrar ceremonia acorde preferencias religiosas adoptarán medidas necesarias seguridad restos mortales seguridad ciudadana orden público ejecutivo descarta restos puedan trasladar helicópteroel consejo ministros establece actuaciones exhumación traslado inhumación presenta ministra justicia dolores delgado condición notaria reino cámaras medios comunicación caso presentes explanada</t>
+          <t>discusión eterna baloncesto grande tiempos pelea encabezada leyendas michael jordan anillos campeón icono trascendió allá baloncesto chicago bulls lebron james elegido años carrera anillos legado gigante prefieren mj grandeza lbj jugador discusión fomenta nbahay apoyos fuertes candidatura lebron draymond green otrora enemigo finales cleveland cavalliers golden state warriors apoya pasó the shop programa produce james hbo equipo títere cabeza lebron grande punto vistalo justifica longevidad cima empezó seguía jugador nba importar pasase juego visto juego hombres hombres relató drayy sufrió carnes james michael jordan batió equipo jamás creado warriors curry klay thompson draymond green temporada tiempos victorias derrotas cayó finales nba cavs lebronademás finales green vitales discusión años agotador competir finales año año nueve seguidas jordan parar descansar lebron finales señalótambién apoya juego fijas habilidades jugado juego baloncesto lebron james quieren jordan entiendo forma controlar partido imposible parar confesó sustenta cree talento juego vendrán viejos realidad apple mejores ingenieros analizóuna unión hechos longevidad talento rendimiento alto discusión años locura sentenció estrella warriors dudas lebron james tiempos</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Deportes_36.txt</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1036,11 +1266,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>británicos piensa brexit frente opina sondeo yougov cree alturas salir ue decisión equivocada sostiene decisión correcta encuesta reciente statista convencido brexit vida diaria servido disparar facturas cesta compra sondeo ipsosy pese recelo creciente votaron favor divorcio europa candidatos conservadores boca agua hablando oportunidades brexit prometido fieles presagio lanzado semana boris johnson partida significa brexit piensan equivocados demostrarhasta líder oposición laborista keir starmer defensor permanencia regurgitado lema rival quiero brexit funcione declarado intención reabrir heridas explorar opciones futuro ingreso mercado únicolos políticos quieren hablar tema dimisión johnson hito destino brexit escribe jonathan freedland the guardian autor salida reino unido ue caído proyecto desastroso seguir caminorecuerda freedland victoria referéndum apoyada falsedades marcado años gobierno boris johnson empezando ahorro millones libras semanales millones euros pintado famoso autobús rojo campaña vote leave realidad sirviendo desacreditar brexit sostiene columnista crecimiento lento facturas altas problemas constantes ausencia beneficios concretos saltan vista sigan usando palabras abstractas libertad soberaníadurante debate televisivo brexit convirtió arma arrojadiza candidatos rishi sunak desperdició oportunidad lanzarle liz truss pregunta incisiva noche ¿te arrepientes liberaldemócrata apoyado permanencia uela secretaria exterirores corrió cortina jactó haberle impulso brexit gobierno firmando acuerdos comerciales japón australia parecían impensables plantando cara ue negociación protocolo irlandalos candidatos conservadores profundamente brexiterosconsciente tirón ideológico brexit ala dura partido secretario tesoro rishi sunak marcó tempo debate candidatos conservadores cadena itv prometiendo revisión reforma derogación leyes transferidas ruptura bruselasgracias brexit reino unido siglo xxi nación soberana global defensora comercio libre control leyes regulaciones política comercial internacional anticipó sunak prometió sustitución actual ministerio oportunidades brexit llamado brexit delivery department departamento entrega brexit montasunak defendió salida ue referéndum dudó desempolvar remainer rival secretaria exteriores liz truss terminado explicar razones fondo conversión quiero hijas crezcan mundo necesiten visado permiso europa empresas puedan crecer costes barreras comerciolos defensores liz truss ministro brexit david frost arroparon candidata recordando firmeza hora impulsar unilateralmente ley protocolo irlanda frente postura blanca sunak advirtió frost hagas saltar aires negociaciones ueel veterano diputado bill cash apoyo domingo liz truss comparándola margaret thatcher determinación hora frente ue pidiendo brexiteros unan fuerzas candidatura atrás julio sabrán nombres finalistasla candidata predilecta bases penny mordaunt defendió expediente favor brexit campaña referéndum frente ofensiva mediática defensa derechos trans diputada kemi badenoch representante ala dura incondicionalmente favor brexit quinto discordia moderado tom tugendhat contrario salida ue muestra travestismo político reiteró compromiso exprimir oportunidades brexit llega ministro</t>
+          <t>presidente chino xi jinping rindió martes homenaje público exlíder recién fallecido jiang zemin asegurar supervivencia partido comunista chino pcch tormentas políticas marcaron etapa gobierno acciones modernizar economía nacionaljiang falleció miércoles shanghái años problemas salud logros frente país años noventa figuran sacar china aislamiento diplomático sometió masacre tiananmen enmendar relaciones unidos supervisar crecimiento económico precedentes sentaron bases convertir china potencia mundial hoychinajiang zemin falleció miércoles shanghái años problemas saludel adiós salón pueblo plaza tiananmen precedido minutos silencio siguieron segundos sonaron sirenas bocinas pekín ciudades chinasal tomar palabra xi describió finado prestigioso líder marxista diplomático guerrero comunista lideró país eta desafíos precedentes referencia parcial protestas tiananmen jiang accedió poderhorizontalciudadanos chinos depositan flores homenaje líder fallecido hector retamal afpa finales años ochena principios noventa serias tormentas políticas país extranjero socialismo mundial experimentó graves complicaciones élite política país congregada sala vestida riguroso negro mascarillael actual presidente subrayó persistencia jiang hora seguir proceso apertura reforma auspiciado antecesor deng xiaoping elogió supervisar mandato vuelta soberanía china antiguas colonias británica portuguesa hong kong macao asimismo apuntó visión fallecido país próspero liderazgo hora lograr china ingresase organización mundial comercio chinaxi elogió liderazgo jiang lograr china ingresase organización mundial comercioxi elaboró discurso retrato jiang instalado tribuna situadas cenizas antiguo presidente cubiertas bandera hoz martillo carteles dispuestos sala leían eslóganes amado partido ejército etnias pueblo chino camarada jinag zemin vivirá siempreel cuerpo jiang incinerado lunes acto celebrado cementerio capitalino babaoshan descansan restos numerosos líderes revolucionarios pcch presente sucesor cargo predecesor xi hu jintao cuya inesperada salida forzada xx congreso partido comunista octubre despertó rumores purga públicahorizontalel palacio pueblo celebró acto amaneció martes rodeado fuertes medidas seguridad noel celis afpdurante jornada páginas web medios estatales instituciones tiñeron blanco negro banderas ondearon media asta bolsas shanghái shenzhen cerraron minutos comos señal homenajecon recuerdo fresco recientes protestas políticas anticovid semana fuerzas seguridad reforzaron presencia calles garantizar reprodujeran concentraciones públicas autorización vano muerte jiang provocado ola nostalgia población percibe frente relativa liberalidad comparación actualhorizontalciudadanos chinos siguen vivo discurso presidente xi jinping acto despedida fallecido jiang zemin andy wong apaún numerosas sombras pesan legado jiang mandato evidenció graves desequilibrios modelo crecimiento costa auge explosivo desigualdades sociales daños medioambientales altos índices corrupción pesan espaldas campañas activistas tibetanos miembros organización religiosa falun gongdurante jiang consiguió tejer poderosa red influencias base feudo shanghái alcanzó segmentos país economía ejército remanentes erradicados xx congreso pcch manos xi década frente arrinconado facciones rivales concentrado persona finiquitado modelo gobierno aupó jiang</t>
         </is>
       </c>
       <c r="C47" t="n">
         <v>2</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Politica_60.txt</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -1049,11 +1284,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>hungría asume enero presidencia rotativa consejo unión europea incorporación bloque comunitario forma convertirá tercer país bloque comunista cumplir rol siguiendo eslovenia república checasu debut anfitrión marcado fuerte polémica internacional flamante ley medios aprobada diciembredurante meses hungría hará cargo agenda consejo presidirá reuniones entrada vigor tratado lisboa presidencia ostenta mayoría políticas definen bruselas oportunidad clave mostrarse país tratar instalar temas agenda política internacionalla prioridad clave economía ministro exteriores jános martonyi fijado elementos esenciales coordinación políticas económicas enviar mercados financieros mensaje calma informa efeuno principales desafíos económico buscando aprobar sistema reforzado sanciones países déficit desequilibrios excesivos concluir negociaciones fondo rescate permanente países insolventes eurozonasumado continuará debate futuro presupuesto ue maneras país ocupará privilegiado negociaciones frenar crisis deuda eurozona eurootra prioridad presidencia húngara avanzar estrategia europea afrontar inclusión gitanos encaminar negociaciones integración croacia uehungría principales impulsores incorporación vecino gracias relaciones bilaterales budapest asumido firmar presidencia documento adhesión hará cerrar negociacionesen ámbito energético fomentar seguridad suministro países europa central dependen medida rusia ámbito expertoen febrero celebrará cumbre dedicada energía hungría esperanzas cerrar decisiones estratégicasademás país acogerá mayo cumbre países asociación oriental fortalecer relaciones ue repúblicas soviéticas ucrania bielorrusia moldavia georgia armenia azerbaiyán</t>
+          <t>gripe supone constante amenaza salud pública epidemias estacionales oms provocan millones casos graves millón muertes año mundo riesgo capacidad cambiar cara virus gripal consiga provocar próxima pandemiahace años frente amenaza distintos grupos científicos buscan desarrollar vacuna universal frente gripe permita adelantarse posibles variaciones patógeno ofrecer escudo protector preparado afrontar ataqueuna investigación publicada jueves science acerca paso objetivo datos científicos estadounidenses conseguido desarrollar vacuna universal gripe modelos animales resulta protectora desarrollo prueba concepto llevado cabo tecnología arn mensajero empleó vacunas covideste abordaje permitido científicos liderados claudia arevalo instituto inmunología universidad pensilvania eeuu crear vacuna contiene antígenos correspondientes subtipos identificado virus gripea circulan humanos tipos virus gripe hn hn linajes virus tipo vacunas estacionales cuya efectividad limitada dirigen variantes tipos virus máximo antígenos producto subtipos virus afectan humanos menor medida potencial pandémicoel equipo arevalo conseguido desarrollar formulación incluye antígenos subtipos tecnología arn mensajero podido encapsular producto proteínas específicas subvariantes concreto hemaglutininas proteínas constituyen sitios principales reconocimiento antigénico sistema inmunitariobuenos resultados ensayos preclínicosen experimentos ratones hurones investigadores pudieron comprobar vacuna inducía animales producción anticuerpos específicos frente subtipo permanecían organismo meses vacunación numerosos obtienen vacunación convencionaltras someterles desafío virus gripe investigadores comprobaron animales vacunados presentaban protección frente patógenosnuestro estudio indica vacunas arn mensajero proporcionar protección frente virus antigénicamente variables inducir forma simultánea anticuerpos frente múltiples antígenos señalan investigadores revista científica</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Salud_14.txt</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -1062,11 +1302,16 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>berlusconi incapaz vanidoso ineficaz descansa suficientesilvio berlusconi líder física políticamente débil causa frecuentes largas noches inclinación fiestas descanse suficiente retrato ministro italiano responsable asuntos americanos embajada unidos roma elisabeth dibble revelado mundo filtración wikileaksy documentos enviados embajada americana talia departamento eeuu referencia il cavaliere tipo incapaz vanidoso ineficaz líder moderno amante fiestas salvajespero suficiente diplomacia unidos muestra preocupada estrecha relación existente ministro italiano homólogo ruso vladimir putin relación estrecha estrecha ojos americanos berlusconi presenta portavoz putin europa relación líderes cimienta ojos diplomacia eeuu machismo compartido putin macho dominante político autoritario cuyo estilo machista permite conectar perfectamente berlusconi lee documentospero unidos sospecha fuerte amistad putin berlusconi apuntalado negocios despacho fecha enero hillary clinton secretaria norteamericana solicita cuerpo diplomático busque información relación personal putin berlusconi averigüe inversiones personales condicionar política exterior económicalos contenidos documentos filtrado muestran nivel descrédito ministro llevado imagen italia queja partido democrático principal formación oposición centroizquierda italiana juicio unidos ministro deprimente sostiene francesco rutelli líder centrista alianza italiasin ministro italiano exteriores franco frattini asegura revelaciones piensa realidad unidos gobierno italiano afectar relación países duda calificar filtración wikileaks septiembre diplomacia</t>
+          <t>permíteme dato explicarlo técnicos presupuesto corea sur tiro arco millones euros calcula rubén montes director deportivo federación española tiro arco acaba despejar incógnita dinero montón dinero acabar amamos deporte incertidumbrevamos hechos corea sur ganado oros disputa juegos tokio lunes equipos categoría masculina camino pleno victorias consiguió juegos río país tirador capaz romper racha tiro arco suele abierto sorpresas atrás categoría femenina pierden equipos dejado escapar triunfo individual dream team baloncesto mantiene récord parecidoel arco flechas elementos deporte nacional país asiático indudable conseguido dominio abrumador tradición sitio escuelas primaria institutos universidades equipo tiro arco digo quiero excepción cantera arqueros inagotable cuentan estructura potente liga profesional clubes profesionales sueldos euros anuales media mejores prácticamente millonariosrecrear escenarioel presupuesto federación guinda pastel dinero compre permite tiradores dediquen exclusivamente entrenar mejores instalaciones juegos recreado seúl recinto olímpico construido idéntico tokio acostumbradísimos ambiente analiza montes recuerda coreanos cayeron mundial categorías chicos imbatibles chicas llevan ganando oro interrupción reconoce técnico analiza lanzamientos asiáticos concluye distinto descubierto truco inventado nadade kisik lee seleccionador coreano entrenador unidos corea sur utiliza técnica eficiente analiza biomecánica tiros centenares arqueros profesionales entrenar compiten semana rivales nivel ventaja difícil revertir finaliza montes espera competición queda llegue alegría españolaeste martes tifón permite daniel castro empezará cuadro individual masculino rival coreano kim woojin logra alcanzar cuartos derrotarle complicado realmente complicado montón dinero acabar amamos deporte incertidumbre</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Deportes_48.txt</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1075,11 +1320,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>cuba anunció retirada doctores brasil acusar presidente electo país jair bolsonaro exigir condiciones inaceptables mantener prestación servicios médicos aporta importantes ingresos gobierno cubanoel ejecutivo presidido miguel díazcanel tomado decisión continuar participando programa médicos ministerio salud comunicado ampliamente divulgado entidades medios estatales habanaen marco programa iniciado años doctores cubanos prestan atención médica brasil comunidades desfavorecidas remotas favelas río janeiro sao paulo poblaciones indígenas amazonasel presidente díazcanel pronunció decisión oficial twitter dignidad profunda sensibilidad profesionalidad entrega altruismo colaboradores cubanos prestado valioso servicio pueblo brasilactitudes dimensión humana respetadas defendidas somoscuba mandatario islael gobierno cubano atribuyó decisión retirar médicos declaraciones amenazantes despectivas bolsonaro prometió revisar contrato bilateral endurecer condiciones permanencia especialistas brasil asuma enerosalario integralel presidente electo brasileño tendencia ultraderechista criticado modelo actual programa médicos defendido continuidad modificaciones especialistas cubanos reciban salario integralhoy bolsonaro replicó gobierno cubano tuit recordó exigencias condicionamos continuidad programa médicos aplicación test capacidad salario integral profesionales cubanos destinado dictadura libertad traer familias infelizmente cuba aceptóla exportación servicios médicos importante fuente divisas cuba formación universitaria completamente gratuita año miles estudiantes licencian carrera medicina ejercer paísa cambio gobierno cubano embolsa salario perciben doctores países extranjeros comisión caso destinados brasil estima brasil paga dólares quedan efe médico cubano ejerce especialidad brasilrepatriacionesla fuente reveló comenzado repatriaciones doctores cuba proceso continuará próximas semanaspara destacar irreversibilidad decisión ministerio salud cubano remarcó comunicado directora ops organización panamericana salud líderes políticos brasileños fundaron defendieron iniciativatambién esbozó argumento doctores despachados brasil mantenido puesto salario cuba dólares mes alto comparación profesiones estatales insuficiente frente necesidades diarias islaprograma socialla participación cubana médicos realiza ops años funcionamiento profesionales isleños tratado millones pacientes brasileñosse teme programa aseste duro golpe frágil economía cuba cuya fuente divisas exportación servicios profesionales médicos recauda millones dólares anuales promediolos resultados económicos actividad superan ampliamente industria turismo registró ingresos millones dólares datos disponiblesen septiembre destitución presidenta dilma rousseff surgieron dudas continuidad doctores cubanos programa social brasileño finalmente cuba confirmó mantendríaen discursos ganar elecciones brasil bolsonaro anunciado giro política exterior acercarse eeuu cortar lazos medida venezuela cuba países gobiernos socialistas</t>
+          <t>número afectados fallecidos tuberculosis descendido significativamente mundo camino alcanzar objetivos milenio relativos enfermedad quedan metas cumplir datos alarman especialmente organización mundial salud omsen informe global tuberculosis organismo naciones unidas manifiesta preocupación alarmante aumento resistencias antibióticos tradicionales restricciones acceso fármacos culpa problemas económicos larga lista paísesde documento advierte enfermos tuberculosis mundo tratamiento millones personas escapan sistemas sanitarios convierten preocupante problema salud pública afectados países siquiera diagnosticados reconoce mario raviglione director programa global tuberculosis omsun problema paralelo falta recursos sistemas salud advierte oms capacidad llegar pacientes marginales difíciles captar vías tradicionales significa diagnosticar tratar preocupa especialmente caso cepas resistentes multiresistentes responden mayoría antibióticos disponiblesde tests diagnóstico rápidos permitido aumentar número casos detectados pacientes tuberculosis multiresistente siguen diagnosticados caso detectados pacientes diagnosticados acceso tratamientoen caso tuberculosis iniciar cumplir tratamiento antibióticos esenciales paciente recupere deje transmitir bacilo personas incumplimientos tratamiento antibióticos aumento mundo cepas tuberculosis resistentesla oms calcula personas enfermaron tuberculosis año china india federación rusa casos pacientes coinfectados virus vih recibe tratamiento antirretrovirales tuberculosis patología infecciosa aprovecha inmunodeprimido pacientes desarrollarse calcula tercio población tuberculosis latente riesgo real enfermarel informe oms concluye recomendaciones afrontar patología cumplir objetivos milenio naciones unidas enfermedad tratar llegar millones personas escapan control sistemas salud seguir propagando enfermedadademás pide autoridades esfuerzo económico afrontar problema resistencias recomendaciones concluyen mención especial coinfectados vih acelerar innovación tecnológica tests diagnósticos tratamientos lleguen países necesitados finalmente inversión económica patología recuerda oms países recursos dependen fondos internacionales frente tuberculosis</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Salud_17.txt</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -1088,11 +1338,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>centroderecha triunfa elecciones locales celebradas domingo ayuntamientos italia gracias impulso liga movimiento estrellas conquista ciudad prepara vuelta municipios examen recién estrenado gobierno giuseppe conte nacido pacto ultraderechista liga confirma aumento consenso favor liga ciudades presentaba coalición forza italia silvio berlusconi postfascistas hermanos italiaestoy contento alcaldes ciudadanos óptimos alcaldes exultante matteo salvini ministro interior líder liga resultados afluencia baja superó frente anteriores elecciones millones italianos llamados urnas confirmaron tendencia elecciones políticas marzo confianza liga alza líder indiscutible centroderechael movimiento estrellas presentaba ayuntamientos sufre frenazo perder alcaldía ragusa sicilia única capital provincia votó gobernaba actual alcalde grillino antonio tringali consiguió votos afrontar vuelta electoral municipios mil habitantes candidato supera sicilia celebra vuelta prevista junio mil habitantes suficiente alcanzar mayoría sufragiosel centroderecha presentará partido vuelta capitales provincia centroizquierda hará votabanlos resultados mejores esperados partido democrático pd perdedor elecciones generales marzo logró acceder vuelta bastiones históricos ciudades toscanas siena pisa única ciudad participación aumentó precedentes elecciones respiro partido atravesando grave crisis interna supera pelos examen gracias presentó coalición partidos izquierda pd cambiar abajo noticia muerte fuertemente exagerada ministro paolo gentiloni necesaria alternativa gobierno guiado salvini</t>
+          <t>enfermedades cardiovasculares siguen causa muerte mundo estadísticas actualizadas organización mundial salud oms patologías infecciosas cáncer patologías corazón tercios muertes mundo millones infecciones accidentes responsables tercio restantesegún datos oms millones personas fallecieron causa problema cardiovascular fallecimientos concretamente enfermedad isquémica infartos causó millones muertes accidentes cerebrovasculares ictus causaron millones defuncioneseste fenómeno exclusivo países ricos puesto millones muertes enfermedades comunicables registradas produjeron países bajos medios recursos oms recuerda muertes prematuras evitadas dieta saludable ejercicio físico abandonando tabacopor problemas corazón lista primeras causas muerte mundo encabezada cáncer diabetes afecta población mundial problemas pulmonares crónicos epoc enfisema años aprecia preocupante aumento víctimas cáncer pulmón pasan millones diabetes aumenta millones mundotambién incrementan víctimas accidentes tráfico costaron vida personas descienden víctimas partos prematuros pese top ten causas muerte calcula niños nace semana gestación tuberculosis dejado lista principales causas mortalidad mundoel vih permanece sexta posición dramático ranking causa menor número fallecimientos anuales millones esperanza vida niño nacido ronda años dependerá medida nacimiento oscilar años nacido oms preocupada millones niños mueren año mundo cumplir años causas fácilmente evitables infecciones mala atención parto mueren mujeres complicaciones embarazo parto</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Salud_35.txt</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -1101,11 +1356,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>presidente república sergio mattarella encargado economista carlo cottarelli formación ejecutivo transición conduzca país convocatoria elecciones anticipadas economista aceptado reservas prometido gobierno mantendrá neutralidad asuntos políticos electorales cottarelli comprometido presentarse próximas elecciones asegurado exigirá compromiso miembros futuro gabinetela normativa italiana establece encargado formar gobierno acepte reservas presente jefe retirar reserva garantizado apoyos parlamentarios situación excepcional producido encargo rompe esquemas habituales cottarelli encabezará ejecutivo lista ministros técnicos presentará programa gobierno cámaras parlamento caso obtener confianza programa incluirá aprobación septiembre presupuestos generales año economista reunirse mañana presidente gobierno presentará renuncia convocarán elecciones anticipadas celebrarán probablemente caso obtener mayoría necesaria parlamento opción probable gobierno dimitiría inmediatamente formaría ejecutivo instrumental sustitución dimisionario gobierno paolo gentiloni capacidad gestionar asuntos corrientes mantendría convocatoria elecciones veranoen aumentado tensiones mercados financieros prima riesgo aumentado economía italiana creciendo cuentas públicas control cottarelli comparecencia aceptar encargo gobierno guiado aseguraría gestión prudente cuentas públicas señaladocottarelli aprovechado lanzar mensaje calma mercados internacionales europa diálogo unión europea ue defensa intereses esencial diálogo constructivo reconocimiento pleno papel italia economista confirmado participación italia zona eurocarlo cottarelli años conocido poderes políticos económicos italia experiencia internacional brillante currículo economista convertido reconocido analista actual crisis años trabajando fondo monetario internacional fm banca italia experiencia petrolera italiana eni nombrado comisario reducción gasto público gobierno enrico letta encargo terminó año llegada matteo renzi sabor agridulce podido implementar cien cien propuestas cálculos permitirían país ahorrar millones eurosa finales volvió fmi director ejecutivo director observatorio cuentas públicas italianas universidad católica milán domingo recibió sorpresa llamada presidente mattarella encontraba milán imparte clases economía prestigiosa universidad bocconila jura cargo ministros producirse mañana cottarelli deberá presentarse parlamento someter gobierno voto confianza senado cámara diputados movimiento estrellas liga suman votos parlamento fácil encontrar mayoría apoye ejecutivo</t>
+          <t>enfermedad mental adicciones ocupan plano atención médica abuso sustancias trastornos psiquiátricos reciben recursos dolencias resultados estudio animan pasar problemas plana sanidadsegún datos publicados revista the lancet impacto escala global pensaba subraya investigación males contribuyen medida vih tuberculosis generar enfermedad discapacidad mundonuestros resultados muestran creciente desafío enfermedades suponen sistemas sanitarios regiones desarrolladas vías desarrollo señalan investigadores revista médicaliderados harvey whiteford universidad queensland australia equipo científicos analizó datos salud mental abuso sustancias incluidos the global burden of disease study gbd estudio describir forma sistemática causas distribución principales enfermedades mundoen evaluación observaron enfermedades mentales trastornos relacionados abuso sustancias quinta causa muerte enfermedad mundo afinaron investigación midieron impacto dolencias capacidad generar trastornos letales encontraron problemas cabeza lista contribución discapacidad problemas calidad vida provocan trastornos notables subrayan investigadores hincapié número muertes debidas instancia enfermedad mental suicidios clasificándose categorías impacto infravalorándoseel análisis encontrado diferencias notables esperables distintas regiones mundo proporción trastornos relacionados alimentación alta zona australia asia áfrica subsaharianasegún datos enfermedades mentales abuso sustancias aumentado presencia décadas países vías desarrollo preocupante futuronuestras conclusiones implicaciones sustanciales agenda salud pública aumento esperanza vida supondrá personas enfermedades mentales trastornos relacionados sustancias vivirán periodo tiempopor publicado número the lancet dibuja detallado mapa consumo sustancias ilegales mundo anfetaminas cannabis cocaína opiáceos heroína enfermedades discapacidades generadas consumo tipo drogas aumentado incremento número población quinta aumento estima prevalencia personas adictas particularmente consumo opiaceos muertes atribuidas adicción drogas ocurridas piensa mitad produjeron dependencia opiáceosademás datos análisis revelan tercios adictos hombres diferencia cannabis droga consume mundo millones usuariospor opiáceos heroína sustancias problemas salud provocan mundoal acompaña revista médica investigación muestra importantes variaciones regionales dependencia cocaína elevada américa norte latinoamérica presencia regiones puramente anecdótica caso opiáceos mayores tasas consumo detectaron australia asia europa occidentalreino unido eeuu sudáfrica australia países problemas salud relacionaron consumo estupefacientes</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Salud_26.txt</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -1114,11 +1374,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ultraconservador andrzej duda permanecerá jefatura polaco años iguala mandato socialdemócrata aleksander kwasniewski único presidentes polonia instauración democracia empezando lech walesa punto lograrlo rival liberal rafal trzaskowski logró campaña sacar armario millones polacos atrevían basta deriva democrática hegemónico gubernamental partido ley justicia pis duda apadrinadode años jurista profesión duda carta líder jaroslaw kaczynski líder pis partida unión europea caballo troya reformas bruselas recela justifica discurso nacionalista busca resarcir polacos agravios historia batería leyes adoptadas gobierno pis sancionadas duda figura norma castiga años prisión hablar campos concentración polacos ley holocausto criticada israel considerar desafiaba históricahijo pareja profesores escuela minas metalúrgica cracovia carrera política duda ligada hermanos lech jaroslaw kaczynski edad años jaroslaw ministro convirtió subsecretario justicia diputado eurodiputado vicesecretario presidente lech muerte tragedia aérea smolensk rusia intentó éxito hacerse alcaldía cracovia ciudad natalduda carecía rostro inmensa mayoría polacos finales elecciones presidenciales vista jaroslaw kaczynski anunció pronóstico concurría jefatura hermano trágicamente vacante hombre fuerte pis lanzó candidatura duda mayo edad años desconocido candidato convirtió presidente polacos votos presidenciales ajustadas vividas poloniacontra aborto personas lgtbiarrancó mandato cohabitación partido liberal plataforma cívica po gobierno donald tusk abandonó puesto convertirse presidente consejo europeo elecciones parlamentarias octubre pusieron cohabitación sexta economía ue viraje derecha pis conquistó mayoría aplastante legislativoduda apuntalado kazcynski oficialmente pertenece partido superviviente políticos dóciles compensa falta carisma ejecutivo promesas sociales económicas programa gobierno pis nichos desfavorecidos rural familias tradicionalistas poderosa iglesia católica duda tomado debate aborto llevó miles mujeres calle llamado lunes negro semana plena campaña electoral firmó propuesta prohibir adopción parejas sexo iniciativa inocente rival trazkowski colectivos lgtbi pedido voto pisaba talones encuestas escuchen idioteces sobe derechos humanos gente gente normal repetido portavoces duda campaña enfrentó orgullo prejuiciosla estrategia resultado frente cambios representaba europeísta liberal alcalde varsovia duda apeló continuismo polonia conservadora beneficia derechos libertades ayudas económicas ue sienten sarpullido club dominado vieja potencia invasora llamada alemania excesivamente condescendiente enemigo rusiael aliado europeo fiel trumpno desapercibido semana cita urnas duda viajara unidos entrevistarse presidente donald trump presentó aliado europeo otan fiel solícito encuentro produjo trump anunciara retirada efectivos estadounidenses alemania polonia acogería gradoen recta vuelta duda visto envuelto escándalo intentado escapar removiendo fantasmas puro estilo pis semanario polaco fakt reveló duda concedió marzo perdón presidencial convicto abusos sexuales levantó orden alejamiento pesaba abusar hija petición edadduda respondió difusión información fakt propiedad conglomerado alemán axel springer acusando alemania intromisión elecciones campaña despiadada sucia dirigida personalmente ¿los alemanes quieren elegir presidente polonia injusticia permitiré acto campaña región dolny slask apelo embajador alemán varsovia intervenga deseamos tipo intervenciones extranjeras polonia inmiscuye elecciones alemanas portavoz campaña duda adam bielanel portavoz gobierno alemán steffen seibert rechazó tajantemente acusaciones duda dispersado semillas agarran barbechos polonia apela resentimiento conspiración</t>
+          <t>coronavirus virus gripe gripe mismísimo virus respiratorio sincitial vrs amigos entendernos responsable mayoría bronquilitis jaque consultas servicios urgencias pediátricas españa común virus respiratorios campan respetos menor medida provocar fiebre realmente fiebre tratarlacomo norma fiebre temperatura alcanza °c axila °c toma recto abajo cosa suele caliente necesita grado considerarlo fiebrepor aparece fiebrepor compuestos llamados pirógenos ocurre espectáculo pirotécnico fuegos artificiales falta pólvora alguien encienda mecha caso encienden mecha llamados pirógenos microbios virus bacterias compuestos producen microbios fiebre reacción normal cuerpo generalmente aparece infección virus bacterias fiebre amiga respuesta combatir infección activar defensas organismoqué consecuencias fiebreaquí traigo noticias fiebre causa daño cerebral ceguera sordera muerte pacientes temen fiebre produzca daños elevaciones transitorias modestas temperatura central °c °c infecciones agudas suelen tolerarse fiebre elevada fiebre causa daño enfermedad genera fiebre fiebre causar síntomas escalofríos sudoración malestar sofocos calory °cpor °c cosa empieza fea elevaciones extremas °c causar daños normalmente aumenta temperatura suele términos técnicos conoce hipertermia ambiental grave calor exterior sube fiebre aparece famoso golpe calor fiebre sube °c tomamos drogas ilegales ej cocaína medicamentos anestésicos medicamentos antipsicóticos</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Salud_11.txt</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -1127,11 +1392,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>comité investiga asalto capitolio enero presentó pruebas martes presidente estadounidense donald trump planeó instigar seguidores acudir sede congreso círculo cercano reunió grupos ultra participarontrump escribió tuit envió mensaje conservan archivos nacionales suficiente comité demostrar trump consejeros interesados alentar masasel llamamiento líder republicano avanzaba iba discurso mañana pedía llegar multitudes previstas instaba gente dirigirse capitolio certificando votos condujeron investidura demócrata joe bidenla audiencia puerta abierta reflejó grupos ultraderechistas oath keepers proud boys lideraron protesta coordinado gente confianza trump contacto ellosdías asesor seguridad nacional michael flynn participara reunión despacho oval analizó revertir resultado elecciones fotografiado capitolio miembros destacados oath keepersasimismo colaborador roger stone usó chat encriptado coordinar esfuerzos escrutinio cierre urnas llamado amigos stone participaban miembros ambas organizacionesla audiencia martes séptima comité centró vínculos disparatada reunión diciembre despacho oval trump publicó tuit avanzaba iba protesta enero washington animaba acudir iba salvajeen encuentro insultos acusaciones deslealtad trump dictar decreto abogada sidney powell poderes incautar máquinas votación volver recuento papeletas precisó legislador demócrata jamie raskin miembro comitéfinalmente ganó común entiendo siquiera mala idea idea terrible país powell pat cipollone abogado casa blanca luchó esfuerzos presidente revertir resultado eleccionesel comité obstante descartó martes trump manipulado ignorar asesores cercanos creer fraude electorales hombre años niño impresionable mundo país responsable acciones decisiones acceso información detallada específica mostraba elección robo legisladora liz cheney republicanos forman comité enfrentada mandatarioinstigación armaspor criticó siguiera denuncias mensajes interpretados llamamiento protesta armas extremistas hablaron abiertamente internet acudir armados capitaluno stephen ayres entró capitolio aferraba palabra trump intervención martes convencido elección fraude presidente republicano iba gente protesta enerolos mensajes circulaban redes sociales mayoría naturaleza violenta hablaban celebrar boda roja recordó raskin martes sirve hablar clave masacrelas reuniones casa blanca trump siguiera variadas diciembre comité participaron once republicanos presionó vicepresidente mike pence ayudara darle vuelta resultadosel comité promete revelaciones próximas audiencias reveló cheney trump intentó llamar testigo declarado rechazó responder advirtió abogado tentativa</t>
+          <t>lamentablemente delegación mexicana participa juegos olímpicos tokio jornada resultados positivos competidores disciplinas escasos posibilidades medalla esfumaron quedaron camino competenciassin duda eliminación dolorosa méxico ocurrió tiro arco alejandra valencia cayó estadounidense mackenzie brown duelo máximo flecha desempate competidora barras estrellas terminó círculo central dejar arquera aztecapor clavados aranza vázquez logró colarse ronda trampolín metros individual femenil finalizar ronda preliminares octavo caso contrario compatriota aratxa muñoz lamentablemente erró saltos recibió calificación cero dejándola competenciala selección mexicana beisbol debutó juegos olímpicos desafortunadamente bateo escaso novena verda derrotados república dominicana pizarra arranque atletismo tokio méxico ventana oportunidades pies edgar rivera originario agua prieta sonora terminó participación quedar octavo grupo preliminatoriootra esperanzas país competencias julio dafne navarro gimnasia trampolín calificó resultado óptimo competencia medallas mexicana terminó lugarmientras boxeo rogelio romero eliminado cuartos peso semipesado sucumbir frente arlen lópez cuba cartones mexicano termina participación justa veraniegaeste contenido vídeo disponible zona geográficacarlos ortiz convirtió esperanza medalla méxico finalizar boxeo clasificación tarjetas estadounidense xander schauffele compatriota abraham ancer ubicado posición</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Deportes_42.txt</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -1140,11 +1410,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>líder partido populista austriaco fpö protagonista llamado ibizagate heinzchristian strache vuelve política partido nombre responde tradición formación vicepresidente austria strache obligado marcharse fpö escándalo provocado vídeo indicios corruptelas anunció viena regreso vida pública movimiento equipo hc strache alianza austria formación pretende concurrir elecciones regionales viena mes octubreel equipo hc strache asume ideario principios políticos fpö modeló notable éxito centrará fortalecimiento intereses regionales nacionales austria venos contrapeso globalización mundo control alternativa progresivo desarraigo sociedad política incapaz defender intereses respuesta preocupaciones presentación proyectola caída strache produjo año raíz difusión vídeo negociaba contratos sugería líneas financiación ilegal partido supuesta oligarca rusa imágenes tomaron mayo ibiza isla pasa años vacaciones escándalo supuso grabación abrió fractura coalición gobierno populares övp líder canciller sebastian kurz puso cortafuego escándalo perder cuestión confianza votos fpö austria manos equipo tecnócratas celebración elecciones kurz ganó legislatura eligió socio gobierno verdesstrache anunció retirada política octubre año intentos volver intermitentes previo formación movimiento strache fundó partido alianza austria daö grupo políticos disidentes fpö formación puerto añada siglas sello personallas circunstancias distintas pandemia coronavirus servir abono populismo comparecencia prensa strache apelado precisamente miedo votantes perder riesgo caer pobreza decisión gobierno cerrar fronteras correcta decisión reiniciar actividad económica llegado apoyos previstos afectados insuficientes subrayóstrache concurrirá partido madre línea pasos dados líder histórico populismo derechas austríaco fallecido jörg heider fundador fpö heider llevó fpö gobierno intrigas internas partido provocaron salida fundó alianza futuro austria bzöel anuncio regreso strache política provocado tipo reacciones incluida burla especialmente nombre elegido movimiento aspira posicionarse política nacional equipo strache recuerda equipo stronach tuiteó periodista orf armin wolf aludiendo proyecto político corta duración magnate negocios frank stronach austria strache nuevamente pletórico periodista julia ortner fascinante</t>
+          <t>real sociedad cita historia natalia arroyo viajado múnich difícil misión remontar partido ida conjunto donostiarra compitió gol lea schüller descanso suficiente bávaras llevaran pequeña ventaja reale arena derrota competitividad demostrada conjunto txuriurdin clave duelo siga abierto encuentro vuelta contagiar ilusión afición donostiarrauna pequeña ventaja contará conjunto natalia arroyo descanso bayern jugó domingo donostiarras sábado frente betis pudieron repetir triunfo jornada villarreal centrocampista portuguesa andreia jacinto autora empate amaiur sarriegi marcado temporada delantera suplente partido ida apunta titular liderará ataque fiel escudera nerea eizagirre empezado temporada nivelelene lete iris arnaiz reciente campeona mundo sub ana tejada completan equipo fuerte grupo precisamente central cree remontada muchísimas ganas ilusión afrontar partido múnich creemos posibilidades declaró entrevista as faltó encuentro ida gol faltó poquito acierto sacado conclusión marcarlas efectivas contundentes gracias seguramente podamos llevarnos eliminatoria ganas remontadaaunque conseguirlo deberán superar bayern schüller bühl principales bazas ofensivas anotar encuentro liga werder bremen conjunto bávaro marcha bundesliga puntos real sociedad partidos empate jornada frente eintracht frankfurt parten favoritas noruego alexander straus banquillo buscarán seguir sumando experiencia máxima competición europea temporada cayeron cuartos psg global factor sorpresa ilusión ganas dejar huella europa clasificándose fase grupos principales armas real sociedad seguir historia</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Deportes_30.txt</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1428,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>parlamento indonesia aprobó martes polémica reforma código penal retroceder nación sudeste asiático millones habitantes décadas derechos alcanzados materias libertades sexual religiosa expresión reforma amplia historia archipiélago mundo islas incluye artículos prohíbe sexo extramarital cohabitación parejas casadas apostasía difamación dirigentes recorte libertades promovido presidente joko widodo llega país mandatario recibieran amplio reconocimiento internacional organización cumbre celebró noviembre baliel código aplicará indonesios extranjeros aprobado apoyo partidos políticos temores legislación ahuyente turistas paradisíacas costas tropicales perjudique inversiones decenas ong grupos civiles salido calles denunciar cambios informa prensa localhan años espera declaró viceministro derecho derechos humanos edward omar sharief cámara representantes votase unanimidad favor código penal entrará vigor permitir redacten reglamentos aplicación presidente comisión parlamentaria encargada revisión texto bambang wuryanto código antiguo vestigio dominación colonial holandesa cabidaentre cláusulas morales criticadas figuran pena año prisión practicar sexo matrimonio cualquiera formas castigo meses cárcel parejas viven juntas casarse indonesia país población musulmana grande planeta tradición liberal prohíbe adulterio relaciones prematrimoniales velo hiyab obligatorio escuelasalbert aries portavoz ministerio justicia declarado denunciar padre cónyuge hijo presuntos infractores regulaciones morales objetivo proteger institución matrimonio valores indonesios protege intimidad comunidad niega terceros derecho denunciar asunto jueces nombre moralidad afirmóactivistas sostienen carteles manifestación código penal indonesia martes yakarta carteles lee rechazad reforma código penal código penal amordaza libertad prensa activistas sostienen carteles manifestación código penal indonesia martes yakarta carteles lee rechazad reforma código penal código penal amordaza libertad prensaslamet riyadi apúnete país seguir actualidad leer límitesgrupos favor derechos humanos afirman leyes afectan forma desproporcionada mujeres personas lgtbi minorías étnicas país phil robertson director adjunto asia organización proderechos humanos human rights watch denunciado twitter paso indonesia propone avanzar senda desastre violación derechos penalizar relaciones sexuales matrimonio escandalosa propuesta código penal viola normas internacionales derechos privacidad dañará gravemente paísotros cambios legales críticos socavan libertades civiles democracia planeta condena meses años rejas atentar dignidad presidente vicepresidente insultar instituciones ilegalización apostasía pena años cárcel propagar noticias falsas prohibición difundir opiniones contrarias ideología organizar protestas notificación previaen respuesta críticas vienen resonando semana ministro derecho derechos humanos yasonna laoly expuso martes legisladores fácil país multicultural multiétnico elaborar código penal acomodar interesesel gobierno indonesio llevaba décadas discutiendo revisión código penal enormes protestas anunciarse reelección joko widodo vencedor comicios presidenciales abril detuvieron aprobación norma legisladores tratado suavizar disposiciones widodo instado parlamento aprobar proyecto ley año caldee clima político cara elecciones presidenciales previstas principios martes periódicos nacionales condenado editoriales leyes diario koran tempo sostiene código tintes autoritarios jakarta post expresa profunda preocupación futura aplicación textodesde industria turística mostrado rechazo ley llega economía turismo empieza recuperarse pandemia maulana yusran subsecretario asociación turística país código totalmente contraproducente lamenta gobierno cerrado ojos cita reuters estallido crisis sanitaria indonesia especialmente isla bali intentado atraer nómadas digitales establezcan costas ofreciendo visado flexible espera alcancen niveles turismo anteriores pandemia millones visitantes bali</t>
+          <t>epidemias siglo obesidad considerada enfermedad mermando salud millones personas planeta motivo investigaciones centran luchar afecta países ricos países pobres estadounidense constata ratones ingesta moderada café té ayudar prevenir proteger hígado acumulación grasa conoce hígado grasoaunque mensajes lucha obesidad simples ejercicio dieta sana número personas sobrepeso obesidad aumentando país mujeres hombres obesos estima población hígado graso sigan buscando soluciones problema dispara tensión arterial ictus diabetesalgunas investigaciones tema centran precisamente prevenir aparición hígado graso conocido esteatosis hepática alcohólica vinculado riesgo diabetes procesos inflamatorios crónicos hígado derivar cirrosis cáncerun equipo internacional investigadores liderados paul yen rohit sinha universidad duke eeuu llevado cabo diversos experimentos cultivos celulares ratones comprobar reaccionaban presencia cafeína grasas almacenadas células hepáticas roedores alimentados dieta rica grasasegún datos experimentos publicados revista hepatology consumo equivalente tazas café té diarias beneficioso prevenir frente progresión hígado grasoeste estudio ofrece mecanismo detallado acción cafeína lípidos hígado resultados interesantes explica comunicado yen café té consumen frecuencia idea puedan terapéuticos especialmente ido ganándose reputación malos salud especialmente reveladora señalaestos investigadores señalan estudio datos conducir desarrollo fármacos actúen cafeína propiedades terapéuticas efectos habituales servir punto partida estudios evalúen beneficios cafeina cuerpo humanode actualidad marcha estudios efecto cafeína cuyos datos acaban publicar muestran moderación virtud señalan personas superan tazas café riesgo muerte problemas cardiovascularesen cambio mantenemos ingesta prudente sustancia efectos positivos variados protección frente hígado graso investigaciones evidenciado papel protector diabetes síntomas parkinson aliado memoria bondades té bebida alcanzaría galardones café observado reduce colesterol malo protección cardiovascular</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Salud_31.txt</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -1166,11 +1446,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>explosiones golpearon simultáneamente madrugada domingo lunes aeródromos militares rusos situados cientos kilómetros ucrania muertos heridos cobra fuerza hipótesis ataque medios locales apuntan dron estalló instalaciones desplegados bombarderos estratégicos fuerzas aéreas rusas ministerio defensa ruso responsabilizó lunes ucrania ataque autoría confirmada alto funcionario ucranio declaraciones diario estadounidense the new york times asegurado drones país bombardearon aeródromos rusos previamente mijailo podoliak asesor presidente ucranio volodímir zelenski insinuado twitter explosiones respondían operación especial kiev confirma oficialmente autoría ucrania trataría ataque suelo ruso alejado frontera inicio guerrael ministerio defensa ruso confirmó lunes ataque versión kiev lanzó bases drones baja altitud servicio aviones alcance moscú asegura proyectiles interceptados fragmentos producidos explosión provocaron daños insignificantes aviones información the new york times drones despegado territorio ucranio lograron destruir aviones rusos dañar máshoras conocerse explosiones provincias ucrania kiev sufrieron ataques misiles rusos muertos comunicado ministerio defensa recalcó ataque logró impedir posterior bombardeo masivo infraestructura ucrania moscú alcanzó objetivos misiles disparados tierra mar aire mando fuerzas aéreas ucranias logrado derribar proyectiles lanzados pasaban empresa estatal energética ukrenergo explosiones afectaron infraestructuras objetivos prioritarios ataques ejército ruso ministro ucranio denis shmihal concretó daños producido regiones kiev vinitsia odesael gobernador región rusa sarátov román busarguín telegram explosiones afectaron edificio civil quiero asegurarles producido emergencia zonas residenciales ciudad motivos preocuparse infraestructura civil resultó dañada escribió aeropuerto sarátov situado kilómetros ucrania medios rusos astra baza dron explotó pista base aérea engels región sarátov bombarderos estratégicos resultado dañados aeronaves forman fuerzas disuasión estratégica papel importante ataques misiles convencionales ucraniapor agencia ria novosti informado explosión aeródromo riazán situado kilómetros moscú fuentes personas muerto resultado heridas supuesta explosión camión combustibleantes diario estadounidense publicara información cita alto funcionario confirmó autoría ucrania ataque asesor presidente zelenski insinuado kiev ataques tierra redonda descubrimiento galileo kremlin estudiado astronomía preferencia astrólogos sabrían lanza espacio aéreo países objetos voladores desconocidos volverán punto partida escribió podoliak twitterla industria militar ucrania anunció domingo punto aparato tripulado capaz transportar carga explosiva kilogramos radio kilómetros probar éxito dron entorno guerra electrónica esperamos verlo combate prometimos finales año tratando cumplir promesas anunció jefa prensa conglomerado industrial militar ucranio ukroboronprom recoge agencia unianobjetivos prioritarioslos aeródromos militares rusos objetivos prioritarios fuerzas armadas ucranias agosto paso respuesta rusia bombardearon base aérea saki crimea pese kremlin amenazaba dura réplica acción península anexionada kiev podía incentivo atacar instalaciones sarátov semanario alemán der spiegel publicó semana presencia numerosos bombarderos estratégicos imágenes satélite base engels apuntaban preparación ataque escala ucraniapoco explosiones aeródromos riazán sarátov coincidiendo entrada vigor europeo petróleo ruso suministrado mar tope occidental precio rusia lanzó lunes andanada misiles territorio ucranio alarmas sonaron decenas ciudades ucranias incluida kiev lanzado misiles yuri ihnat portavoz fuerza aérea ucrania ignore alarmas advirtió ciudadanía andri yermak jefe gabinete presidencial ucraniolos misiles golpearon provincias peores consecuencias vivieron zaporiyia sudeste ucrania autoridades informaron muerte personas ataque afectó infraestructuras suministran electricidad kiev odesa vinitsia regiones sufrieron cortes luz agua odesa mikolaiv sur sumi norte ciudad natal presidente zelenski krivi rig estealgunos expertos rusos alertan explosión puente kerch península anexionada crimea retaguardia rusa voladura puente quedan instalaciones estratégicas rusia puedan considerarse absolutamente seguras asesinato daria dugina hija ideólogo kremlin alexander dugin decía redes sociales corresponsal guerra ruso alexánder kots ¿sarátov clandestinidad ucrania opera territorio ruso fuerzas especiales detienen agentes kiev regularmente flujo refugiados puedes seguimiento añadía kots advertir población acostumbrada vida tranquilaputin teme ataques puente crimeavladímir putin recorrido lunes reconstruido puente crimea meses destrucción parcial visita simbólica inicio invasión ucrania febrero presidente ruso visitado península anexionada forma ilegal importantes bases aéreas rusas sufrían explosiones cientos kilómetros frente mandatario advertía rusia reforzar control disputado sur ucrania proteger suministro península mar negro continuas amenazas expresadas oficialmente kiev posibles ataques puente putin enfatizado importancia vía terrestre conecta crimea resto rusia afirmado portavoz kremlin dmitri peskoval volante mercedes alemán marca abandonado país sanciones putin inauguró apertura carriles vehículos dañados fuerte explosión octubre obstante abiertos vehículos ligeros putin admitido apuntalados alcanzar perfecto prosigue reparación vías ferrocarril ruta clave enviar suministros fuerzas ejército desplegado sur ucrania putin tráfico debería volver operar mediados verano putin informado vice ministro marat jusnullin progreso obras restauración conversó obreros condujimos derecho entendido izquierdo puente condiciones operar falta terminarlo sufrió putin declaraciones recogidas agencia interfax vice ministro respondió tramo condiciones funcionar reforzado posteriores ataque indica pondremos condiciones reparación puente kerch visto afectada ¿las tormentas interfirieron preguntó putin jusnullin coche interfirieron fuerza tormentas respondió alto cargomoscú acusó ministerio defensa ucranio fuertes daños sufrió infraestructura kremlin convirtió símbolo conquista territorial años investigación sabotaje perpetrado compleja operación servicios especiales kiev colaboradores rusos ocultaron bomba camión carga explosivo enviado ciudad rusa armavir bulgaria armenia georgia introducido cargamento rollos película cuya entrega solicitó dirección falsa crimea gobierno ucranio confirmó autor ataque</t>
+          <t>david popovici bate récord libre natación destroza estigma bañadores prohibidosel rumano años establece marca segundos centésimas rápido logrado césar cielo bañador enterizo impermeablecaeleb dressel nadador rápido mundo bañador textil campeón mundial campeón olímpico naturalmente tratándose velocista unidos años apogeo junio mundiales budapest decidió retirarse competición alegando razones médicas especificadas justo constatar disputaría metros libre flaco pómulos salientes mirada brillante años largos semifinal segundos llamaba david popovicisi dressel huyó visión futuro inhóspito pareció razones faltaron futuro nado libre pertenecía tallo estatura inesperado extraño origen rumano previsible progresión sábado piscina foro itálico sede campeonatos europa natación popovici confirmó trayectoria devastadora anuncian marcas años ian thorpe convirtió campeón mundial prematuro tiempos años surgía nadador libre autoritario muchacho vida entrenándose club bucarest principales corrientes natación élite destrozó segundos récord mundial césar cielo enquistado memoria infausta bañadores flotantes poliuretanoexactamente siglo johnny weissmüller batiera plusmarca destino reservó círculo perfectamente irónico popovici convirtió hombre joven batir récord prueba legendaria natación localización carga simbólica piscina foro itálico viejos pinos escenario estableció récord precedente años atrás mundiales roma julio embutido mono goma ayudaba deslizarse superficie empleando fuerza sostenerle ocupaba tecnología césar cielo tocó pared gritó victorioso gloria brasil arena fabricante bañadores marca segundos acababa nacer parecía grabada piedra hombre rompiera debería nadar llevara incorporado artefacto flotador gamaprohibidos bañadores impermeables natación alumbró sobria espectacular armados bermuda tela agua fluía freno caeleb dressel australianos kyle chalmers cameron mcevoy intentaron éxito aproximarse territorio inhumano cielo dressel bajó segundos mundiales convirtieron hito rayo esperanza peregrinos avanzaban cumbre helada habitó cieloel salvajepopovici años mundiales carecía memoria complejos sintió inferior pecho desnudo cubierta entrepierna bermuda tela luciendo multitud pecho insinuante esternón desafiado húngaro kristof milak mariposista transformado librista debió encontrar aliciente sacan salvaje ganar oro budapest mes milak nadaba izquierda empujó terreno adrenalinamilak salió francés maxime grousset mandó prueba viraje segundos popovici tocó pared posición sesenta centésimas parcial cielo regreso inaudito popovici avanzó cuchillo agua ofrecer resistencia ofrecer superficie rozamiento rotando tronco clavando manos equilibrio perfecto falta metros traspasaba umbral ritmo récord mundo constituyen mayores hazañas historia deporte señal ominosa unidos australia potencias nado libre camino juegos parís</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Deportes_56.txt</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -1179,11 +1464,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>argentina pendiente fallo juicio presunta corrupción política poderosa argentina cristina fernández kirchner sentencia conocerá martes diciembre filtración prensa mensajes jueces políticos opositores empresarios medios elevado tensión previa chat publicado domingo medios locales participantes debaten difundir versión falsa contrarrestar denuncia dádivas vinculada viaje pagado realizaron patagonia octubre presidente argentino alberto fernández anunciado cadena nacional solicitará justicia investiguen penalmente hechos relacionados viaje financiación consejo magistratura abra sumario jueces implicadosel kirchnerismo exhibe conversación supuestamente obtenida hackers radiografía precisa podredumbre lawfare judicatura fines políticos palabras ministro justicia martín soria macrismo cambio montaje objetivo salvar kirchner esperan martes sentencia negativa llamada causa vialidadlos mensajes involucran juez julián ercolini cargo instrucción investigación cristina kirchner colegas pablo yadarola carlos mahiques pablo cayssials fiscal ciudad aires juan bautista mahiques ministro seguridad ciudad aires marcelo dalessandro directivos grupo clarín chats publicados diario argentino portal web cohete luna hackeo línea teléfono celular implicados origen ilegal fuente impide puedan usados prueba justicialos participantes chat telegram muestran preocupados publicación diario página viaje pagado realizaron octubre avión privado bariloche alojarse par noches estancia multimillonario inglés joe lewis lago escondido lewis cercano expresidente mauricio macri estancia vieja conocida argentinos decisión empresario bloquear turistas ingresos lago intercambio involucrados analizan responder periodistas llaman confirmar viaje debaten distintas estrategias pasar viaje escapada conjunta pagaron bolsillopodríamos averiguar tema facturita comprobante pago lago escondido escucha mensaje voz juan bautista mahiques fiscal ciudad aires cayssals propone pagar avión quedaron casa amigo ercolini pregunta fácil facture lago escondido noches media pensión carajo inventar insiste ercolini mensajes filtrados coincide necesidad mantener llave fotos sacaron travesíalos participantes burlan critican periodistas contactan alardean responderles llamar directivos medios frenar difusión noticia principal blanco críticas policía seguridad aeroportuaria psa consideran origen filtración planilla viaje avión octubre tocará ministro nación disolver psa escribe dalessandro cargo cartera seguridad ciudad airesdesmentida clarínsegún medios publicaron noticia viaje financiado directivos grupo clarín versión conglomerado medios niega fuentes grupo clarín advierten contenidos chat totalmente truchos falsos adulterados procedencia ilegalel escándalo derivó doble denuncia consejo magistratura presunto desempeño funciones jueces fiscales presuntamente involucrados justicia bariloche supuesta violación deberes funcionario público admisión dádivas tráfico influenciasla filtración vuelto dividir argentina previas conozca sentencia juicio kirchner vicepresidenta acusada delitos asociación ilícita defraudación adjudicación centenar obras públicas provincia patagónica santa cruz mandatos presidenta kirchneristas sostienen mensajes evidencian connivencia judicial oposición vicepresidenta antikirchneristas operación espionaje ilegal orquestrada brazada ahogado sentenciala polémica creció llegar alto casa rosada alberto fernández convocó cadena nacional queda expuesta enorme contundencia corporaciones operan funcionarios jueces fiscales procurando favores casos buscan ventajas indebidas simplemente propician persecución enfrentan fernández pidió justicia investiguelos legisladores coalición gobernante frente pedido comunicado conjunto desempeño funciones comisión delitos graves escandalosas inconductas éticas confesas exigimos inmediata regularización institucional consejo magistratura paralizado accionar inocente corte suprema justicia renuncia funcionarios públicos involucrados seria profunda investigación señalan texto legisladores afirman público conocimiento magistrados fiscales manejan margen ley verlo escucharlo voz excede imaginadodesde alianza opositora juntos cambio provienen políticos involucrados voces media salido defender ministro seguridad porteño primeras presidenta propuesta republicana pro patricia bullrich filtración forma intentos desesperados kirchnerismo eludir justiciala hipótesis bullrich coincide dalessandro acusado redes kirchnerismo financiar impuestos operación tragicómica inteligencia salvar jefa kirchner equipo dalessandro contactado diario respondió consultasla filtración empeora imagen judicial argentina relación política juez federal prefiere mantener nombre reserva opinó sucedido gravísimo vergüenza impunidad manejan verduguean periodistas quedar jueces presidente cámara federal casación penal alejandro slokar máxima autoridad judicial corte suprema judicial vive crisis radical pidió tomar medidassuscríbase newsletter país américa reciba claves informativas actualidad región</t>
+          <t>junts per catalunya entregado miércoles govern generalitat reunión presupuestos documento demandas negociar cuentas generalitat anunciaron semanas bases negociación presupuesto propuesta seria rigurosa pensada sesgo ideológico necesidades país apuntado secretario formación jordi turull atención medios insistimos fiscalidad justa añadido líder jxcatla formación articulado propuesta ejes –desarrollo económico derechos cohesión social equidad seguridad catalán lengua cultura medios comunicación equilibrio territorial soberanía nacional– medidas destacadas ámbito fiscalidad educación seguridad medidas paliar inflación fiscalidadasí junts aboga deflactar irpf tramos paliar efectos inflación desbocada revisar reducir impuesto sucesiones forma progresiva vuelva niveles bonificación adquisiciones debidas muerte familiar grado padres hermanos hijossi deflacta irpf aumento fiscal encubierto ingresos adicionales administraciones inflación acabará año subidas salariales llegarán nivel contabilizamos subida media piden media organizaciones sindicales puedes saltar tramo deflacta perder adquisitivo apuntan fuentes jxcatninguna medida élites conjunto familias paísjunts apuesta bajar irpf tramo rentas bajas tributen catalunya territorios incrementar mínimos personales familiares irpf inflación medida protección fiscal sucesión empresas familiares permitir continuidad llegando bonificar toca mínimo exento personal familiar acabas pagando impuestos comunidades previsto añaden fuentes consultadasal incluye propuesta fiscal modificación impuesto patrimonio barajado posibilidad subir mínimo exento niveles euros actuales personas lleguen extranjero pagar patrimonio acumulado llegar catalunya compromiso permanencia adquisición vivienda circunstancias similares formación facilitar descartado punto afecta ciudadanos pedimos luna aseguran junts medida élites conjunto familias país sostienen formaciónescuela concertada actualización módulosotras propuestas destacadas ámbito educación jxcat pide actualizar incrementar precio módulos escuela concertada revertir presupuestariamente infrafinanciación escuela concertada perjuicio escuela pública pública preparada quite escuela concertada favor mejorar escuela pública fraguando problema concertada prejuicios ideológicos lamentan posconvergentes incluyen garantizar universalidad gratuidad concertación plazas seguridad ocupaciones delincuencialesen materia seguridad formación reclama crear unidad mossos desquadra especializada ocupaciones delincuenciales materia partido viene insistiendo semanas extitulares justícia drets socials lourdes ciuró violant cervera impulsado cambios código civil catalán vecinos administraciones locales pudieran denunciar casos propietarios casos tenedores actúan sanidaden materia sanidad apuesta incremento presupuestario millones euros años destinar presupuesto sanidad reforzar atención primaria incrementar partidas destinadas salud mental avanzar agència integrada social sanitària previsto exconseller josep maria argimon exconsellera cervera asimismo pide compromiso avanzar dilaciones proyecto hard rock aprobar plan desarrollo urbanístico acabe año previsto ejecuten inversiones necesarias creación incaoli institut català loli completar despliegue fibra óptica territorio catalán propuesta seria rigurosa pensada sesgo ideológico necesidades jordi turullsecretario junts per catalunyaen apartado reclama departamentos govern trabaje mentalidad trabaje reducir dependencia figura propuesta incremento millones euros fomento impulso catalánno líneas rojas aceptan medidas advierten junts asegura jugarán dilatar tiempos negociación govern pere aragonès acelerado negociación grupos reunió psc perfila socio probable ritmo espera ejecutivo catalán comunes peso parlament reunido ocasiones govern apoyo concurso socialistas posconvergentes insuficiente</t>
         </is>
       </c>
       <c r="C58" t="n">
         <v>2</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Politica_21.txt</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -1192,11 +1482,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>caminar pandillero recomiendo policía anda tatuado voz queda eva mujer años habitante montreal populosa colonia área metropolitana san salvador gobierno nayib bukele instauró régimen excepción salvador meses habitantes montreal histórico bastión mara salvatrucha ms miedo pandilleros cambio temen policía ejército sitiado multitud comunidades paísaquí policías soldados absoluto cualquiera cae vuelto pandilla insiste eva sentada viejo sillón pequeña sala casa observa reojo puerta vigilando escuche conversación eva pide revelar nombre completo seguridad acompañan esposo madre hijos pequeños vecinas reunido contar vive lugarhasta años entrar montreal desconocido temeridad dimensionarlo vendetta ms barrio controlaba colonia terminó asesinato personas murieron quemadas microbús transporte colectivo regresaban trabajarahora calles colonia ven pandilleros atuendos holgados tatuajes rostro armas cinto ve caminando mujeres comprando pequeña tienda regresan traer hijos escuela patrullas policías soldados rostro cubierto pasean escaneando mirada transeúntes detienen hombre joven pasahace meses llevaron yerno jorge erazo años joven trabajador estudiante tercer año licenciatura administración empresas papá llamaba conductor buseta quemaron pandilleros ″ ana vecinas reunidas salalo sucede montreal único salvador meses régimen excepción mara salvatrucha estructura criminal grande país languidece medidas presidente bukele cuestionadas autoritarismo personas detenidas miles denuncias arrestos ilegales casos torturas desplazamiento forzado causado policía ejército asesinatos prisiones gobierno país centroamericano acerca objetivo vencer pandillas costa suspensión libertades derechos constitucionales violaciones derechos humanos informe amnistía internacional publicado principios junio sitio decretado bukele desembocado violaciones masivas derechos humanos detenciones arbitrarias miércoles human rights watch hrw organización salvadoreña cristosal previsto presentar informe conjunto documenta graves abusos incluyendo desapariciones forzadas torturas malos tratosentre septiembre noviembre país habló empresarios transporte colectivo líderes mercados investigadores policiales fiscal antipandillas visitó comunidades área metropolitana san salvador históricamente controladas ms analizar resultados mediano plazo régimen excepción apunta ms huesos miembros policía ejército ocupado vacío dedican denuncias cometer delitosaunque aplicar ecuación comunidades país resultado desplazamiento ms perdido fuerza medida actividades vitales extorsión control territorial capacidad reclutamiento integrantes vinieron policías soldados capturaron mundo vinieron camiones quisieran dejar llevaron pandilleros llevaron montón gente inocente continúa evasegún lugareños consultados reportaje montreal sufrido éxodo pandilleros huyeron autoridad habitantes vínculos pandillas huir país policía amenazara encarcelarlos colaboraban ofrecían informacióny miedo desaparecido montreal comunidades visitadas periódico vecinos siguen obedeciendo normas establecidas pandillas recibir visitas familiares vengan zonas pandilla contraria hablar policías soplón vea ahorita pandilla ojos oídos lados salir cárcel explica anael marzo bukele emprendió embestida grande gobierno lanzado pandillas ms barrio medida práctica significado sistemática violación derechos humanos organizaciones humanitarias impuesta estructuras criminales masacraran personas semana supuestamente consecuencia ruptura pacto secreto gobierno mantenía investigaciones periodísticas ejecutivo niega secretoaquella matanza significó golpe administración bukele jactaba mundo control pandillas gobierno salvadoreño logrado organismos nacionales internacionales comité tortura onu señalado graves violaciones derechos humanos régimen excepción bukele gabinete desechan argumentando país eventos públicos masivos reciente concierto bad bunny medida despliegue policías militares cercar territorios ciudades país operativo empezó sábado municipio soyapango área metropolitana san salvador principios abril presidente número pandilleros ascendía encarceladoslas prácticas negociación embestida pandillas gobierno bukele salvador mandato expresidente francisco flores gobiernos dedicado reprimir negociar grupos logrado fortalecerlos expertos tema coinciden diferencia radical concentración control sistema justicia persona presidenteun pandilleros salir salir sed venganzados empresarios transporte colectivo aceptaron hablar país explicar drástica reducción cobro extorsión sector explicaron condición proteger identidad mediados década años noventa cubren rutas circulan área metropolitana san salvador pertenecen organizaciones gremiales transportistas país llevan década pagando extorsión pandillas ms barrio pago extorsión mes pague empresarios decirlo empezó régimen excepción pago prosigue coinciden meses extorsión transporte colectivo reducido calculan datos difieren expresados representante mesa nacional transporte calculó reducción agosto pasadoes mentira dejado pagar rutas pagamos dólares euros mensuales ms asegura empresarios muestra teléfono conversaciones whatsapp coordina pandillero entrega extorsión fe compañeros siguen pagando siguen pagando añadedatos mesa nacional transporte señalan transportistas pagaron millones dólares pandillas año crisis pandemia covid obligó cerrar economía país monto redujo millonesambos empresarios aseguraron transportistas dejado pagar extorsión razones principales pandillas perdido capacidad cobrarla menor control territorio pagar considerado delito empresario ruta ab acusado testaferro pandilla seguía pagando extorsión policía tomó financista víctima extorsión delito relata continúan pagando miedo pandilleros salgan prisión salir salir sed venganza afirma unoaunque ms diversificado fuentes ingresos incursionando droga lavado dinero extorsión principal fuente financiación vital práctica ms punto tratado negociaciones gobiernos país década negociaciones pandilla dejado matar extorsionarmiembros fuerza aramada salvador patrullan comubnidades reparto guadalupe campanera municipio soyapangomiembros fuerza aramada salvador patrullan comubnidades reparto guadalupe campanera municipio soyapangovíctor peñaun informe organización crisis group publicado estimó monto global extorsión salvador rondaba millones dólares año equivalente producto interno bruto pib enorme cantidad pandillas salvador siguen mafia pobresotro sectores extorsión reducida drásticamente comercio informal mercados país consultó líderes principales gremiales vendedores centro san salvador corazón comercio informal capital recorridos mercados ciudad conversaciones vendedores mayoría dejado pagar atrevo extorsión bajado comparación régimen excepción asegura líderes vendedores consultadosun estudio naciones unidas publicado junio señala vendedores ambulantes repartidores productos pagaban millones dólares concepto peaje pandillas noviembre entrevista noticiero local ministro justicia seguridad gustavo villatoro extorsión reducido nivel nacionalla bestia herida muerteun investigador policía fiscal investiga diez años negocios ms salvador aceptaron hablar principios noviembre país condición anonimato coinciden capacidad reclutamiento control territorial economía criminal pandilla punto críticola bestia herida muerte ahorita señal diga cambiar investigador policial bestia agente formas nombrar ms usada pandilleros investigador dedica años combatirla ms perdido capacidad controlar territorio reclutar miembrosahorita comiendo mierda extorsionar robar controlar negocios lavan dinero empresa formal rato ms quebrada fiscal hundimiento costando salvador profundos retrocesos libertades derechos bukele ganando guerra denuncias costa violar ley</t>
+          <t>max verstappen consiguió domingo octava victoria temporada fórmula cantidad triunfo logrado circuito américas encabeza lista favoritos helmut marko asesor deportivo red bull racingla victoria austin absolutamente mejores carreras visto max comenzó marko entrevista exclusiva motorsportcom países bajosal principio significativamente rápidos mercedes neumáticos medios hamilton pudimos convertir ventaja ganancias neumáticos duros mercedes realmente rápidospor marko alaba verstappen marcara diferencia fase complicada carrera ronda pits lograron undercut adelantar detención piloto campeón mundo sencillodespués parada max salió rápido resultado neumáticos evaporaron parada aprendió claramente max frenó deliberadamente curvas marko movimiento calificó gestióncomo resultado hamilton acercó max pusiera nervioso hamilton segundos max volvió acelerar vuelta mercedes vio posibilidad jugado nosotrosese juego recordó marko victoria verstappen fórmula circuit barcelonacatalunya apuntó viejas características presentes austinexactamente combinación gestión velocidad ahorro neumáticos demostró barcelona gusta comparar victoria aquellala comparación válida razón españa verstappen concentró puntos clave circuito austin mayo atacó sector texas enfocándose curva zona drs hamilton llegar curvas sverstappen formaun aspecto impresionó marko cooperación verstappen estrategia cabina dividiendo labor conducción ayudar planificación personas situadas muro boxeseso extraordinario modos pensábamos meter sergio pérez pits directamente hamilton pudiera continuar mensaje max radio miren háganlo demuestra queda capacidad pensar estrategia carrerasmarko aplauso extra verstappen sentía domingo sucedió pérez presentó malestar estomacal previo competenciano completamente forma desmayó ejercicios respiración líquido consiguió superarlo bajó coche victoria diría inestable pies choque silverstone compara austriaco años impacto fuerzas sufrido colisión lewis hamiltonlos esfuerzos verstappen recompensa puntos rival campeonato carreras concluir temporada</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Deportes_4.txt</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -1205,11 +1500,16 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>mes luiz inácio lula silva arranque tercer mandato presidente brasil anunciado nombre futuro gobierno siquiera persona llevará riendas economía principal desafío presidente electo encabeza coalición decena partidos semana brasilia inmerso carrusel contactos misión apremiante negociar socios composición gobierno congreso permita sortear techo gasto cumplir principal promesa electoral millones pobres compatriotas sigan recibiendo paga mensual reales dólares euroslula desvelará gobierno diciembre explicado viernes prensa capital brasilia ceremonia tribunal superior electoral formalizará definitivamente triunfo logrado octubre ministerios cabeza querido recordar ganó proyecto amplio derrotar bolsonaro gobierno fuerzas apoyaron lograr victoriauno principales mantras izquierdista campaña pobres volverán presupuesto políticas sociales prioridad mandatos cuentas públicas situación precaria lula necesita fondos cumplir necesitados muchísimos brasileños pasa hambre tercio vive pobreza extrema pobrezael partido trabajadores pt presentó semana propuesta legislativa pretende dejar límite impone techo gasto partida gigantesca años dura mandato presidencial cifra propuesta millones reales millones dólares destinados mantener paga mensual pobres espero señorías sensibilidad lula falta llegar negociar congreso elegido bolsonarismo principio mayoría duda cobrará caro lula apoyo necesita plazos apremian toma posesión prevista año nuevoel nombre suena ministerio haciend fernando haddad candidato presidencial pt líder encarcelado ministro alcalde são paulo mercados recibido disgusto pérdidas quejas presidente electo corsé supone techo gasto preferían duda alguien liberal asumir riendas principal economía américa latina trimestre creció soló simultáneamente inflación desempleo moderandocuadrar sudoku ministerios infierno lula necesita satisfacer múltiples intereses partido pt corrientes ideológicas decena formaciones abrazaron liderazgo misión salvaguardar democracia brasileña logró apoyo antiguos adversarios situados derecha izquierda representación territorial brasil clave promesas futuro gobierno ministras negros indígenas reflejo dificultades conciliar tantas demandas lula avisado viernes iba ministerio pueblos originarios queda secretaría dependiente presidenciael único respiro apretada agenda política mundial compatriotas pierde partido enfunda camiseta amarilla izquierdistas dejaron medida convertía símbolo bolsonarista presidente electo confesado reciente operación garganta callado insistido ayuda divina curarme comentadola ayuda mensual cubrir necesidades acuciantes pobres basa antiguo bolsa familia programa aplaudido eficaz barato símbolo políticas progresistas pt llegar presidente jair bolsonaro rebautizó auxilio brasil quería arrebatarle izquierda potente marca electoral pandemia subió cuantía amplió cifra beneficiarios convirtió principales reclamos electorales realidad mantener paga reales promesa electoral bolsonaro lula único punto coincidencia visiones antagónicas extremoen tiempos pt cuantía bolsa familia tercio actual lula asumió inicio campaña podía tocar reales pretende retomar requisitos eliminados bolsonaro garantizar niños familias incluidas escuela vacunados embarazadas someten chequeos médicosbolsonaro logró fondos pagar ayuda diciembre mandato maniobra congreso renovó declaración emergencia pandemia amainado quedara excepciones contempladas saltarse límites constitucionales gasto público bolsonaro concurrir comicios auxilio brasil gancho atraer pobres insuficiente lula ganó millones votos</t>
+          <t>organización nacional trasplantes ont puso marcha programa pacientes recibido trasplante renal cruzado llevamos año cifra duplica año efectuaron trasplantes tipo cuadruplica datos ont demuestran creciente aceptación pacientes familiares nefrólogos urólogos inmunólogos modalidad trasplante renal participan hospitales españa laboratorios histocompatibilidad basada intercambio órganos donantes vivo parejas objetivo ofrecer pacientes insuficiencia renal crónica posibilidad recibir injerto gracias generosidad pareja compatibleempezamos programa múltiples problemas reconoce elmundoes director organización nacional trasplantes ont rafael matesanzlos cruces requerían traslado donantes ciudad problemas logísticos conlleva agrega viaja donante riñón programa consolidado sirve estímulo donaciones renales vivo años desarrolladas suponen trasplantes vivo objetivo llegar modalidad terapéutica desarrollado países elevada actividad trasplante renal donante vivo caso corea sur holanda reino unido australia canadá unidos llevan realizando tipo trasplantes década excelentes resultadosel técnicas quirúrgicas invasivas estudio cuidado donante intervención permitido potenciar tipo trasplantes posibles complicaciones donante disminuido considerablemente actualidad extracción renal vivo procedimiento riesgoen país trasplante renal cruzado intercambio parejas intervenidas país vasco cataluña donantes receptores dados alta encuentran perfecto saludeste tipo trasplantes conlleva complicado proceso logístico requiere colaboración oficina central ont coordinadores autonómicos trasplantes hospitales equipos médicos participan operativo</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Salud_21.txt</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -1218,11 +1518,16 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>presidente chino xi jinping rindió martes homenaje público exlíder recién fallecido jiang zemin asegurar supervivencia partido comunista chino pcch tormentas políticas marcaron etapa gobierno acciones modernizar economía nacionaljiang falleció miércoles shanghái años problemas salud logros frente país años noventa figuran sacar china aislamiento diplomático sometió masacre tiananmen enmendar relaciones unidos supervisar crecimiento económico precedentes sentaron bases convertir china potencia mundial hoychinajiang zemin falleció miércoles shanghái años problemas saludel adiós salón pueblo plaza tiananmen precedido minutos silencio siguieron segundos sonaron sirenas bocinas pekín ciudades chinasal tomar palabra xi describió finado prestigioso líder marxista diplomático guerrero comunista lideró país eta desafíos precedentes referencia parcial protestas tiananmen jiang accedió poderhorizontalciudadanos chinos depositan flores homenaje líder fallecido hector retamal afpa finales años ochena principios noventa serias tormentas políticas país extranjero socialismo mundial experimentó graves complicaciones élite política país congregada sala vestida riguroso negro mascarillael actual presidente subrayó persistencia jiang hora seguir proceso apertura reforma auspiciado antecesor deng xiaoping elogió supervisar mandato vuelta soberanía china antiguas colonias británica portuguesa hong kong macao asimismo apuntó visión fallecido país próspero liderazgo hora lograr china ingresase organización mundial comercio chinaxi elogió liderazgo jiang lograr china ingresase organización mundial comercioxi elaboró discurso retrato jiang instalado tribuna situadas cenizas antiguo presidente cubiertas bandera hoz martillo carteles dispuestos sala leían eslóganes amado partido ejército etnias pueblo chino camarada jinag zemin vivirá siempreel cuerpo jiang incinerado lunes acto celebrado cementerio capitalino babaoshan descansan restos numerosos líderes revolucionarios pcch presente sucesor cargo predecesor xi hu jintao cuya inesperada salida forzada xx congreso partido comunista octubre despertó rumores purga públicahorizontalel palacio pueblo celebró acto amaneció martes rodeado fuertes medidas seguridad noel celis afpdurante jornada páginas web medios estatales instituciones tiñeron blanco negro banderas ondearon media asta bolsas shanghái shenzhen cerraron minutos comos señal homenajecon recuerdo fresco recientes protestas políticas anticovid semana fuerzas seguridad reforzaron presencia calles garantizar reprodujeran concentraciones públicas autorización vano muerte jiang provocado ola nostalgia población percibe frente relativa liberalidad comparación actualhorizontalciudadanos chinos siguen vivo discurso presidente xi jinping acto despedida fallecido jiang zemin andy wong apaún numerosas sombras pesan legado jiang mandato evidenció graves desequilibrios modelo crecimiento costa auge explosivo desigualdades sociales daños medioambientales altos índices corrupción pesan espaldas campañas activistas tibetanos miembros organización religiosa falun gongdurante jiang consiguió tejer poderosa red influencias base feudo shanghái alcanzó segmentos país economía ejército remanentes erradicados xx congreso pcch manos xi década frente arrinconado facciones rivales concentrado persona finiquitado modelo gobierno aupó jiang</t>
+          <t>igualdad concepto términos generales positivo enfermedad cambios hábitos vida incorporación mujer consumo sustancias tóxicas igualdad extienda problemas típicos varón ictus conocido accidente cerebrovascular generando discapacidad planetadesde sustancias presentes cigarrillos tóxicas generan problemas relacionado pulmón cáncer insuficiencia respiratoria corazón tabaquismo aumenta riesgo sufrir ataque cardiacopero tabaco afecta órganos acción allá realidad tejido arteria pasen sustancias nocivas resultar dañado arterias riegan cerebro inmunes peligrolo ocurre tabaco arterias fomenta acumulación residuos denominados genéricamente placa ateromatosa placa estrechando calibre vaso sanguíneo pudiendo llegar cerrarse completamente circunstancias destruirse formar trombo desplazando torrente sanguíneo llega vaso pequeño cerebro produciendo obstrucciónen caso genera llamado ictus isquémico falta circulación zona cerebro muerte tejido derivar graves secuelas parálisis incapacidad hablar tipo ictus denominado hemorrágico genera similar grave supone rotura arteria hemorragia daños ampliossegún expertos españoles sufrirá ictus vida apunta estudio cuyos datos acaban publicar revista stroke mujeres fumadoras riesgo hombres fuman sufrir episodio tipo probabilidad menor mujeres consumen tabacotras analizar datos estudios internacionales ictus publicados investigadores universidad queensland brisbane australia encontraron tabaquismo relacionado riesgo sufrir ictus isquémico hombres mujeres</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Salud_30.txt</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -1231,11 +1536,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>pasa desapercibido frente problemas salud vih importante amenaza salud pública europa demuestra informe elaborado conjunto centro europeo prevención control enfermedades ecdc oficina europea organización mundial salud omsla fotografía arroja informe cambia función continente aumentando número personas viven vih diagnosticar restringe foco unión europea situación esperanzadoraa pasa desapercibido frente problemas salud vih importante amenaza salud pública europa demuestra informe elaborado conjunto centro europeo prevención control enfermedades ecdc oficina europea organización mundial salud omsla fotografía arroja informe cambia función continente aumentando número personas viven vih diagnosticar restringe foco unión europea situación esperanzadoraen cambio fronteras ue tendencia global invierte muestran datos década diagnósticos ligeramente frecuentes infecciones significa cantidad personas vive vih saberlo disminuido años estima personas vih ue diagnosticarsi realizan test forma regular personas riesgo generarse periodo infección diagnóstico beneficia persona posibilidades desarrollar enfermedad grave muerte diagnostica salud pública personas seropositivas transmitir vih parejas sexuales saberlo subrayado ammonen informe indica mitad diagnósticos vih realizados recuento células cd menor células milímetro cúbico sangre diagnóstico indica llevaban años conviviendo infecciónhay necesidad crucial aumentar testeo detección señala informe reclama estrategias mejorar diagnóstico concienciar población necesidad someterse pruebasen vías transmisión datos informe relaciones hombres mantienen sexo hombres vía común transmisión unión europea transmisión heterosexual drogas inyectables frecuente regióndurante décadas diagnosticado millones casos región europea oms unión europeaen años transmisión heterosexual disminuido considerablemente unión europea occidente años especialmente mujeres número casos debidos relaciones sexuales hombres determinados países ue occidente transmisión drogas inyectables disminuido constantemente alta europa</t>
+          <t>salma paralluelo vivió montaña rusa emociones domingo civitas metropolitano aragonesa joyas cantera española fichó verano barcelona definitivamente pasión atletismo difícil decisión apostar deporte dando alegrías campeona mundo sub profesional años andadura azulgrana empezó altibajoslas lesiones impedido continuidad octubre levante debutar azulgrana noviembre marcó gol jugadora barcelona levante planas progresión importante llegando titular frente conjunto catalán alavés ganado confianza ausencia jugadoras importantes mariona hansen protagonismo domingo giráldez puso titular salió onces oficiales raro pasaba salieron calentar doce jugadoras crnogorcevic partía once salma retiró barcelona anunció aragonesa crnogorcevic saliese inicio hacía indicar salma lesionadola joven extremo salió banquillo lágrimas contener rabia emoción titular duelo altos vuelos estadio civitas metropolitano asisat oshoala intentaba consolar joven futbolista relato efecto minuto salma saltó campo descartando lesión minutos césped cuarto encuentro minutos recogió rechace lola gallardo penalti lanzó mariona quinto particular celebración podía oshoala minutos salma actuó posición nueve abrazo agradecimiento palabras banquillo aragonesa podía contener lágrimasha problema logístico entrar detalle cambio hora jonatan giráldez rueda prensa posterior ausencia salma once anunciar titular desveló razones jugado abierta banda derecha normalmente diestras juegan ana crnogorcevic caro hansen juegue pierna cambiada delantera cualidades izquierda talento descomunal puliendo salma vivió montaña rusa acabó victoria doblete demostración talento atesora</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Deportes_26.txt</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1554,16 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>coronavirus virus gripe gripe mismísimo virus respiratorio sincitial vrs amigos entendernos responsable mayoría bronquilitis jaque consultas servicios urgencias pediátricas españa ¿qué común virus respiratorios campan respetos menor medida provocar fiebre ¿sabemos realmente fiebre tratarlacomo norma fiebre temperatura alcanza °c axila °c toma recto abajo cosa suele caliente necesita grado considerarlo fiebre¿por aparece fiebrepor compuestos llamados pirógenos ocurre espectáculo pirotécnico fuegos artificiales falta pólvora alguien encienda mecha caso encienden mecha llamados pirógenos microbios virus bacterias compuestos producen microbios fiebre reacción normal cuerpo generalmente aparece infección virus bacterias fiebre amiga respuesta combatir infección activar defensas organismo¿qué consecuencias fiebreaquí traigo noticias fiebre causa daño cerebral ceguera sordera muerte pacientes temen fiebre produzca daños elevaciones transitorias modestas temperatura central °c °c infecciones agudas suelen tolerarse fiebre elevada fiebre causa daño enfermedad genera fiebre fiebre causar síntomas escalofríos sudoración malestar sofocos calor¿y °cpor °c cosa empieza fea elevaciones extremas °c causar daños normalmente aumenta temperatura suele términos técnicos conoce hipertermia ambiental grave calor exterior sube fiebre aparece famoso golpe calor fiebre sube °c tomamos drogas ilegales ej cocaína medicamentos anestésicos medicamentos antipsicóticos</t>
+          <t>presidente república sergio mattarella encargado economista carlo cottarelli formación ejecutivo transición conduzca país convocatoria elecciones anticipadas economista aceptado reservas prometido gobierno mantendrá neutralidad asuntos políticos electorales cottarelli comprometido presentarse próximas elecciones asegurado exigirá compromiso miembros futuro gabinetela normativa italiana establece encargado formar gobierno acepte reservas presente jefe retirar reserva garantizado apoyos parlamentarios situación excepcional producido encargo rompe esquemas habituales cottarelli encabezará ejecutivo lista ministros técnicos presentará programa gobierno cámaras parlamento caso obtener confianza programa incluirá aprobación septiembre presupuestos generales año economista reunirse mañana presidente gobierno presentará renuncia convocarán elecciones anticipadas celebrarán probablemente caso obtener mayoría necesaria parlamento opción probable gobierno dimitiría inmediatamente formaría ejecutivo instrumental sustitución dimisionario gobierno paolo gentiloni capacidad gestionar asuntos corrientes mantendría convocatoria elecciones veranoen aumentado tensiones mercados financieros prima riesgo aumentado economía italiana creciendo cuentas públicas control cottarelli comparecencia aceptar encargo gobierno guiado aseguraría gestión prudente cuentas públicas señaladocottarelli aprovechado lanzar mensaje calma mercados internacionales europa diálogo unión europea ue defensa intereses esencial diálogo constructivo reconocimiento pleno papel italia economista confirmado participación italia zona eurocarlo cottarelli años conocido poderes políticos económicos italia experiencia internacional brillante currículo economista convertido reconocido analista actual crisis años trabajando fondo monetario internacional fm banca italia experiencia petrolera italiana eni nombrado comisario reducción gasto público gobierno enrico letta encargo terminó año llegada matteo renzi sabor agridulce podido implementar cien cien propuestas cálculos permitirían país ahorrar millones eurosa finales volvió fmi director ejecutivo director observatorio cuentas públicas italianas universidad católica milán domingo recibió sorpresa llamada presidente mattarella encontraba milán imparte clases economía prestigiosa universidad bocconila jura cargo ministros producirse mañana cottarelli deberá presentarse parlamento someter gobierno voto confianza senado cámara diputados movimiento estrellas liga suman votos parlamento fácil encontrar mayoría apoye ejecutivo</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Politica_51.txt</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1572,16 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>covid convirtiendo importante aliado enfermedades sarampión pandemia ayudando alas trastorno advierte reciente informe elaborado conjunto organización mundial salud oms centros control enfermedades estadounidenses cdc siglas ingléssegún datos cobertura vacunal sarampión disminuido forma sostenida comienzo pandemia convirtiendo enfermedad amenaza inminente escala globalen millones niños recibieron dosis vacuna sarampión señalan organismos advierten cifra precedentes millones recibieron dosis pauta vacunal millones quedaron segundaeste descenso supone importante retroceso avance mundial logro mantenimiento eliminación sarampión deja millones niños expuestos infecciónlos citados organismos señalan nueve millones casos sarampión provocaron muertes mundoun países sufrieron brotes causantes perturbaciones disminución cobertura vacunal debilitamiento vigilancia sarampión continuas interrupciones retrasos actividades inmunización covid persistencia brotes año sarampión amenaza inminente regiones mundo señaladoel sarampión enfermedad viral altamente contagiosa cuyos síntomas fiebre elevada tos exantema generalizado cuadro dura evolución causar complicaciones gravesen década desarrollo vacuna millones niños mundo infectaban año virus sarampión producían millones muertes consecuencia enfermedadla vacuna triple vírica administra dosis protege frente sarampión rubeola parotiditis españa dosis recibe meses añosel mes abril organización naciones unidas onu alertó casos sarampiónsubieron meses organismo advirtió pandemia covid seguirle tormenta perfecta brotes enfermedadesya llegada covid sarampión experimentado importante resurgimiento oms casos enfermedad infecciosa triplicaron año causas citadas figuraban falta acceso servicios salud vacunación brotes zonas conflicto comunidades desplazadas desinformación falta concienciación necesidad vacunarse alusión fenómenos movimientos antivacunas meses pandemia circulación virus resintió impacto llegada sarscov programas vacunación dándole alas</t>
+          <t>numerosas investigaciones demostrado sufrir experiencia traumática aumenta riesgo padecer secuelas años suceso episodios alto impacto saltar aires vida experimentapero pasa golpes consideran excepcionales efecto problemas conflictos cambios marcan llamar vida normal investigación tratado arrojar luz factores estrés psicosocial consecuencias salud neurológicasus datos costumbre advierten riesgos vivir rodeado quebraderos cabeza mediana edad estudio muestra factores comunes estrés psicosocial consecuencias severas prolongadas tipo fisiológico tipo psicológico señalan autores investigación acaba publicar revista bmj open conclusiones ponen mesa estrecha relación número estresores sufre persona mitad vida posibilidades sufrir demencia décadas despuéspara llegar resultados científicos liderados lena johansson unidad epidemiología neuropsiquiátrica universidad gotemburgo suecia seguimiento mujeres suecas nacidas periodo añoslas participantes enrolaron ensayo evolución salud sometieron distintos exámenes test neuropsiquiátricos periódicamente vida visita aparte pruebas habituales participante debía relatar sufría síntomas relacionados estrés irritabilidad miedos frecuentes problemas sueñoademás encuentro investigadores mujeres preguntó afectaban factores estresantes comunes haberse divorcionado haberse quedado viuda familiar enfermedades mentales sufrir problemas necesitar ayuda social estadosegún datos muestra reconoció experimentar factores estresantes vida porcentaje quebraderos cabeza importantes vidas ascendía problema frecuente citado mujeres pariente cercano aquejado trastorno psiquiátricoa investigación muestra mujeres desarrollaron demencia diagnosticadas alzheimer observaron investigadores cruzar datos número factores estrés declarados mujeres asociaba riesgo padecer demencia especialmente alzheimer relación subrayan independiente factores determinantesen conclusiones científicos reconocen necesarios estudios confirmen resultados indaguen necesario marcha iniciativas manejar estreés determinados pacientes preservar saludsin adelantan explicaciones refrendar hipótesis punto vista estrés causar cascada reacciones fisiológicas sistema nervioso central sistema endocrino sistema inmune sistema cardiovascular forma conjunta afectarían funcionamiento cerebro consecuencia aumentarían posibilidades desarrollar demencia</t>
         </is>
       </c>
       <c r="C64" t="n">
         <v>1</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Salud_22.txt</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -1270,11 +1590,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>cae sistema desolador gente prefiere irse sitio centro salud afirmaciones vienen residentes medicina familia pediatría madrid entrevistados raíz huelga indefinida médicos atención primaria amyts mantiene noviembrelos mir destacan problemas sindicato denunciando falta profesionales facultativos saturados atender calidad pacientes responsabilizándose demasiados trámites burocráticos contratos condiciones atractivas generaciones huyen primaria consecuencia pacientes buscan urgencias atención ofrecer nivelen contexto falta médicos teoría comunidad permitirse lujo perder generaciones médicos familia formados cuatrienio autonomía decidieron quedarse servicio madrileño salud sermas mes junio llamamiento contratos temporales atención primaria incluidas plazas creación plan mejora nivel cubrió ofertay residentes entrevistados pesimistas panorama nivel veo atención primaria totalmente destruida afirma marta andrés medicina familia minutos pacientes entrevista clínica ponerte explorar pacientes pensar pasarnos metemos atenderles sistema planteado imposible hacerloal tercer año residentes mantienen contacto hospital viven persona situación urgencias médico siento sobrepasada pacientes vienen urgente pongo pasa centro salud cita semanas piensa aguantar preocupante crónicos médico acaban descontrolados riesgo acabar patologías graves médicos familia abasto lamentaclara gómez familia explica vive centro mayoría centros salud área plantillas infradotadas recambio altísimo médicos cupo directamente cupos médico asignado pacientes vienen urgencias cuentan atienden tardan mes darles cita médico médico marchó cupo reparten distintos facultativos centro sustitutoañade gómez muchísimos médicos familia quemados pacientes darles atención energía casa actualizarse difícil formacióncuando terminamos ocupar plazas llegas centro salud cupos médico vas cupo asignar caer sobrecarga médicos cubrir alternativas summa urgencias hospitalarias atención domicilio gente prefiere irse sitio centro salud situación precarización crónica años alguien coger plaza trampolín aguanta meses</t>
+          <t>ultraconservador andrzej duda permanecerá jefatura polaco años iguala mandato socialdemócrata aleksander kwasniewski único presidentes polonia instauración democracia empezando lech walesa punto lograrlo rival liberal rafal trzaskowski logró campaña sacar armario millones polacos atrevían basta deriva democrática hegemónico gubernamental partido ley justicia pis duda apadrinadode años jurista profesión duda carta líder jaroslaw kaczynski líder pis partida unión europea caballo troya reformas bruselas recela justifica discurso nacionalista busca resarcir polacos agravios historia batería leyes adoptadas gobierno pis sancionadas duda figura norma castiga años prisión hablar campos concentración polacos ley holocausto criticada israel considerar desafiaba históricahijo pareja profesores escuela minas metalúrgica cracovia carrera política duda ligada hermanos lech jaroslaw kaczynski edad años jaroslaw ministro convirtió subsecretario justicia diputado eurodiputado vicesecretario presidente lech muerte tragedia aérea smolensk rusia intentó éxito hacerse alcaldía cracovia ciudad natalduda carecía rostro inmensa mayoría polacos finales elecciones presidenciales vista jaroslaw kaczynski anunció pronóstico concurría jefatura hermano trágicamente vacante hombre fuerte pis lanzó candidatura duda mayo edad años desconocido candidato convirtió presidente polacos votos presidenciales ajustadas vividas poloniacontra aborto personas lgtbiarrancó mandato cohabitación partido liberal plataforma cívica po gobierno donald tusk abandonó puesto convertirse presidente consejo europeo elecciones parlamentarias octubre pusieron cohabitación sexta economía ue viraje derecha pis conquistó mayoría aplastante legislativoduda apuntalado kazcynski oficialmente pertenece partido superviviente políticos dóciles compensa falta carisma ejecutivo promesas sociales económicas programa gobierno pis nichos desfavorecidos rural familias tradicionalistas poderosa iglesia católica duda tomado debate aborto llevó miles mujeres calle llamado lunes negro semana plena campaña electoral firmó propuesta prohibir adopción parejas sexo iniciativa inocente rival trazkowski colectivos lgtbi pedido voto pisaba talones encuestas escuchen idioteces sobe derechos humanos gente gente normal repetido portavoces duda campaña enfrentó orgullo prejuiciosla estrategia resultado frente cambios representaba europeísta liberal alcalde varsovia duda apeló continuismo polonia conservadora beneficia derechos libertades ayudas económicas ue sienten sarpullido club dominado vieja potencia invasora llamada alemania excesivamente condescendiente enemigo rusiael aliado europeo fiel trumpno desapercibido semana cita urnas duda viajara unidos entrevistarse presidente donald trump presentó aliado europeo otan fiel solícito encuentro produjo trump anunciara retirada efectivos estadounidenses alemania polonia acogería gradoen recta vuelta duda visto envuelto escándalo intentado escapar removiendo fantasmas puro estilo pis semanario polaco fakt reveló duda concedió marzo perdón presidencial convicto abusos sexuales levantó orden alejamiento pesaba abusar hija petición edadduda respondió difusión información fakt propiedad conglomerado alemán axel springer acusando alemania intromisión elecciones campaña despiadada sucia dirigida personalmente alemanes quieren elegir presidente polonia injusticia permitiré acto campaña región dolny slask apelo embajador alemán varsovia intervenga deseamos tipo intervenciones extranjeras polonia inmiscuye elecciones alemanas portavoz campaña duda adam bielanel portavoz gobierno alemán steffen seibert rechazó tajantemente acusaciones duda dispersado semillas agarran barbechos polonia apela resentimiento conspiración</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Politica_52.txt</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -1283,11 +1608,16 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>gripe supone constante amenaza salud pública epidemias estacionales oms provocan millones casos graves millón muertes año mundo riesgo capacidad cambiar cara virus gripal consiga provocar próxima pandemiahace años frente amenaza distintos grupos científicos buscan desarrollar vacuna universal frente gripe permita adelantarse posibles variaciones patógeno ofrecer escudo protector preparado afrontar ataqueuna investigación publicada jueves science acerca paso objetivo datos científicos estadounidenses conseguido desarrollar vacuna universal gripe modelos animales resulta protectora desarrollo prueba concepto llevado cabo tecnología arn mensajero empleó vacunas covideste abordaje permitido científicos liderados claudia arevalo instituto inmunología universidad pensilvania eeuu crear vacuna contiene antígenos correspondientes subtipos identificado virus gripea circulan humanos tipos virus gripe hn hn linajes virus tipo vacunas estacionales cuya efectividad limitada dirigen variantes tipos virus máximo antígenos producto subtipos virus afectan humanos menor medida potencial pandémicoel equipo arevalo conseguido desarrollar formulación incluye antígenos subtipos tecnología arn mensajero podido encapsular producto proteínas específicas subvariantes concreto hemaglutininas proteínas constituyen sitios principales reconocimiento antigénico sistema inmunitariobuenos resultados ensayos preclínicosen experimentos ratones hurones investigadores pudieron comprobar vacuna inducía animales producción anticuerpos específicos frente subtipo permanecían organismo meses vacunación numerosos obtienen vacunación convencionaltras someterles desafío virus gripe investigadores comprobaron animales vacunados presentaban protección frente patógenosnuestro estudio indica vacunas arn mensajero proporcionar protección frente virus antigénicamente variables inducir forma simultánea anticuerpos frente múltiples antígenos señalan investigadores revista científica</t>
+          <t>explosiones golpearon simultáneamente madrugada domingo lunes aeródromos militares rusos situados cientos kilómetros ucrania muertos heridos cobra fuerza hipótesis ataque medios locales apuntan dron estalló instalaciones desplegados bombarderos estratégicos fuerzas aéreas rusas ministerio defensa ruso responsabilizó lunes ucrania ataque autoría confirmada alto funcionario ucranio declaraciones diario estadounidense the new york times asegurado drones país bombardearon aeródromos rusos previamente mijailo podoliak asesor presidente ucranio volodímir zelenski insinuado twitter explosiones respondían operación especial kiev confirma oficialmente autoría ucrania trataría ataque suelo ruso alejado frontera inicio guerrael ministerio defensa ruso confirmó lunes ataque versión kiev lanzó bases drones baja altitud servicio aviones alcance moscú asegura proyectiles interceptados fragmentos producidos explosión provocaron daños insignificantes aviones información the new york times drones despegado territorio ucranio lograron destruir aviones rusos dañar máshoras conocerse explosiones provincias ucrania kiev sufrieron ataques misiles rusos muertos comunicado ministerio defensa recalcó ataque logró impedir posterior bombardeo masivo infraestructura ucrania moscú alcanzó objetivos misiles disparados tierra mar aire mando fuerzas aéreas ucranias logrado derribar proyectiles lanzados pasaban empresa estatal energética ukrenergo explosiones afectaron infraestructuras objetivos prioritarios ataques ejército ruso ministro ucranio denis shmihal concretó daños producido regiones kiev vinitsia odesael gobernador región rusa sarátov román busarguín telegram explosiones afectaron edificio civil quiero asegurarles producido emergencia zonas residenciales ciudad motivos preocuparse infraestructura civil resultó dañada escribió aeropuerto sarátov situado kilómetros ucrania medios rusos astra baza dron explotó pista base aérea engels región sarátov bombarderos estratégicos resultado dañados aeronaves forman fuerzas disuasión estratégica papel importante ataques misiles convencionales ucraniapor agencia ria novosti informado explosión aeródromo riazán situado kilómetros moscú fuentes personas muerto resultado heridas supuesta explosión camión combustibleantes diario estadounidense publicara información cita alto funcionario confirmó autoría ucrania ataque asesor presidente zelenski insinuado kiev ataques tierra redonda descubrimiento galileo kremlin estudiado astronomía preferencia astrólogos sabrían lanza espacio aéreo países objetos voladores desconocidos volverán punto partida escribió podoliak twitterla industria militar ucrania anunció domingo punto aparato tripulado capaz transportar carga explosiva kilogramos radio kilómetros probar éxito dron entorno guerra electrónica esperamos verlo combate prometimos finales año tratando cumplir promesas anunció jefa prensa conglomerado industrial militar ucranio ukroboronprom recoge agencia unianobjetivos prioritarioslos aeródromos militares rusos objetivos prioritarios fuerzas armadas ucranias agosto paso respuesta rusia bombardearon base aérea saki crimea pese kremlin amenazaba dura réplica acción península anexionada kiev podía incentivo atacar instalaciones sarátov semanario alemán der spiegel publicó semana presencia numerosos bombarderos estratégicos imágenes satélite base engels apuntaban preparación ataque escala ucraniapoco explosiones aeródromos riazán sarátov coincidiendo entrada vigor europeo petróleo ruso suministrado mar tope occidental precio rusia lanzó lunes andanada misiles territorio ucranio alarmas sonaron decenas ciudades ucranias incluida kiev lanzado misiles yuri ihnat portavoz fuerza aérea ucrania ignore alarmas advirtió ciudadanía andri yermak jefe gabinete presidencial ucraniolos misiles golpearon provincias peores consecuencias vivieron zaporiyia sudeste ucrania autoridades informaron muerte personas ataque afectó infraestructuras suministran electricidad kiev odesa vinitsia regiones sufrieron cortes luz agua odesa mikolaiv sur sumi norte ciudad natal presidente zelenski krivi rig estealgunos expertos rusos alertan explosión puente kerch península anexionada crimea retaguardia rusa voladura puente quedan instalaciones estratégicas rusia puedan considerarse absolutamente seguras asesinato daria dugina hija ideólogo kremlin alexander dugin decía redes sociales corresponsal guerra ruso alexánder kots sarátov clandestinidad ucrania opera territorio ruso fuerzas especiales detienen agentes kiev regularmente flujo refugiados puedes seguimiento añadía kots advertir población acostumbrada vida tranquilaputin teme ataques puente crimeavladímir putin recorrido lunes reconstruido puente crimea meses destrucción parcial visita simbólica inicio invasión ucrania febrero presidente ruso visitado península anexionada forma ilegal importantes bases aéreas rusas sufrían explosiones cientos kilómetros frente mandatario advertía rusia reforzar control disputado sur ucrania proteger suministro península mar negro continuas amenazas expresadas oficialmente kiev posibles ataques puente putin enfatizado importancia vía terrestre conecta crimea resto rusia afirmado portavoz kremlin dmitri peskoval volante mercedes alemán marca abandonado país sanciones putin inauguró apertura carriles vehículos dañados fuerte explosión octubre obstante abiertos vehículos ligeros putin admitido apuntalados alcanzar perfecto prosigue reparación vías ferrocarril ruta clave enviar suministros fuerzas ejército desplegado sur ucrania putin tráfico debería volver operar mediados verano putin informado vice ministro marat jusnullin progreso obras restauración conversó obreros condujimos derecho entendido izquierdo puente condiciones operar falta terminarlo sufrió putin declaraciones recogidas agencia interfax vice ministro respondió tramo condiciones funcionar reforzado posteriores ataque indica pondremos condiciones reparación puente kerch visto afectada tormentas interfirieron preguntó putin jusnullin coche interfirieron fuerza tormentas respondió alto cargomoscú acusó ministerio defensa ucranio fuertes daños sufrió infraestructura kremlin convirtió símbolo conquista territorial años investigación sabotaje perpetrado compleja operación servicios especiales kiev colaboradores rusos ocultaron bomba camión carga explosivo enviado ciudad rusa armavir bulgaria armenia georgia introducido cargamento rollos película cuya entrega solicitó dirección falsa crimea gobierno ucranio confirmó autor ataque</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Politica_56.txt</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -1296,11 +1626,16 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>posibilidad corregir genes defectuosos técnica sencilla predecesoras convertido hito científico opinión revista science tecnología denominada crispr utilizada éxito laboratorio ratones adultos patología genética logra resultados esperanzadoresla publicación eligió crispr hallazgo importante año termina recoge número investigaciones independientes idéntico resultado cortapega genético logrado mejorar atrofia muscular ratones afectados distrofia duchennela distrofia duchenne enfermedad degenerativa afecta varones nacidos vivos causa rápido deterioro sufren pacientes media suelen verse postrados silla ruedas años vida defecto gen codifica proteína esencial funcionamiento músculosesa proteína distrofina codificada gen compuesto regiones exones piezas puzle funciona cadena producción distrofina pone marcha gen cromosoma distrofia duchenne afecta varones doble copia mujeres garantiza cromosoma disponen copia intacta gen distrofinahasta llevado cabo intentos reparar gen distintos métodos terapia génica publica revista science ratones esperanzadoresutilizando virus adenoasociado taxi herramientas corte genético gen defectuoso animales equipos científicos logrado resultados similareslos investigadores universidades duke harvard texas eeuu lograron eliminar exones defectuosos ratones distrofia concretamente necesidad sustituirlo copia corregida simplemente borrado pieza defectuosa lograr producción distrofina animales versión reducida funcional gen recuperaron parcialmente función muscularen opinión lluis montoliu centro nacional biotecnología trabajos interesantes abren puerta futuras aplicaciones clínicas pacientescomo explica diario experimentos similares células realizados vivo novedad relevancia aclara pasocomo aclara virus adenoasociados sirve vehículo transporte vector tijeras genéticas exon mutado local inyección pata sistémica viajen organismohasta técnica crispr funciona especie cortapega genético reemplazar regiones genéticas mutadas probado únicamente líneas celulares éxito animales vivos adultos cuya enfermedad genética causado daños muscularesen trabajos dirigido christopher nelson universidad duke inyectaron pata abdomen virus adenoasociados lograr llegar exon borrarlo relatan artículo inyecciones locales lograron restaurar nivel distrofina mejoría músculos pata animal caso inyección abdomen pruebas posteriores mostraron mejoría músculos cardiaco pulmonar estructuras ven afectadas falta producción distrofina relacionadas mortalidad prematura lso afectados duchenneen caso chengzu long universidad texas southwestern emplearon virus patógeno humano adenovirus denominado aav llegar herramientas crispr exon caso probaron óvulos espermatozoides lograron ratones libres mutación casos posteriormente repitieron prueba grupo ratones duchenne nacer ocasión inyección genética aplicada directamente músculos logró mejorías significativas animales persistieron meses terapiaa resultados tercer idénticamente positivos autores cautos traducción hallazgos humanos posibilidad crispr corregir defectos embriones humanos generado enorme controversia ética recientemente explica charles gersbach coautor estudio declaraciones transmitidas universidad aplicación tejidos adultos afectada debate estudios demuestran posibilidad queda reconoce</t>
+          <t>sirenita michelle alonso santa cruz tenerife conquistó piscina oro metros braza categoría discapacidad intelectual registrando récord mundo prueba estrella corona londres revalidó río tokio demostrado reina indiscutible oros juegos incontestable canaria daba decimoséptima medalla españa sincera esperaba oro plata sabía rivales siento soñando sonar despertador medallas paralímpicas especial significado conseguirla tokio confesóeste oro redondear juegos papel protagonista nadadora elegida ricardo ten abanderada equipo español ceremonia inauguración vio desparpajo estadio nacional tablas michelle ejerció abanderada clausura ríounos problemas espalda lanzaron piscina años apuntaba maneras maneras recibieron mejores pensó marcharse volver problemas comunicación encajaba resto compañeras burlas tornaron situación insostenible ademi josé luis guadalupe alias guada mentor entrenador padre natacióny sirenita voz empezó hablar alto brazada metro recorrido ganaba confianza dejaba atrás rechazo compañeras daban discapacidad intelectual tokio deslumbrando carrera cimentada esfuerzo brilla base medallas sonríe disfruta países favoritos puesto loca sushi anime manga cultura japonesa pisa tokio últimaademás rostro michelle desconocido público nipón años protagonizó documental cadena nipona wowow michelle reina aguas mares resistan sirenita</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Deportes_52.txt</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -1309,11 +1644,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>centroamérica enfrentando epidemia dengue vive constatado organización panamericana salud ops señalado presencia cepa agresiva virus costado vida centenar personas contagiado regióntal informaba conferencia prensa socorro gross representante ops nicaragua serotipo agresivo virus propagó rápidamente américa central actual temporada lluviassegún cifras oficiales dengue cobrado vidas centroamérica honduras nicaragua guatemala salvador costa rica fallecido informa personas contagiadas cifra alta país años elevada centroaméricapor presidente nicaragua daniel ortega muertes registrado afectados enero decretado alerta roja sanitaria contener epidemiaa autoridades honduras sanitarias san pedro sula ciudad importante honduras elevado nivel alarma umbral emergencia médica registrado casos periodo año contabilizan enfermos denguese variante peligrosa enfermedad indicado médicos fronteras msf comunicado ong prestando servicios hondureños afectadosla epidemia dengue representa amenaza población hondureña empezamos visto flujo constante pacientes incluyendo casos graves niños explicado coordinador médico msf doctor luis neirasegún podido constatar ong agosto subida casos sospechosos dengue fecha año pasadonicaragua medidas implantar urgente realizará jornadas fumigación mosquito aedes aegyti vector transmite infección movilizarán miles brigadistas salud mañana país brigadistas llevarán instrucciones correspondientes detectar casos sospechosos dengue visitas casa casa remitirlos inmediato unidades salud evaluación clínicalos síntomas enfermedad fiebre dolor cabeza cuerpo casos graves deshidratación grave hemorragias internas conducen muerteexiste situación desastre calamidad país señala rosa murillo dama portavoz oficial centros salud hospitales públicos encuentran atestados enfermosel mosquito transmisor dengue incuba larvas depósitos agua limpia cáscaras huevo macetas vacías llantas automóvil patios jardines viviendas negocios oficinas</t>
+          <t>congreso sociedad americana oncologia clínica asco congreso esperanza año oncólogos mundo comparten escenario avances torno lucha cáncer queda oncología especialidad viva avances tipos cáncer continuos casos brillan ausencia tumores cerebrales pertenecen categoríael único estudio presentado sesión plenaria selecciona trabajos importantes tumor cerebral alternativa afectados glioblastoma tumores cerebrales utiliza éxito línea cáncer recurrido funciona matando hambre vasos sanguíneos utiliza tumor alimentarse conoce angiogénesisel polémico coincidido presentación estudio importante participación española concluye contrariamente añadir fármaco antiangiogénico bevacizumab radio quimioterapia aumentaba supervivencia libre progresión mesesasí rueda prensa presentaron resultados preguntas relativas diferencia estudios potencial encontramos pacientes correctos estudio encontrado mark gilbert md anderson cancer center autor trabajoel neuroncólogo español juan manuel sepúlveda participado estudios valora diferencia trabajos cuestión diseño estudios rtog llama estadounidense excluyó pacientes inoperables constituyen administración antiangiogénico tardía avaglio nombre estudio europeo positivo estudio estadounidense permitía conoce crossover pacientes recurrían daba opción recibir fármaco mayoría pacientes tratado medicamentomás allá polémica siquiera estudio positivo permitía hablar reducción global mortalidad presentado asco sepúlveda defiende avances despacioeste especialista destaca cabo grupo español investigación neuroncología geino combina investigación básica puntera clínica señala cambiado radicalmente años asistido mejora radioterapia introducción quimioterapia bevacizumab tumor reproduce pequeñas noticias subraya especialistael problema tumores cerebrales activan alteraciones moleculares parecido pasa cáncer páncreas continuamente buscando punto débil apunta expertoesos presumibles puntos débiles frutos molécula dirigida proteína juega papel esencial tumores cerebrales tgf beta presentado resultados seguridad congreso equipo sepúlveda participando ensayos clínicos hospitales españolesno único fármaco estudio geino analiza eficacia inhibidor familia receptores her pacientes glioblastoma recurrente amplificaciones gen egfr destaca neuroncólogo español equipo biólogos instituto salud carlos iii dirigidos pilar sánchez acaban describir diana terapéutica glioblastomas proteína dyrkaquizás congresos noticias torno tumor cerebral</t>
         </is>
       </c>
       <c r="C68" t="n">
         <v>1</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Salud_38.txt</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -1322,11 +1662,16 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>número afectados fallecidos tuberculosis descendido significativamente mundo camino alcanzar objetivos milenio relativos enfermedad quedan metas cumplir datos alarman especialmente organización mundial salud omsen informe global tuberculosis organismo naciones unidas manifiesta preocupación alarmante aumento resistencias antibióticos tradicionales restricciones acceso fármacos culpa problemas económicos larga lista paísesde documento advierte enfermos tuberculosis mundo tratamiento millones personas escapan sistemas sanitarios convierten preocupante problema salud pública afectados países siquiera diagnosticados reconoce mario raviglione director programa global tuberculosis omsun problema paralelo falta recursos sistemas salud advierte oms capacidad llegar pacientes marginales difíciles captar vías tradicionales significa diagnosticar tratar preocupa especialmente caso cepas resistentes multiresistentes responden mayoría antibióticos disponiblesde tests diagnóstico rápidos permitido aumentar número casos detectados pacientes tuberculosis multiresistente siguen diagnosticados caso detectados pacientes diagnosticados acceso tratamientoen caso tuberculosis iniciar cumplir tratamiento antibióticos esenciales paciente recupere deje transmitir bacilo personas incumplimientos tratamiento antibióticos aumento mundo cepas tuberculosis resistentesla oms calcula personas enfermaron tuberculosis año china india federación rusa casos pacientes coinfectados virus vih recibe tratamiento antirretrovirales tuberculosis patología infecciosa aprovecha inmunodeprimido pacientes desarrollarse calcula tercio población tuberculosis latente riesgo real enfermarel informe oms concluye recomendaciones afrontar patología cumplir objetivos milenio naciones unidas enfermedad tratar llegar millones personas escapan control sistemas salud seguir propagando enfermedadademás pide autoridades esfuerzo económico afrontar problema resistencias recomendaciones concluyen mención especial coinfectados vih acelerar innovación tecnológica tests diagnósticos tratamientos lleguen países necesitados finalmente inversión económica patología recuerda oms países recursos dependen fondos internacionales frente tuberculosis</t>
+          <t>psoe mantiene intención voto pp bajaría punto mes barómetro noviembre centro investigaciones sociológicas cis público viernes sondeo concluye partido socialista socio mayoritario gobierno coalición ganaría hipotéticas elecciones generales apoyos octubre principal partido oposición liderado alberto núñez feijóo reuniría papeletas punto resultados socialistas aumentan puntos distancia populares unidas socio psoe ejecutivo lograría votos punto mes vox recupera punto ciudadanos baja levemente formación independentista erc rasca décima sondeo pregunta principal responsable ruptura delas negociaciones gobierno populares renovación consejo judicial tribunal constitucional encuestados apuntan pp frente señala psoeel campo sondeo analiza información entrevistas noviembre error muestral barómetro pp rompiera negociaciones gobierno renovar judicial años caducado límite tribunal supremo imposibilidad nombramientos funciones pregunta encuestados principal responsable naufragio conversaciones renovación órgano gobierno jueces tribunal constitucional cuya designación encallada disyuntiva señala pp responsable ruptura frente apunta psoe encuestas coincidieron anuncio presidente gobierno pedro sánchez reforma código penal suprimirá delito sedición motivo alegó partido feijóo romper negociación renovación judicial polémica política posteriorla posición pp psoe principales fuerzas políticas país mantiene línea similar barómetro tendencias voto municipales incluía estimación comicios generales calculaba distancia puntos formaciones barómetro noviembre pregunta preparación personal líderes pedro sánchez alberto núñez feijóo respuestas sitúan plano similar presidente gobierno saque ventaja líder oposición encuestados ve líder socialista preparado preparado frente dirigente popular preparado preparado mes barómetro evaluado popularidad aceptación líderes visible choque exlíder pablo iglesias ministra yolanda díaz precisamente díaz vicepresidenta líder unidas gobierno coalición política encuestados puntuación siguen presidente gobierno pedro sánchez líder pp alberto núñez feijóo líder país íñigo errejón alcanza inés arrimadas ciudadanos valorado santiago abascal principales preocupaciones ciudadanas crisis económica problema nombrado seguido paro sanidad problemas políticos ocupan cuarto ―un citan― educación sitúa quinto puesto comportamiento políticos citado pregunta encuestados problemas afectan personalmente mantienen puestos crisis económica sanidad paro educación continuación entran incertidumbres relacionadas calidad cambio climático inseguridad ciudadana</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Politica_23.txt</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -1335,11 +1680,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>décadas figurado lista principales enemigos salud consumo demonizado apuntalado larga lista riesgos dejado crecer estrategias combatirlas grasas empezando redimidas cienciavarias investigaciones recientes señalado hora quitarles estigma dañinas constatación tipos grasa tomar aceite oliva cuyas propiedades cardiosaludables ratificadas ingerir conocidos ácidos grasos trans presentes alimentos procesados cuyos riesgos probados evidencias grasas principales culpables epidemia enfermedades cardiovascularesla relación aparentemente lógica consumo grasa alimentaria acumulación grasa corporal tambaleado señalaba diario meses josé maría ordovás director laboratorio nutrición genómica usdahuman nutrition research center on aging universidad tufts eeuu principales expertos áreacoincidía punto vista semanas dariush mozaffarian codirector programa epidemiología cardiovascular universidad harvard visita centro nacional investigaciones cardiovasculares señalaba empezó colesterol sangre único parámetro evaluar calidad dieta llevó recomendación reducir grasas dieta error dieta depende mides colesterol fotografía reducidaesta semana comentario publicado revista bmj firmado cardiólogo británico aseem malhotra une argumentario sugiriendo suprimir mantra asocia grasa saturada enfermedad cardiovascularpara malhotra historia culpable señalar dedo duda azúcar industria añade productosel miedo grasa señala cardiólogo llevó considerable reducción presencia productos procesados problema ejemplifica quitas grasa comida industria alimentaria compensó falta reemplazando grasa saturada azúcares añadidosla evidencia científica actual añade demostrando azúcar factor riesgo independiente desarrollar síndrome metabólico personas llegan hospital infarto concentraciones colesterol totalmente normales subraya malhotra seguidamente pregunta replantearse colesterol realmente problemala obsesión colesterol llevado sobremedicación millones personas comenta cardiólogo reflexiona demostrado adoptar dieta mediterránea ataque corazón efectivo tomar estatina reducir mortalidad</t>
+          <t>preguntas grupo parlamentario socialista sesión control gobierno miércoles pedir explicaciones escándalos corrupción afectan pp protagonismo ministros rafael catalá juan ignacio zoido caso lezo iniciará ofensiva portavoz antonio hernando quen preguntará presidente gobierno piensa recuperar confianza ciudadanos sucesión casos corrupción afectan pp ministro catalá protagonismo preguntas portavoz adjunta isabel rodríguez abordará gobierno pensado maniobras fiscalía obstaculizar determinadas causas judiciales corrupción denuncias fiscales presiones jefe anticorrupción manuel moix caso lezo diputado rafael simancas exigirá explique vínculos implicados operación lezo intercambió mensajes sms ignacio gonzález operación lezo diputado felipe sicilia preguntará ministro interior juan ignacio zoido secretario seguridad justificado suficientemente reunión hermano ignacio gonzález comparecencia número interior arremetió prensa oposición cuestionar actuaciónotras preguntas dirigirán ministro hacienda portavoz economía pedro saura preguntará cristobal montoro pensando amnistía fiscal beneficiosa lucha corrupción sabido implicados operación lezo apuntado amnistía fiscal diputada soraya rodríguez reclamará valoración revelaciones relacionadas actuaciones irregulares rodrigo rato interpelación urgente ministro justicia ofensiva corrupción afecta pp grupo socialista presentará sesión control interpelación urgente ministro justicia responsabilidades políticas piensa asumir consecuencia maniobras producido seno ministerio fiscal dirigidas obstaculizar determinadas causas judiciales corrupción actuaciones ministro relación causasesta interpelación dará paso pleno mayo moción grupo socialista reclamará reprobación destitución ministro justicia fiscal fiscal anticorrupción</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Politica_16.txt</t>
+        </is>
       </c>
     </row>
     <row r="71">
@@ -1348,11 +1698,16 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>diagnóstico cáncer mama llega zarpazo dudas miedos búsqueda pacientes familiares empiezan consultar cae manos enfermedad entran mitos leyendas mentiras repetición quedando cabeza tratara jornadas viaje cáncer mama celebrada madrid necesarias derribar verdades medias terminan losa tranquilidad afectados tumorel año auditorio escuchando contó hacía mes diagnosticado cáncer mama vine informarme sirvió importante recibir información sitio adecuado hablar expertos afirmaba jueves periodista inés ballester maestra ceremonias jornada hm universitario sanchinarro madridtanto pacientes presentes auditorio pudieron solventar dudas alimentación mano ricardo cubedo oncólogo hospital universitario puerta hierro majadahonda madrid derribó mitos enfermedad montón ideas falsas leyendas internet encontrar personas buscan información internet ¿quién mira fecha actualización página diferencia paciente basaría respuesta clara concreta pregunta médicos objetivo móvil fabricando artículos científicos señalóde minutos especialista echó tierra ideas circulan foros cáncer soja fomentar tumores próstata prevenir mama constatado generalizado evidencia científica datos avalen consumo leche vaca influencia tumorhay terreno amplio mitos realidades desinformación ruido explica cubedo entrar profundidades enumeró leyendas sujetador aro causa cáncer mama desodorantes peligrosos teñirse pelo diagnóstico tumor</t>
+          <t>presidente comité olímpico español coe alejandro blanco valorado miércoles decisión federación tiro arco volver juego plaza olímpica asegurado respeta normas pone federación conceder billete juegos tokio aplazados encuentro telemático ufedega unión federaciones deportivas gallegas comité olímpico español blanco interpelado presidente federación gallega tiro arco decisión tomado deportista gallego miguel alvariño ganarse billete tokioespaña plaza tokio asegurada verano mano pablo acha clasificatorios juegos olímpicos arquero gallego adjudicó volverá disputarse billete presidente coe distinguió hora clasificación jjoo clases deportes equipo ypor individuales diferencias casos deportista gana plaza juegos acudir gana país representa tiro arco ganado deportista plaza país pablo acha federación plaza jjoo pongo serie condiciones razonó blanco recordó potestad tomar decisión requisitos clasificarse tokio federación deportivacorrespondiente plaza país coe presenten equipos potestad entrar decisiones tome federaciónademás alejandro blanco deseo gobierno acelere desescalada deportistas puedan regresar entrenamientos hice peticiones corresponde debemosser iguales desescalada responsable coe trasladado ufedega comunicado puedes argumentar razonablemente futbolista entrenar piragüista tenista judoca ejemplos puedan pedido gobierno acelere desescalada</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Deportes_44.txt</t>
+        </is>
       </c>
     </row>
     <row r="72">
@@ -1361,11 +1716,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>viernes firma iniciativa salud libre mercurio marco convenio minamata pide eliminación definitiva termómetros tensiómetros contengan mercurio pondrá producción importanción exportación instrumentos médicos incluyan elemento químico productos contienen pilas interruptores firma convención minamata conseguiremos proteger mundo devastadoras consecuencias mercurio salud afirma directora margaret chan elementos químicos preocupación salud pública dispersa permanece organismos años causando graves enfermedades discapacidad intelectual población expuesta continúa causar daño cerebral especialmente jóvenes desórdenes sistema nervioso inmunitario reproductor daños renales digestivoshace años expertos advertían anunciaban incremento emisiones metal negociaciones principios año países llegaron vinculante reducción emisiones finalmente suscribe viernespara conseguirlo convenio establece plan acción países firmantes eliminen formas perjudiciales mercurio reduzcan emisiones metal procedentes industria promuevan alternativas mercurio asequibles seguras protejan niños mujeres edad fértil mercurio plantea amenaza especial desarrollo niño útero exposición elemento químico tomen medidas mejorar salud bienestar trabajadores contacto mercurioaunque convención minamata permite sigan utilizando aparatos médicos medición mercurio circunstancias especiales organización mundial salud oms coalición internacional salud daño insisten dadas tremendas consecuencias exposición mercurio salud debería mantenerse fecha límitela oms trabajará gobiernos garantizar cumplan obligaciones virtud convenio especialmente áreas salud señala doctora maría neira directora oms salud pública ambiente requiere eliminación termómetros tensiómetros mercurio oms asociados sector salud comprometen eliminar mercurio antisépticos tópicos cosméticos aclarar piel quieren desarrollar medidas eliminar mercurio empastes productos dentales fomentar intercambio información investigación salud pública</t>
+          <t>cae sistema desolador gente prefiere irse sitio centro salud afirmaciones vienen residentes medicina familia pediatría madrid entrevistados raíz huelga indefinida médicos atención primaria amyts mantiene noviembrelos mir destacan problemas sindicato denunciando falta profesionales facultativos saturados atender calidad pacientes responsabilizándose demasiados trámites burocráticos contratos condiciones atractivas generaciones huyen primaria consecuencia pacientes buscan urgencias atención ofrecer nivelen contexto falta médicos teoría comunidad permitirse lujo perder generaciones médicos familia formados cuatrienio autonomía decidieron quedarse servicio madrileño salud sermas mes junio llamamiento contratos temporales atención primaria incluidas plazas creación plan mejora nivel cubrió ofertay residentes entrevistados pesimistas panorama nivel veo atención primaria totalmente destruida afirma marta andrés medicina familia minutos pacientes entrevista clínica ponerte explorar pacientes pensar pasarnos metemos atenderles sistema planteado imposible hacerloal tercer año residentes mantienen contacto hospital viven persona situación urgencias médico siento sobrepasada pacientes vienen urgente pongo pasa centro salud cita semanas piensa aguantar preocupante crónicos médico acaban descontrolados riesgo acabar patologías graves médicos familia abasto lamentaclara gómez familia explica vive centro mayoría centros salud área plantillas infradotadas recambio altísimo médicos cupo directamente cupos médico asignado pacientes vienen urgencias cuentan atienden tardan mes darles cita médico médico marchó cupo reparten distintos facultativos centro sustitutoañade gómez muchísimos médicos familia quemados pacientes darles atención energía casa actualizarse difícil formacióncuando terminamos ocupar plazas llegas centro salud cupos médico vas cupo asignar caer sobrecarga médicos cubrir alternativas summa urgencias hospitalarias atención domicilio gente prefiere irse sitio centro salud situación precarización crónica años alguien coger plaza trampolín aguanta meses</t>
         </is>
       </c>
       <c r="C72" t="n">
         <v>1</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Salud_13.txt</t>
+        </is>
       </c>
     </row>
     <row r="73">
@@ -1374,11 +1734,16 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>organización nacional trasplantes ont puso marcha programa pacientes recibido trasplante renal cruzado llevamos año cifra duplica año efectuaron trasplantes tipo cuadruplica datos ont demuestran creciente aceptación pacientes familiares nefrólogos urólogos inmunólogos modalidad trasplante renal participan hospitales españa laboratorios histocompatibilidad basada intercambio órganos donantes vivo parejas objetivo ofrecer pacientes insuficiencia renal crónica posibilidad recibir injerto gracias generosidad pareja compatibleempezamos programa múltiples problemas reconoce elmundoes director organización nacional trasplantes ont rafael matesanzlos cruces requerían traslado donantes ciudad problemas logísticos conlleva agrega viaja donante riñón programa consolidado sirve estímulo donaciones renales vivo años desarrolladas suponen trasplantes vivo objetivo llegar modalidad terapéutica desarrollado países elevada actividad trasplante renal donante vivo caso corea sur holanda reino unido australia canadá unidos llevan realizando tipo trasplantes década excelentes resultadosel técnicas quirúrgicas invasivas estudio cuidado donante intervención permitido potenciar tipo trasplantes posibles complicaciones donante disminuido considerablemente actualidad extracción renal vivo procedimiento riesgoen país trasplante renal cruzado intercambio parejas intervenidas país vasco cataluña donantes receptores dados alta encuentran perfecto saludeste tipo trasplantes conlleva complicado proceso logístico requiere colaboración oficina central ont coordinadores autonómicos trasplantes hospitales equipos médicos participan operativo</t>
+          <t>covid convirtiendo importante aliado enfermedades sarampión pandemia ayudando alas trastorno advierte reciente informe elaborado conjunto organización mundial salud oms centros control enfermedades estadounidenses cdc siglas ingléssegún datos cobertura vacunal sarampión disminuido forma sostenida comienzo pandemia convirtiendo enfermedad amenaza inminente escala globalen millones niños recibieron dosis vacuna sarampión señalan organismos advierten cifra precedentes millones recibieron dosis pauta vacunal millones quedaron segundaeste descenso supone importante retroceso avance mundial logro mantenimiento eliminación sarampión deja millones niños expuestos infecciónlos citados organismos señalan nueve millones casos sarampión provocaron muertes mundoun países sufrieron brotes causantes perturbaciones disminución cobertura vacunal debilitamiento vigilancia sarampión continuas interrupciones retrasos actividades inmunización covid persistencia brotes año sarampión amenaza inminente regiones mundo señaladoel sarampión enfermedad viral altamente contagiosa cuyos síntomas fiebre elevada tos exantema generalizado cuadro dura evolución causar complicaciones gravesen década desarrollo vacuna millones niños mundo infectaban año virus sarampión producían millones muertes consecuencia enfermedadla vacuna triple vírica administra dosis protege frente sarampión rubeola parotiditis españa dosis recibe meses añosel mes abril organización naciones unidas onu alertó casos sarampiónsubieron meses organismo advirtió pandemia covid seguirle tormenta perfecta brotes enfermedadesya llegada covid sarampión experimentado importante resurgimiento oms casos enfermedad infecciosa triplicaron año causas citadas figuraban falta acceso servicios salud vacunación brotes zonas conflicto comunidades desplazadas desinformación falta concienciación necesidad vacunarse alusión fenómenos movimientos antivacunas meses pandemia circulación virus resintió impacto llegada sarscov programas vacunación dándole alas</t>
         </is>
       </c>
       <c r="C73" t="n">
         <v>1</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Salud_12.txt</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -1387,11 +1752,16 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>numerosas investigaciones demostrado sufrir experiencia traumática aumenta riesgo padecer secuelas años suceso episodios alto impacto saltar aires vida experimentapero ¿qué pasa golpes consideran excepcionales ¿cuál efecto problemas conflictos cambios marcan llamar vida normal investigación tratado arrojar luz factores estrés psicosocial consecuencias salud neurológicasus datos costumbre advierten riesgos vivir rodeado quebraderos cabeza mediana edad estudio muestra factores comunes estrés psicosocial consecuencias severas prolongadas tipo fisiológico tipo psicológico señalan autores investigación acaba publicar revista bmj open conclusiones ponen mesa estrecha relación número estresores sufre persona mitad vida posibilidades sufrir demencia décadas despuéspara llegar resultados científicos liderados lena johansson unidad epidemiología neuropsiquiátrica universidad gotemburgo suecia seguimiento mujeres suecas nacidas periodo añoslas participantes enrolaron ensayo evolución salud sometieron distintos exámenes test neuropsiquiátricos periódicamente vida visita aparte pruebas habituales participante debía relatar sufría síntomas relacionados estrés irritabilidad miedos frecuentes problemas sueñoademás encuentro investigadores mujeres preguntó afectaban factores estresantes comunes haberse divorcionado haberse quedado viuda familiar enfermedades mentales sufrir problemas necesitar ayuda social estadosegún datos muestra reconoció experimentar factores estresantes vida porcentaje quebraderos cabeza importantes vidas ascendía problema frecuente citado mujeres pariente cercano aquejado trastorno psiquiátricoa investigación muestra mujeres desarrollaron demencia diagnosticadas alzheimer observaron investigadores cruzar datos número factores estrés declarados mujeres asociaba riesgo padecer demencia especialmente alzheimer relación subrayan independiente factores determinantesen conclusiones científicos reconocen necesarios estudios confirmen resultados indaguen necesario marcha iniciativas manejar estreés determinados pacientes preservar saludsin adelantan explicaciones refrendar hipótesis punto vista estrés causar cascada reacciones fisiológicas sistema nervioso central sistema endocrino sistema inmune sistema cardiovascular forma conjunta afectarían funcionamiento cerebro consecuencia aumentarían posibilidades desarrollar demencia</t>
+          <t>mes luiz inácio lula silva arranque tercer mandato presidente brasil anunciado nombre futuro gobierno siquiera persona llevará riendas economía principal desafío presidente electo encabeza coalición decena partidos semana brasilia inmerso carrusel contactos misión apremiante negociar socios composición gobierno congreso permita sortear techo gasto cumplir principal promesa electoral millones pobres compatriotas sigan recibiendo paga mensual reales dólares euroslula desvelará gobierno diciembre explicado viernes prensa capital brasilia ceremonia tribunal superior electoral formalizará definitivamente triunfo logrado octubre ministerios cabeza querido recordar ganó proyecto amplio derrotar bolsonaro gobierno fuerzas apoyaron lograr victoriauno principales mantras izquierdista campaña pobres volverán presupuesto políticas sociales prioridad mandatos cuentas públicas situación precaria lula necesita fondos cumplir necesitados muchísimos brasileños pasa hambre tercio vive pobreza extrema pobrezael partido trabajadores pt presentó semana propuesta legislativa pretende dejar límite impone techo gasto partida gigantesca años dura mandato presidencial cifra propuesta millones reales millones dólares destinados mantener paga mensual pobres espero señorías sensibilidad lula falta llegar negociar congreso elegido bolsonarismo principio mayoría duda cobrará caro lula apoyo necesita plazos apremian toma posesión prevista año nuevoel nombre suena ministerio haciend fernando haddad candidato presidencial pt líder encarcelado ministro alcalde são paulo mercados recibido disgusto pérdidas quejas presidente electo corsé supone techo gasto preferían duda alguien liberal asumir riendas principal economía américa latina trimestre creció soló simultáneamente inflación desempleo moderandocuadrar sudoku ministerios infierno lula necesita satisfacer múltiples intereses partido pt corrientes ideológicas decena formaciones abrazaron liderazgo misión salvaguardar democracia brasileña logró apoyo antiguos adversarios situados derecha izquierda representación territorial brasil clave promesas futuro gobierno ministras negros indígenas reflejo dificultades conciliar tantas demandas lula avisado viernes iba ministerio pueblos originarios queda secretaría dependiente presidenciael único respiro apretada agenda política mundial compatriotas pierde partido enfunda camiseta amarilla izquierdistas dejaron medida convertía símbolo bolsonarista presidente electo confesado reciente operación garganta callado insistido ayuda divina curarme comentadola ayuda mensual cubrir necesidades acuciantes pobres basa antiguo bolsa familia programa aplaudido eficaz barato símbolo políticas progresistas pt llegar presidente jair bolsonaro rebautizó auxilio brasil quería arrebatarle izquierda potente marca electoral pandemia subió cuantía amplió cifra beneficiarios convirtió principales reclamos electorales realidad mantener paga reales promesa electoral bolsonaro lula único punto coincidencia visiones antagónicas extremoen tiempos pt cuantía bolsa familia tercio actual lula asumió inicio campaña podía tocar reales pretende retomar requisitos eliminados bolsonaro garantizar niños familias incluidas escuela vacunados embarazadas someten chequeos médicosbolsonaro logró fondos pagar ayuda diciembre mandato maniobra congreso renovó declaración emergencia pandemia amainado quedara excepciones contempladas saltarse límites constitucionales gasto público bolsonaro concurrir comicios auxilio brasil gancho atraer pobres insuficiente lula ganó millones votos</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Politica_59.txt</t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -1400,11 +1770,16 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>allá bomba insulina tradicional deseado páncreas artificial fase experimentación sistema pensado personas diabetes tipo conectados bomba sensor toma medidas constantemente niveles glucosa estudio publicado jama comunicación dispositivos reduce episodios hipoglucemia significativamente simple bombalo tecnología diseñada niveles glucosa disminuyen límite establecido médico automáticamente bomba suspende infusión insulina evita episodio hipoglucemia grave causar pérdida conciencia convulsiones coma muerte argumentan autores investigación realizada hospital infantil princesa margarita perth australiapero casos suspende administración insulina subraya mercedes galindo educadora especialista diabetes servicio endrocrinología nutrición hospital clínico san carlos madrid funcionamiento aparato requiriendo acción paciente ordenar bomba caso observar sensor niveles alterados glucosa contrario hablando páncreas artificial fase experimentaciónen caso ideal tratamiento diabetes tipo ventajas sistema suspensión administración insulina único bomba insulina demuestra investigación jama única centra subtipo pacientes diabetes tipo cuyo riesgo sufrir hipoglucemias graves remarca pratik choudhary autor editorial acompaña estudiolos investigadores hospital princesa margarita australia seleccionaron pacientes trastorno edad media años bomba insulina característica común peculiar nota síntomas alerta inminente hipoglucemia remedio decidimos individuos estudio ocurre pacientes diabetes tipo riesgo hipoglucemias graves preocupanes conoce hipoglucemias inadvertidas señala edelmiro menéndez endocrino hospital universitario central asturias mayoría diabéticos experimentan señales iniciales sudores temblores mareos malestar sensación hambre etc subgrupo pacientes advierten signos tomar medidas entrar coma conduciendo estrellarse grupo pacientes realmente preocupan puntualiza editorial jama hipoglucemias graves niños ocurren noche duermen remediopor razón equipo científicos australia evaluó eficacia mecanismos bomba insulina tradicional sistema incorpora sensor capacidad suspender administración insulinacon consiguieron reducir episodios hipoglucemia grave transcurso año grupo bomba insulina episodios mantienen redujo significativamente exposición valores mgdl mgdl grupo suspensión hipoglucemia comprobamos sistema capaz disminuir frecuencia duración episodios grupo pacientes especialmente riesgo reza artículoa resultados disponible mercado español demanda baja aseguran fuentes empresa comercializa medtronic motivos fundamentalmente económicos expertos consultados elmundoes bomba insulina financiada sistema nacional salud sensor</t>
+          <t>científico fruto años colaboración instituto medicina oncológica molecular asturias imoma universidad oviedo contado participación científicos ingleses alemanes revelado prelamina proteína causa envejecimiento acelerado capaz frenar progresión tumores malignoseste hallazgo supone avance comprensión relación mecanismos causan envejecimiento desencadenan cáncer resultados obtenidos publican martes revista nature communicationslas conclusiones publicación inspirar terapias cáncer refuerzan esperanzas depositadas estrategias ensayadas combatir envejecimiento aceleradoel codirigido carlos lópezotín catedrático universidad oviedo juan cadiñanos director laboratorio medicina molecular imoma labor experimental realizada jorge rosa saa becario predoctoral fundación maría cristina masaveu petersonel proyecto financiado fundación botín ministerio economía competitividad wellcome trust obra social cajastur fundación centro médico asturiasel envejecimiento cáncer procesos íntimamente relacionados conexiones complejas riesgo aparición tumores aumenta edad mecanismos favorecen envejecimiento frenan aparición desarrollo tumoresun mecanismos activación supresor tumoral estudiado proteína reveló proteína conocida prelamina responsable envejecimiento acelerado experimentan pacientes progeria capaz impedir avance tumores malignos investigadores asturianos utilizaron mosaicos ratones modificados genéticamente portan prelamina mitad células ratones prelamina células desarrollan envejecimiento acelerado viven meses dificulta estudio cáncer enfermedad desarrolle indicado jorge rosalos ratones mosaico viven ratones normales mantienen células prelamina tejidos vida permitido estudiar efecto proteína cáncer comentado juan cadiñanos</t>
         </is>
       </c>
       <c r="C75" t="n">
         <v>1</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Salud_32.txt</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -1413,11 +1788,16 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>método imágenes estructura cromosomas dibujando cuadro real forma rara científicos consejo biotecnología ciencias biológicas investigación bbsrc reino unido colaboración universidad cambridge reino unido instituto weizmann israel producido modelos muestran precisión compleja forma pliegan interior adnla forma utiliza describir cromosomas instantánea complejidad doctor peter fraser instituto barbraham financia bbsrc imagen cromosoma mancha forma adn familiar imagen microscópica cromosoma realidad muestra estructura produce transitoriamente células punto punto dividirse mayoría células organismo termina dividiendo cromosomas parecen forma cromosomas células forma imposible crear imágenes precisas estructura investigadorel equipo fraser desarrollado método visualizar forma consiste miles mediciones moleculares cromosomas células individuales utilizando tecnología secuenciación adn combinación pequeñas mediciones potentes ordenadores creado retrato tridimensional cromosomas tecnología gracias financiación bbsrc consejo investigación médica mrc wellcome trust reino unido imágenes únicas muestran estructura cromosoma camino adn permite mapear genes específicos características importantes modelos comenzado desentrañar principios básicos estructura cromosomas papel funcionamiento genoma fraseresta investigación publicada revista nature pone adn contexto célula transmitiendo belleza complejidad genoma mamíferos eficaz muestra estructura cromosomas forma adn interior pliega íntimamente relacionadas cantidad genes expresan consecuencias directas salud envejecimiento enfermedaddouglas kell directivo bbsrc sentencia comprensión estructura cromosómica limitado imágenes borrosas diagramas conocida ven división celular imágenes verdaderas ayudarán entender parecen cromosomas mayoría células cuerpo intrincados pliegues ayudan desentrañar cromosomas interactúan controlan funciones genoma</t>
+          <t>open australia dejado sonrisas lágrimas ranking circuito wta tenistas sonríen australiana ashleigh barty checa barbora krejcikova polaca iga swiatek estadounidense danielle collins barty logra ampliar liderato krejcikova swiatek collins suben posiciones establecerse topsin jugadoras pesado open australia provocado sufran caída considerable ranking wta semana jugadoras simona halep petra kvitova habituales top años semana figuran puestos clasificación cabe destacar caída bianca andreescu campeona us open semana aparece puesto especialmente llamativas graves caídas clasificación campeonas open australia japonesa naomi osaka campeona estadounidense sofia kenin campeona osaka desploma clasificación defender puntos campeona semana pierde posiciones figurar puesto puntos impactante caída ranking sofia kenin verse sorprendida ronda madison keys cae puestos semana aparece puesto puntostambién cae clasificación checa karolina muchova compitió open australia alcanzar semifinales año provocado semana pierda puestos baje puesto ranking situación similar estadounidense jennifer brady finalista open australia podido participar lesión razón brady perdido posiciones clasificación salido top quedarse puntoslas hermanas williams topla ausencia serena williams open australia serias consecuencias tenista estadounidense ranking semana serena williams aparece puesto clasificación puntos abajo aparece hermana venus semana figura puesto caer posiciones jugar partido oficial torneo chicago mes agosto</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Deportes_20.txt</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -1426,11 +1806,16 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>registro mundial trasplantes gestiona organización nacional trasplantes ont años colaboración organización mundial salud oms estima número trasplantes órganos sólidos efectuados mundo año representa aumento año trasplantesde riñón hígado corazón pulmón páncreas intestino único baja levemente año datos recogidos newsletter transplant publicación oficial comisión trasplantes consejo europasegún explicado europa press director organización nacional trasplantes ont rafael matesanz destacar aumento significativo trasplantes mundo añocuando visión global ocurriendo mundo ve realmente países creciendo inmensa mayoría tomado referencia sistema organizativo parecido español añadidoasí matesanz destaca crecimiento américa latina dato parado crecer españa empieza colaboración forma estructurada coordinadores programa alianza cooperación formación profesionales trasplantesel crecimiento donantes zona mundo zona mundo crecimiento añade concretamente publicación año efectuaron donantes órganos procedentes personas fallecidas aumento permitido trasplantes supone trasplantes año anteriorla publicación consejo europa incluye datos eeuu canadá australia países estancados cifras donación señala matesanz eeuu tasa donación permanece estable años oscila donantes millón personas canadá desciende puntos tasa donación sitúa australia eleva ligeramente alcanza donantes millón personasdel informe destacar fallos matesanz observa nivel mundial debería crecer velocidad creciendo realmente esfuerzos zonas mundo ritmo crecimiento debería destaca crecimiento donantes europa año crecido décimas pasando directiva europea donantes donantes millón personas significa crecido alegríasen futuro destacar evidencia países tomado enfoque modelo español copiado adoptado principales características creciendo mundo espera crecimiento países emergentes acaba producir principal fallo global</t>
+          <t>investigación contar carga viralexplorando vías tratamiento niños vihun laboratorio centro investigación natco sur india reutersun laboratorio centro investigación natco sur india reutersnuevos datos apoyan efectividad iniciar precozmente terapia niñostambién indican parar forma temporal tratamientocristina lucio madridactualizado miércoles horasdisminuye tamaño textoaumenta tamaño textoen año resultados preliminares estudio llevando cabo sudáfrica niños seropositivos supusieron cambio paradigma datos mostraban iniciar terapia antirretroviral forma temprana recién nacidos conseguía reducir mortalidad progresión enfermedad cambio dilatar comienzo tratamiento arrojaba consecuencias negativasdos años organización mundial salud cambiaba recomendaciones inmunológico pequeños situación clínica iniciase tratamiento antirretrovirales pequeños seropositivos menores añosla revista the lancet publicado resultados finales estudio datos vuelven apoyar efectividad iniciar forma temprana atención farmacológica niños vih apunta perspectiva terapéutica cuentaaunque punto corroborado análisis investigación sugiere interrumpir temporalmente terapia inicio efectivo seguro favorece progresión rápida enfermedadeste importante hallazgo indica parar forma temporal tratamiento evitar niños efectos tóxicos antirretrovirales seguimiento cuidadoso señalado comunicado mark cotton profesor universidad stellenbosch sudáfrica principales firmantes trabajotanto equipo revista médica comentario acompaña subrayan hipótesis ratificada diseño podido comparar efectos interrupción terapia seguir forma continuada tratamientono suficientes datos plazo consecuencias interrupción señalan robert colebunders victor mussime especialistas vih autores comentario publica the lancet añaden interrupciones tratamiento requieren monitorización cercana clínica inmunológica asegurar detección temprana progresión enfermedad restablecer tratamiento necesaria estrategia factible mayoría lugares recursos áfrica subsahariana viven niños vihde opinión claudia fortuny pediatra especialista atención niños vih hospital sant joan déu barcelona reconoce demuestra determinadas circunstancias parecería plausible interrumpir tratamiento</t>
         </is>
       </c>
       <c r="C77" t="n">
         <v>1</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Salud_28.txt</t>
+        </is>
       </c>
     </row>
     <row r="78">
@@ -1439,11 +1824,16 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>enfermedad mental adicciones ocupan plano atención médica abuso sustancias trastornos psiquiátricos reciben recursos dolencias resultados estudio animan pasar problemas plana sanidadsegún datos publicados revista the lancet impacto escala global pensaba subraya investigación males contribuyen medida vih tuberculosis generar enfermedad discapacidad mundonuestros resultados muestran creciente desafío enfermedades suponen sistemas sanitarios regiones desarrolladas vías desarrollo señalan investigadores revista médicaliderados harvey whiteford universidad queensland australia equipo científicos analizó datos salud mental abuso sustancias incluidos the global burden of disease study gbd estudio describir forma sistemática causas distribución principales enfermedades mundoen evaluación observaron enfermedades mentales trastornos relacionados abuso sustancias quinta causa muerte enfermedad mundo afinaron investigación midieron impacto dolencias capacidad generar trastornos letales encontraron problemas cabeza lista contribución discapacidad problemas calidad vida provocan trastornos notables subrayan investigadores hincapié número muertes debidas instancia enfermedad mental suicidios clasificándose categorías impacto infravalorándoseel análisis encontrado diferencias notables esperables distintas regiones mundo proporción trastornos relacionados alimentación alta zona australia asia áfrica subsaharianasegún datos enfermedades mentales abuso sustancias aumentado presencia décadas países vías desarrollo preocupante futuronuestras conclusiones implicaciones sustanciales agenda salud pública aumento esperanza vida supondrá personas enfermedades mentales trastornos relacionados sustancias vivirán periodo tiempopor publicado número the lancet dibuja detallado mapa consumo sustancias ilegales mundo anfetaminas cannabis cocaína opiáceos heroína enfermedades discapacidades generadas consumo tipo drogas aumentado incremento número población quinta aumento estima prevalencia personas adictas particularmente consumo opiaceos muertes atribuidas adicción drogas ocurridas piensa mitad produjeron dependencia opiáceosademás datos análisis revelan tercios adictos hombres diferencia cannabis droga consume mundo millones usuariospor opiáceos heroína sustancias problemas salud provocan mundoal acompaña revista médica investigación muestra importantes variaciones regionales dependencia cocaína elevada américa norte latinoamérica presencia regiones puramente anecdótica caso opiáceos mayores tasas consumo detectaron australia asia europa occidentalreino unido eeuu sudáfrica australia países problemas salud relacionaron consumo estupefacientes</t>
+          <t>belleza ojo espectador millones ojos coches fórmula contemplan drástico adición cabina protección presenta red bull aeroscreen opiniones míalos coches fórmula cabina abierta argumentar mediados años mercedes demostró tipo monza tendencia tiempos cambian requisitos descartar movimiento modelo coche reconocer movimiento conocemos enorme movimiento duda ofenderá sensibilidades seguro gente molestará comparación encantarán minoría probablemente jurará verá carrera salva vida vale pena quiero estrellas fórmula vivos problema protecciones propuestas coches quedar debemos capaces cascos pilotos claridad esconderlos escudo jenson button pasó historia diciendo prefiere aspecto coche cubierta presentada red bull – fundamentando opinión carreras lanchas solía disfrutar niño rodeado niño ciencia ficción películas xwing fighter luke skywalker muestran máquinas equipadas cabina dosel dirijo mirada red bull daniel ricciardo pista sochi mañana viernes observarlo miré punta nariz divertida pegajosa sección abruptamente angular similar forma alain prost llegar sección plana encontrarme cabina escudo antidisturbios lewis hamilton montado superioren paso flujo aspecto uniforme lotus cabina envolvente fachada – veo superficies constreñidas norma regulaciones modernas fórmula creado frontal coche diseñada personas piense millones dólares gastan año traducen coches abultados pregunta acerca culpar aerodinámica resultado formas cambio producir vuelta hora reglas cambien exigir aspecto atractivo sección frontal coches motogp debería prohibir alerones pensamiento niño molestaba coches producción línea salían forma caja aburridos lejanos gloriosos coches conceptos salones automóvil podían diseño frescoeso parecido conceptos visto red bull ferrari mclaren acerca visión futuro construye supercoche feo debemos aceptar cosa fórmula especialmente oportunidad reglas recuerdo conversación peter stevens diseñador icónico mclaren acerca narices actuales fórmula calificarlas abominaciones visuales entraron funcionamiento sugirió aerodinámica olvidado enseñado arte vea oportunidad presentar diseño atrozestoy ciento</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Deportes_2.txt</t>
+        </is>
       </c>
     </row>
     <row r="79">
@@ -1452,11 +1842,16 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>hablado consumo alcohol vinculación cáncer estudio viene constatar relación concretando riesgo ingesta bebe embarazo probabilidad cáncer mama aumenta comparación mujeres optan bebidas alcohólicasel estudio cuyos datos publicado revista journal of the national cancer institute establecido vínculo ingesta alcohol cáncer mama riesgo problema enfermedad benigna mama independientemente consumo alcohólico realice gestaciónestudios previos demostrado alcohol consumido año afecta riesgo cáncer mama mujer datos relación ingesta bebidas alcohólicas periodo menstruación mujer embarazo enfermedad tejido mamario particularmente susceptible agentes carcinógenos espacio temporalying liu escuela medicina universidad washington st louis unidos colegas analizaron datos enfermeras edades años historia médica reproductiva estilo vida gracias cuestionarios estudio salud enfermeras ii nhsiise obtuvieron datos consumo alcohol periodos edad preguntando participantes número bebidas alcohólicas consumían edades años excluir mujeres cumplían criterios estudio predeterminados incluyó análisis mujeres embarazo términoentre mujeres seleccionadas investigación registraron casos cáncer mama casos bbd periodo estudio confirmados médicos revisaron información historias clínicas pacienteel consumo alcohol mujer embarazo asoció riesgo cáncer mama bbd proliferativa independientemente bebida hubera tomado embarazo datos indicaron relación dependiente dosis significa alcohol toma mujer probabilidad desarrollar cáncer mama tomar gramos alcohol vinculó aumento riesgo cáncer mujeres tomaron gramos diarios alcohol unidades vaso vino riesgo investigadores informan beber alcohol embarazo asoció riesgo cáncer mama bbd constató retrasar maternidad hijos vincula probabilidad alta desarrollar tumorla consistencia patrones asociación alcohol riesgo bbd proliferativa cáncer mama apoya hipótesis ingesta alcohol especialmente embarazo probable tejido mama etapa vulnerable jugar papel importante etiología cáncer mama concluyen investigadores</t>
+          <t>tíos arcos flechas sonaba viejo cuento mitología cualquiera héroes pegados artilugio tiro arco gente españa sabía deporte relacionaban robin hood películas… explica juan carlos holgado cáceres miembro tridente antonio vázquez aller asturias alfonso menéndez presentes podio competición ponerse lanzar clavaron flechas dios cupido indiferenciaen diarios aparecían opciones medalla llegué tiro arco ponía ¡demoledor recuerda holgado lanzar flechas llevaba cupido dorada amor enamorar oro finlandia agosto subían vall dhebron olimpo elevado antonio rebollo arquero español excelencia arqueros españoles entrenador ucraniano victor sydoruklos arqueros españoles entrenador ucraniano victor sydoruk eduard omedesel flechazo antonio vázquez sangre fría sensible prisas flecha lanzar impacto amarillo puntos victoriosos marcador nervios miré reloj marcador simplemente pendiente gente chillaba oía sofrológico importante mariano espinosa explica rebollo inauguración difícil disparó flecha fuego caído llegar pebetero gente había…¡la liado asegura asturiano enero sponsor retiró patrocinio falta resultados ¡ellos perdieron añade pícara sonrisa vázquez contaba único objetivo pasar ronda dinamarca ronda liberamos asegurado beca año claves supimos jugar viento señala alfonso menéndez actualidad gerente club natación santa olaya gijón tantos flechazos gente encaprichó trío cuya cortado telediario amor repentino antonio look ideal celebridad abundante revolucionado pelo afro asustónos hicimos famosos golpe pelo afro decidí cortármelo pasar desapercibidoantonio vázquezyo reservado sentía agobiado anónimos fama futbolistas llegué pueblo asturias tardé hora recorrer metros casa peluquería gente agasajaba llegué peluquería dije barbero quitara pelo quería pasar desapercibido dudando ¡al salir tardé minuto volver casa camino explica partiéndose risa antonio vázquez entrenador federación catalana tiro arco monitor club olesa montserrat divina historia sobrehumano surgida flechas lanzadas años razón diarias crudeza dureza intransigente método soviético ucraniano victor sydoruk entrenador cincuentón vuelta coronel ejército urss campeón mundo tiro arco dejar lucha grecorromana lesión rodilla devoto teorías charles darwinholgado vázquez entreno competiciónholgado vázquez entreno competición pep moratalos quedamos juegos pura selección natural únicos lesionamos entrenamientos durísimos hacíamos sesiones nocturna cenar mandó golpe casa valían explica vázquez cascarrabias frecuente reparos sydoruk volcar rabia sentía ilustra anécdota holgadoyo quería campeonato regional madrid victor dejaba acabar cogió pechera llegamos manos puso doble entrenamiento desobediente guerra fría duro trato costó acostumbrarse cultura entendía pudiera utilizar instalación hora ocupada obsesión llegar españa pegó patada rabia piedra motivo rompió dedo pie mes escayolado disciplina ganar meses momentos tensión desgaste conllevaba familia caracteres superamos relata holgado director deportes federación internacional deporte universitariome emociona hablar victor sydoruk vive situación difícil ucraniaalfonso menéndezotra anécdota sucedió piscina natación formaba preparación física antonio sabía nadar victor ven enseñaré ¡le tiró agua alfonso rápido enseñarle método sydoruk supervivencia explica mondándose risa holgado hijo españoles nacido alemania trasladado años cáceres sentimiento sydoruk gratitud aspereza ternura hombre parco seco encajamos emociona recordar justo medalla victor ucraniano situación pasando suerte relación estrecha boda destaca voz quebrada alfonso menéndez sydoruk presidente federación tiro arco ucrania años energía admirable resalta holgadoalfonso menéndez foto actual oro barcelona medalla oro real orden mérito deportivo orden olímpicaalfonso menéndez foto actual oro barcelona medalla oro real orden mérito deportivo orden olímpica sergio vegasepultada dinamarca ronda cumplido expediente aguardaba relamiéndose favoritísimo oro equipo unificado nombre competían rusia resto países urss bálticos desintegración imperio soviético suerte echada abundante acumulado oyeron holgado vázquez menéndez susurrar mente arrebato patriótico sydorukya año rusos podéis perder sesiones castigo tema personal podíamos perder equipo rusia barcelona contento explica risas juan carlos semifinales tridente español despidió reino unido finlandia menéndez supimos jugar vientonosotros usábamos condones resto atletas villa ¡victor controladosjuan carlos holgadonuestra medalla explica puntuaciones hicimos sorpresa marcábamos entrenamientos pienso principal punto fuerte caracteres complementábamos virtud compensaba defecto extrovertido antonio introvertido alfonso punto compitiendo lanzaba miraba puntuación valoraba viento innovador equipo adaptara circunstancias destaca holgadojuan carlos holgado foto reciente orojuan carlos holgado foto reciente oroy vázquez menéndez holgado llevaron oro moldeado entrenamientos extenuantes convergencia caracteres concentración… abstinencia dormimos villa olímpica comimos entrenamos dormimos barcelona vivimos ambiente villa victor controlados decía villa dormir estadística quinto sexto juegos utilizan preservativos atleta ¡habría usaría vimos exclama carcajadas juan carlos holgado vieron afrodita lanzaron dorada flecha amor cupido españa gente tiro arco deporte medallistas olímpicos concluye holgado imprevistos héroes equipo español tiro arco bonita casualidad barcelona tiro arcocon gente miguel alvariño medalla olímpica ahoralo equipo español tiro arco barcelona aislado continuidad pudieron volver subir podio competición recortes plan ado alegrías juegos permanece única medalla olímpica españa deporte plata mundial victoria canadá josé ignacio catalán juan sancho antonio cerra único metal campeonato mundosin destaca figura gallego miguel alvariño junio alzó campeón europa tiro arco recurvo aupó número ránking mundial competición daniel castro gallego cuarto españa llevó plata equipos alvariño castro burgalés pablo acha predecesor alvariño prueba individual ganar título continental éxitos vienen creciendo abajo delegación española trajo medallas mundial juvenilelías cuesta trabajando seleccionador nacional haciéndose nombre miguel alvariño trabajado europeo logrado resultados arqueros golpe medalla olímpica destaca antonio vázquez metido tiro arco español entrenador federación catalana</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Deportes_50.txt</t>
+        </is>
       </c>
     </row>
     <row r="80">
@@ -1465,11 +1860,16 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>investigación contar carga viralexplorando vías tratamiento niños vihun laboratorio centro investigación natco sur india reutersun laboratorio centro investigación natco sur india reutersnuevos datos apoyan efectividad iniciar precozmente terapia niñostambién indican parar forma temporal tratamientocristina lucio madridactualizado miércoles horasdisminuye tamaño textoaumenta tamaño textoen año resultados preliminares estudio llevando cabo sudáfrica niños seropositivos supusieron cambio paradigma datos mostraban iniciar terapia antirretroviral forma temprana recién nacidos conseguía reducir mortalidad progresión enfermedad cambio dilatar comienzo tratamiento arrojaba consecuencias negativasdos años organización mundial salud cambiaba recomendaciones inmunológico pequeños situación clínica iniciase tratamiento antirretrovirales pequeños seropositivos menores añosla revista the lancet publicado resultados finales estudio datos vuelven apoyar efectividad iniciar forma temprana atención farmacológica niños vih apunta perspectiva terapéutica cuentaaunque punto corroborado análisis investigación sugiere interrumpir temporalmente terapia inicio efectivo seguro favorece progresión rápida enfermedadeste importante hallazgo indica parar forma temporal tratamiento evitar niños efectos tóxicos antirretrovirales seguimiento cuidadoso señalado comunicado mark cotton profesor universidad stellenbosch sudáfrica principales firmantes trabajotanto equipo revista médica comentario acompaña subrayan hipótesis ratificada diseño podido comparar efectos interrupción terapia seguir forma continuada tratamientono suficientes datos plazo consecuencias interrupción señalan robert colebunders victor mussime especialistas vih autores comentario publica the lancet añaden interrupciones tratamiento requieren monitorización cercana clínica inmunológica asegurar detección temprana progresión enfermedad restablecer tratamiento necesaria estrategia factible mayoría lugares recursos áfrica subsahariana viven niños vihde opinión claudia fortuny pediatra especialista atención niños vih hospital sant joan déu barcelona reconoce demuestra determinadas circunstancias parecería plausible interrumpir tratamiento</t>
+          <t>francia nicolas batum suspendido aire taponando balón prepelic puesta escena doncic argentina despedidas gasol scola imagen torneo baloncesto tokio francia sueñan salto batum prolongue llegue cielo selección vincent collet logre imposible madrugada viernes sábado ganar consecutivas unidos torneo oficial colgarse oro olímpico historia francia mandó vuelta casa unidos dongguan mundial china aparentes dificultades puntos fournier puntos rebotes gobert jornada fase grupos juegos fournier gobert repitieron actuación francia iluminada difícil pensar suficiente ahoraporque números team llegado saitama misión vengar derrotas francia limpiar nombre japón mundial cayó semifinal sorprendente grecia pese equipo campanillas fiasco atenas sensación chicos popovich llegaron dudas malhumorados japón extraña concentración vegas terminado entenderse jugamos países repiten equipo año año jugadores conocen campeonatos juntamos equipo menor consiguiendo lillard semifinal australiapopovich kerr team consciente desventaja verano vertebrar récord selecciones año bandera agarrarse líder define devin booker kevin durant años jugador washington echado team espalda ratitos apuro españa australia exhibido encontrado camino fino seda durant persigue tercer oro consecutivo convertiría leyenda juegos olímpicos puesto carmelo llegado cifra abriría puerta participación parís años vistalas apuestas volcadas favor unidos querido pegar pisotón acelerador francia necesita partido perfecto fournier gobert colo nivel semifinal luwawu jugador anónimo empezó romper eslovenia triple decisivo minuto aparezca noche larga francia viernes veremos avanzó scariolo oro reservado unidos</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Deportes_40.txt</t>
+        </is>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1878,16 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>organización mundial salud oms actualizado listado principales causas muerte mundo mantienen enfermedades transmisibles patologías coronarias accidentes cerebrovasculares enfermedad pulmonar obstructiva crónica epoc top ten aparece diabetes sale tuberculosiseste organismo naciones unidas utilizado datos relativos año estiman murieron mundo millones personas enfermedades transmisibles responsables fallecimientos millones años representaban muertes millonesla causa muerte siguen enfermedades cardiovasculares mataron millones personas representaron fallecimientos millones cardiopatía isquémica millones accidente cerebrovasculara ambas dolencias siguen ranking infecciones vías respiratorias inferiores causantes millones muertes enfermedad pulmonar obstructiva crónica epoc millones enfermedades diarreicas millones vihsida millones cánceres tráquea bronquios pulmón millones diabetes mellitus millones accidentes tráfico millones nacimientos prematuros peso nacer millonesprecisamente oms destaca top ten sale tuberculosis obstante principales causas muerte provocando millón fallecimientos informe destacan causas muerte variar países altos bajos ingresos países ricos enfermedades transmisibles representan muertes países bajos ingresos representan ganan protagonismo enfermedades infecciosas vihsida enfermedades diarreicas malaria tuberculosis representan tercio muertes paísestambién diferencias edad fallecidos países ingresos altos muertes producen personas años muertes niños menores años países bajos ingresos muertes producen años personas años máslas complicaciones derivadas parto prematuro asfixia lesiones nacer encuentran principales causas muerte cobrando vida recién nacidos lactantesen oms pone relieve millones niños murieron cumplir años países bajos medianos ingresos complicaciones nacer neumonía enfermedades diarreicas malaria importante causa muerte edades especialmente áfrica subsahariana causa muertes menores años fallecimientos franja edad produjo vida</t>
+          <t>diagnóstico cáncer mama llega zarpazo dudas miedos búsqueda pacientes familiares empiezan consultar cae manos enfermedad entran mitos leyendas mentiras repetición quedando cabeza tratara jornadas viaje cáncer mama celebrada madrid necesarias derribar verdades medias terminan losa tranquilidad afectados tumorel año auditorio escuchando contó hacía mes diagnosticado cáncer mama vine informarme sirvió importante recibir información sitio adecuado hablar expertos afirmaba jueves periodista inés ballester maestra ceremonias jornada hm universitario sanchinarro madridtanto pacientes presentes auditorio pudieron solventar dudas alimentación mano ricardo cubedo oncólogo hospital universitario puerta hierro majadahonda madrid derribó mitos enfermedad montón ideas falsas leyendas internet encontrar personas buscan información internet mira fecha actualización página diferencia paciente basaría respuesta clara concreta pregunta médicos objetivo móvil fabricando artículos científicos señalóde minutos especialista echó tierra ideas circulan foros cáncer soja fomentar tumores próstata prevenir mama constatado generalizado evidencia científica datos avalen consumo leche vaca influencia tumorhay terreno amplio mitos realidades desinformación ruido explica cubedo entrar profundidades enumeró leyendas sujetador aro causa cáncer mama desodorantes peligrosos teñirse pelo diagnóstico tumor</t>
         </is>
       </c>
       <c r="C81" t="n">
         <v>1</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Salud_19.txt</t>
+        </is>
       </c>
     </row>
     <row r="82">
@@ -1491,11 +1896,16 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>igualdad concepto términos generales positivo enfermedad cambios hábitos vida incorporación mujer consumo sustancias tóxicas igualdad extienda problemas típicos varón ictus conocido accidente cerebrovascular generando discapacidad planetadesde sustancias presentes cigarrillos tóxicas generan problemas relacionado pulmón cáncer insuficiencia respiratoria corazón tabaquismo aumenta riesgo sufrir ataque cardiacopero tabaco afecta órganos acción allá realidad tejido arteria pasen sustancias nocivas resultar dañado arterias riegan cerebro inmunes peligrolo ocurre tabaco arterias fomenta acumulación residuos denominados genéricamente placa ateromatosa placa estrechando calibre vaso sanguíneo pudiendo llegar cerrarse completamente circunstancias destruirse formar trombo desplazando torrente sanguíneo llega vaso pequeño cerebro produciendo obstrucciónen caso genera llamado ictus isquémico falta circulación zona cerebro muerte tejido derivar graves secuelas parálisis incapacidad hablar tipo ictus denominado hemorrágico genera similar grave supone rotura arteria hemorragia daños ampliossegún expertos españoles sufrirá ictus vida apunta estudio cuyos datos acaban publicar revista stroke mujeres fumadoras riesgo hombres fuman sufrir episodio tipo probabilidad menor mujeres consumen tabacotras analizar datos estudios internacionales ictus publicados investigadores universidad queensland brisbane australia encontraron tabaquismo relacionado riesgo sufrir ictus isquémico hombres mujeres</t>
+          <t>premio italia convirtió montaña emociones marcar drásticamente campeonato pilotos incidente max verstappen lewis hamilton ocasión diferencia sucedido silverstone quedaron eliminadoslos compases competencia destellos emociones arrancada clímax daniel ricciardo largó atacó interior verstappen arrebatarle plaza hamilton puso neerlandés ligero toque obligó salir circuito chicane permitió avance lando norris plaza dejando red bull coches casa wokingel virtual safety car apareció rápidamente consecuencia alfa romeo antonio giovinazzi cruzado golpeado posterior ferrari carlos sainz italiano ubicado primeras posiciones esperanza aspirar puntos carrera condenada finalizar ° frontal parrilla acciones valtteri bottas iniciaba remontada giro escandinavo mercedes zona puntos largado posterior cambio unidad potenciadaniel ricciardo pits giro colocando neumático duro verstappen siguiéndole vuelta posterior red bull perdió segundos detención falla pistolas cambio neumáticosal hamilton adelantó pista norris plaza líder campeonato regresó circuito mclaren británico perdido pitsa arrancar neumático duro hamilton entró colocar vuelta parada lenta segundos perder ritmo líderesal salir boxes empezó drama competencia campeón mundo extendió movimiento exterior curva arrinconar verstappen neerlandés cedió transitó chicana historia cambió neumáticos izquierdos tocó bordillos elevó monoplaza red bull desencadenar choque contendientes títuloel neumático trasero derecho rbb pasó halo mercedes finalmente posarse frontal obligar salida safety carde inmediato charles leclerc carlos sainz sergio pérez george russell valtteri bottas pilotos aprovecharon cumplir detención colocando duro excepción finlandés mercedes apostó cierrela carrera reinició giro ricciardo liderato seguido leclerc norris pérez sainz bottas británico mclaren atacó inmediato ferrari monegasco establecer casa wokingpérez desaprovechó sorpresa llevado leclerc atacó tomar posiciónsin adelantamiento mexicano vio ensombrecido salirse circuito concretar rebase recortar chicana acción considerada comisarios ilegal otorgaron sanción segundos finalbottas superó monegasco quitarle cuarto puesto enfocarse duelo directo mexicano red bull finlandés ataque giros logró mantener posición enfoque mantener mínima diferencia mexicano espera castigo segundos cruzar metanorris pidió mclaren dejarle atacar ricciardo boxes negaron posibilidad significaba equipo escuadra gp canadá australiano cruzó meta ventaja segundos norris bottas cerrando podio leclerc llevó cuarta plaza pérez finalizó quinto sanción aplicada justo ferrari sainz</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Deportes_6.txt</t>
+        </is>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1914,16 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>epidemias siglo obesidad considerada enfermedad mermando salud millones personas planeta motivo investigaciones centran luchar afecta países ricos países pobres estadounidense constata ratones ingesta moderada café té ayudar prevenir proteger hígado acumulación grasa conoce hígado grasoaunque mensajes lucha obesidad simples ejercicio dieta sana número personas sobrepeso obesidad aumentando país mujeres hombres obesos estima población hígado graso sigan buscando soluciones problema dispara tensión arterial ictus diabetesalgunas investigaciones tema centran precisamente prevenir aparición hígado graso conocido esteatosis hepática alcohólica vinculado riesgo diabetes procesos inflamatorios crónicos hígado derivar cirrosis cáncerun equipo internacional investigadores liderados paul yen rohit sinha universidad duke eeuu llevado cabo diversos experimentos cultivos celulares ratones comprobar reaccionaban presencia cafeína grasas almacenadas células hepáticas roedores alimentados dieta rica grasasegún datos experimentos publicados revista hepatology consumo equivalente tazas café té diarias beneficioso prevenir frente progresión hígado grasoeste estudio ofrece mecanismo detallado acción cafeína lípidos hígado resultados interesantes explica comunicado yen café té consumen frecuencia idea puedan terapéuticos especialmente ido ganándose reputación malos salud especialmente reveladora señalaestos investigadores señalan estudio datos conducir desarrollo fármacos actúen cafeína propiedades terapéuticas efectos habituales servir punto partida estudios evalúen beneficios cafeina cuerpo humanode actualidad marcha estudios efecto cafeína cuyos datos acaban publicar muestran moderación virtud señalan personas superan tazas café riesgo muerte problemas cardiovascularesen cambio mantenemos ingesta prudente sustancia efectos positivos variados protección frente hígado graso investigaciones evidenciado papel protector diabetes síntomas parkinson aliado memoria bondades té bebida alcanzaría galardones café observado reduce colesterol malo protección cardiovascular</t>
+          <t>barcelona nivel azulgrana volvieron demostrar europa candidatas lograr pleno títulos quieren puerta grande pleno victorias cuentan partidos temporada triunfos bayern demostración importantes bajas alexia mariona hansen equipo planeta pasaron bayern aguantó mitad acercamiento sucumbió geyse abrió marcador empezar golazos aitana pina fiesta camp nou espectadores batiendo récord fase gruposel barcelona salió azulgrana querían volver salir camp nou heroínas entrada coliseo azulgrana empezar aitana geyse ocasiones serios avisos bayern queria veía superado azulgrana cómodas crnogorcevic entrando derecha pina juntándose centro aitana dirigiendo orquesta geyse llegando bayern espacios hacía daño bühl remate lateral red ocasiones contadas notaba bávaras dinamita stanway evitar disparo activa aitana lados barcelona dominaba bayern esperaba ocasión canterana ocasión clarísima alto sendas llegadas área barcelona iba aprentando bayern intentando balón tramo aparecer grohs evitando gol olímpico mapi paradón aitana goles sensación barcelona merecía descansoen jugada rolfö internó izquierda cambió banda crnogorcevic asistió primeras geyse puso muralla alemana caía barcelona sabía straus dejar espacios barcelona cómodo quería media hora rolfö volvió internarse izquierda pase atrás metió aitana fondo red remate primeras premio merecido canterana motor equipo bayern intentaba asomar barcelona permitía guinda ′ pina sacó chistera golazo tiro área mandó escuadra camp nou fiesta giráldez empezó mover banquillo salma debutó champions bruna disfrutó camp nou barcelona quiso sangre tiro aitana oshoala gozó ocasiones nigeriana falta puntería bayern tiró toalla quería gol honra barcelona vuelve ganar camp nou muestra poderío fiesta azulgrana año pleno</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Deportes_28.txt</t>
+        </is>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1932,16 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>científico fruto años colaboración instituto medicina oncológica molecular asturias imoma universidad oviedo contado participación científicos ingleses alemanes revelado prelamina proteína causa envejecimiento acelerado capaz frenar progresión tumores malignoseste hallazgo supone avance comprensión relación mecanismos causan envejecimiento desencadenan cáncer resultados obtenidos publican martes revista nature communicationslas conclusiones publicación inspirar terapias cáncer refuerzan esperanzas depositadas estrategias ensayadas combatir envejecimiento aceleradoel codirigido carlos lópezotín catedrático universidad oviedo juan cadiñanos director laboratorio medicina molecular imoma labor experimental realizada jorge rosa saa becario predoctoral fundación maría cristina masaveu petersonel proyecto financiado fundación botín ministerio economía competitividad wellcome trust obra social cajastur fundación centro médico asturiasel envejecimiento cáncer procesos íntimamente relacionados conexiones complejas riesgo aparición tumores aumenta edad mecanismos favorecen envejecimiento frenan aparición desarrollo tumoresun mecanismos activación supresor tumoral estudiado proteína reveló proteína conocida prelamina responsable envejecimiento acelerado experimentan pacientes progeria capaz impedir avance tumores malignos investigadores asturianos utilizaron mosaicos ratones modificados genéticamente portan prelamina mitad células ratones prelamina células desarrollan envejecimiento acelerado viven meses dificulta estudio cáncer enfermedad desarrolle indicado jorge rosalos ratones mosaico viven ratones normales mantienen células prelamina tejidos vida permitido estudiar efecto proteína cáncer comentado juan cadiñanos</t>
+          <t>allá bomba insulina tradicional deseado páncreas artificial fase experimentación sistema pensado personas diabetes tipo conectados bomba sensor toma medidas constantemente niveles glucosa estudio publicado jama comunicación dispositivos reduce episodios hipoglucemia significativamente simple bombalo tecnología diseñada niveles glucosa disminuyen límite establecido médico automáticamente bomba suspende infusión insulina evita episodio hipoglucemia grave causar pérdida conciencia convulsiones coma muerte argumentan autores investigación realizada hospital infantil princesa margarita perth australiapero casos suspende administración insulina subraya mercedes galindo educadora especialista diabetes servicio endrocrinología nutrición hospital clínico san carlos madrid funcionamiento aparato requiriendo acción paciente ordenar bomba caso observar sensor niveles alterados glucosa contrario hablando páncreas artificial fase experimentaciónen caso ideal tratamiento diabetes tipo ventajas sistema suspensión administración insulina único bomba insulina demuestra investigación jama única centra subtipo pacientes diabetes tipo cuyo riesgo sufrir hipoglucemias graves remarca pratik choudhary autor editorial acompaña estudiolos investigadores hospital princesa margarita australia seleccionaron pacientes trastorno edad media años bomba insulina característica común peculiar nota síntomas alerta inminente hipoglucemia remedio decidimos individuos estudio ocurre pacientes diabetes tipo riesgo hipoglucemias graves preocupanes conoce hipoglucemias inadvertidas señala edelmiro menéndez endocrino hospital universitario central asturias mayoría diabéticos experimentan señales iniciales sudores temblores mareos malestar sensación hambre etc subgrupo pacientes advierten signos tomar medidas entrar coma conduciendo estrellarse grupo pacientes realmente preocupan puntualiza editorial jama hipoglucemias graves niños ocurren noche duermen remediopor razón equipo científicos australia evaluó eficacia mecanismos bomba insulina tradicional sistema incorpora sensor capacidad suspender administración insulinacon consiguieron reducir episodios hipoglucemia grave transcurso año grupo bomba insulina episodios mantienen redujo significativamente exposición valores mgdl mgdl grupo suspensión hipoglucemia comprobamos sistema capaz disminuir frecuencia duración episodios grupo pacientes especialmente riesgo reza artículoa resultados disponible mercado español demanda baja aseguran fuentes empresa comercializa medtronic motivos fundamentalmente económicos expertos consultados elmundoes bomba insulina financiada sistema nacional salud sensor</t>
         </is>
       </c>
       <c r="C84" t="n">
         <v>1</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Salud_23.txt</t>
+        </is>
       </c>
     </row>
     <row r="85">
@@ -1530,11 +1950,16 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>autoridad europea seguridad alimentaria aesa alertado papel térmico utilizado recibos compra supermercados alimentos fuente exposición bisfenol bpa consumidoreslos expertos agencia llevado cabo estudio cuyos resultados provisionales concluyen dieta constituye grupos población fuente exposición sustanciaademás revela contacto pensaba lactantes niños adultos estima exposición media vía alimentaria llega dosis diaria tolerable fijada aesalos científicos concluido asimismo niños años expuestos bisfenol dieta consumo alimentos relación peso corporal superior edadesel informe revisión riesgo exposición bisfenol agencia llevado cabo ocasión analizan fuentes alimenticias tipo papel térmico aireel papel térmico utiliza resguardos bancarios representa fuente contacto importante bisfenol alimentación pudiendo suponer exposición grupos población señala comunicado agenciano obstante aesa matiza falta datos particular absorción sustancia piel hábitos manejo resguardos compra ofrecer estimación precisa exposición víael estudio forma proceso fases pretende analizar riesgo global ligado sustancia etapa posterior autoridad alimentaria organizará consulta pública evaluar riesgos potenciales salud humanael bisfenol sustancia química presente plástico policarbonato fabrican botellas resinas recubrir interior latas comida bebidadistintos estudios científicos concluyen niveles bajos concentración bpa asociado diabetes obesidad infertilidad cáncer mama próstata problemas cardiovasculares alteraciones desarrollo neurológico cerebral trastornos comportamiento</t>
+          <t>aficionados sorprenderán mirar clasificación euroliga armani milan clasificado victorias jornadas situación crítica equipo aspirante año reforzó nombres importantes funcionando queda euroliga realidad victorias puestos playoffs analizamos causas naufragio italiano acumula derrotas consecutivaslesiones encadenadasla realidad justos armani milán prácticamente podido plantilla completa euroliga lesión duda marcado shavon shields problemas aquiles jornada daño partido bayern vuelto jugar sufren ausencia meses kevin pangos deja tocado puesto base perdieron compromisos billy baron naz mitrou long stefano tonut juega jornada luigi datome podido jugar partidos euroliga recién llegado luwawucabarrot retirar partido baskonia fuerte golpe cabeza impidió regresar encuentro carrusel bajas importantes shields recambio natural equipo reinventarse semana continuidaddudas confección plantillafue verano intenso milán marcha sergio rodríguez malcolm delaney provocaba cambio estructural importante equipo italiano apostó fuerte kevin pangos debía romper cska johaness voigtmann salió rusia planificación funcionando dupla bases pangos mitrou long jugar equipo resolutiva juego interior deshaun thomas fichajes juega minutos partido voigtmann promedia discretos puntos partido brandon davies superado valoración partidos euroliga rendimiento discreto incorporaciones caché europa cromos plantilla estructuradas rotaciones roles ataque gente niccolo melli voigtmann hines hall versión problema reajustar minutos roles equilibrio complejoproblemas ataquees evidente ataque milán funciona soluciones probado messina hablamos equipo puntos mete partido euroliga cazoo baskonia presentan rating ofensivo competición puntos posesiones porcentaje triples porcentaje tiros equipo línea tiro libre rebote ofensivo aparece rebotes ofensivos capturas totales ataque posesiones fluidez problemas encontrar ventajas ataque messina ido cambiando rotaciones obligado lesiones buscando soluciones conseguido atascos provocado problemas espaciado abuso media distancia tramos falta soluciones ofensivas jugadores devon hall promediando tiros triples cartas tiro equipo italiano temporadael puesto basees punto clave baloncesto europeo armani milán dando clave partidos kevin pangos recambio garantías ausencia mitroulong pangos lesionado mitroulong asumir rol costando partidos anotaciones zalgiris frente fenerbahçe choque cazoo baskonia desastre tiros valoración bases ganar euroliga messina derrota buesa arena equipo acudirá mercado ficharon luwawu cabarrot desmentido negociado facundo campazzo mitroulong seguir asumiendo peso ofensivo equipo dudas puesto toma decisiones errática pistala defensa único salvablesorprendentemente equipo italiano presenta defensa euroliga rating defensivo puntos encajados posesiones exterior bajar datos asistencias forzar pérdidas rival equipo muestra cara defensiva dato paradojico preocupante atasco resuelve cambio actitud baskonia partido sufrieron rebote ofensivo concediendo tope temporada problema milán resumen cemento bloque sólido defensa soluciones ataqueel caso brandon daviesen capítulo fichajes brandon davies llamado incorporaciones rindiendo nivel esperado encuentro baskonia escarmiento messina jugar duelo fenerbahçe volvió liga italiana brilló cazoo baskonia puntos rebotes encuentros superado puntos choques graves problemas faltas limitado promedia ′ pista puntos rebotes brandon davies determinante vimos tramos barcelona justificando fuerte inversión económica armani milán élmessinala realidad milán funciona banquillo institución europea ettore messina vemos equipo plano fantasía explosividad ofensiva jugadores años mike james sergio rodríguez kevin punter banquillo messina cómodoel equipo deprimido derrota baskonia semanas amagó dejar banquillo principal responsable equipo equipo juega siento responsable reunido equipo click único manejar situación italia euroliga seguimos jugando sacaré conclusiones iré señor armani diré necesario encontrar guía equipo perder efes llegado derrotas máshablamos técnico ascendencia enorme club responsabilidades director deportivo christos stavropoulos echar messina iría sucedió etapa real madrid capaz reconducir rumbo calendario llevará milán visitar oaka enfrentarse panathinaikos posteriormente recibir maccabi viajar belgrado enfrentarse estrella roja veremos cambia situación equipo italiano</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Deportes_32.txt</t>
+        </is>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1968,16 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>virus hepatitis afectan millones personas mundo millones mueren año epidemia silenciosa mayoría personas padecen desconocen infectados personas conocimiento acerca hepatitis potencial gravedad serias consecuencias salud calidad vida señala doctora carissa etienne directora organización panamericana salud ops vísperas mundial enfermedadla oms alertado países tomen medidas alerta prevención epidemia causa muertes minuto mundo número defunciones asociadas hepatitis personas mueren carreteras lesiones tráfico compara rafael mazin asesor principal vih organización mundial salud omsexisten tipos hepatitis mortales desencadenar cáncer hígado cirrosis detectan tratan doctor keiji fukuda director oms advertido infecciones silenciosas afectados presentan síntomas presentan graves daños alertado importancia hacerse pruebas deteccióneste año motivo mundial hepatitis celebra julio oms elaborado estudio países acerca virus identificar zonas índice riesgo infectados hepatitis seguir programa prevención inmunizacióndicho estudio reveló países cuentan plan escrito combatir infección cuentan unidades especializadas drogas inyectables relaciones sexuales riesgo tatuajes piercings transfusiones sanguíneas posibles vías contagioen oms comenzó programas advertencia hepatitis colaborado nivel mundial combatirla enfermedad supone pesada carga sistemas salud elevados costes tratamiento países principal causa trasplantes hígado medidas prevenir contagio virus hepatitis implantando compensar costes económicos tratamientos futuro explica doctor sylvie briand director epidemias pandemias omsla hepatitis inflamación hígado causada infección vírica tipos virus contagian distintas vías transmisión hepatitis comida agua contaminada tipo fluidos cuerpo sangre mantener relaciones sexuales protección otrasla oms aprobado vacunas prevención hepatitis incluido fármacos virus lista esencial medicinas recomienda adopten desarrollando guías tratamiento hepatitis</t>
+          <t>berlusconi incapaz vanidoso ineficaz descansa suficientesilvio berlusconi líder física políticamente débil causa frecuentes largas noches inclinación fiestas descanse suficiente retrato ministro italiano responsable asuntos americanos embajada unidos roma elisabeth dibble revelado mundo filtración wikileaksy documentos enviados embajada americana talia departamento eeuu referencia il cavaliere tipo incapaz vanidoso ineficaz líder moderno amante fiestas salvajespero suficiente diplomacia unidos muestra preocupada estrecha relación existente ministro italiano homólogo ruso vladimir putin relación estrecha estrecha ojos americanos berlusconi presenta portavoz putin europa relación líderes cimienta ojos diplomacia eeuu machismo compartido putin macho dominante político autoritario cuyo estilo machista permite conectar perfectamente berlusconi lee documentospero unidos sospecha fuerte amistad putin berlusconi apuntalado negocios despacho fecha enero hillary clinton secretaria norteamericana solicita cuerpo diplomático busque información relación personal putin berlusconi averigüe inversiones personales condicionar política exterior económicalos contenidos documentos filtrado muestran nivel descrédito ministro llevado imagen italia queja partido democrático principal formación oposición centroizquierda italiana juicio unidos ministro deprimente sostiene francesco rutelli líder centrista alianza italiasin ministro italiano exteriores franco frattini asegura revelaciones piensa realidad unidos gobierno italiano afectar relación países duda calificar filtración wikileaks septiembre diplomacia</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Politica_48.txt</t>
+        </is>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1986,16 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>enfermedades cardiovasculares siguen causa muerte mundo estadísticas actualizadas organización mundial salud oms patologías infecciosas cáncer patologías corazón tercios muertes mundo millones infecciones accidentes responsables tercio restantesegún datos oms millones personas fallecieron causa problema cardiovascular fallecimientos concretamente enfermedad isquémica infartos causó millones muertes accidentes cerebrovasculares ictus causaron millones defuncioneseste fenómeno exclusivo países ricos puesto millones muertes enfermedades comunicables registradas produjeron países bajos medios recursos oms recuerda muertes prematuras evitadas dieta saludable ejercicio físico abandonando tabacopor problemas corazón lista primeras causas muerte mundo encabezada cáncer diabetes afecta población mundial problemas pulmonares crónicos epoc enfisema años aprecia preocupante aumento víctimas cáncer pulmón pasan millones diabetes aumenta millones mundotambién incrementan víctimas accidentes tráfico costaron vida personas descienden víctimas partos prematuros pese top ten causas muerte calcula niños nace semana gestación tuberculosis dejado lista principales causas mortalidad mundoel vih permanece sexta posición dramático ranking causa menor número fallecimientos anuales millones esperanza vida niño nacido ronda años dependerá medida nacimiento oscilar años nacido oms preocupada millones niños mueren año mundo cumplir años causas fácilmente evitables infecciones mala atención parto mueren mujeres complicaciones embarazo parto</t>
+          <t>virus hepatitis afectan millones personas mundo millones mueren año epidemia silenciosa mayoría personas padecen desconocen infectados personas conocimiento acerca hepatitis potencial gravedad serias consecuencias salud calidad vida señala doctora carissa etienne directora organización panamericana salud ops vísperas mundial enfermedadla oms alertado países tomen medidas alerta prevención epidemia causa muertes minuto mundo número defunciones asociadas hepatitis personas mueren carreteras lesiones tráfico compara rafael mazin asesor principal vih organización mundial salud omsexisten tipos hepatitis mortales desencadenar cáncer hígado cirrosis detectan tratan doctor keiji fukuda director oms advertido infecciones silenciosas afectados presentan síntomas presentan graves daños alertado importancia hacerse pruebas deteccióneste año motivo mundial hepatitis celebra julio oms elaborado estudio países acerca virus identificar zonas índice riesgo infectados hepatitis seguir programa prevención inmunizacióndicho estudio reveló países cuentan plan escrito combatir infección cuentan unidades especializadas drogas inyectables relaciones sexuales riesgo tatuajes piercings transfusiones sanguíneas posibles vías contagioen oms comenzó programas advertencia hepatitis colaborado nivel mundial combatirla enfermedad supone pesada carga sistemas salud elevados costes tratamiento países principal causa trasplantes hígado medidas prevenir contagio virus hepatitis implantando compensar costes económicos tratamientos futuro explica doctor sylvie briand director epidemias pandemias omsla hepatitis inflamación hígado causada infección vírica tipos virus contagian distintas vías transmisión hepatitis comida agua contaminada tipo fluidos cuerpo sangre mantener relaciones sexuales protección otrasla oms aprobado vacunas prevención hepatitis incluido fármacos virus lista esencial medicinas recomienda adopten desarrollando guías tratamiento hepatitis</t>
         </is>
       </c>
       <c r="C87" t="n">
         <v>1</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Salud_34.txt</t>
+        </is>
       </c>
     </row>
     <row r="88">
@@ -1569,11 +2004,16 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>usos toxina botulínica seborrea psoriasis moléculas descubiertas capaces combatir cáncer piel dermatólogos ponen hallazgos científicos candentes año congreso nacional academia española dermatología venereología celebrando valencialos destacados relacionados tumores cutáneos interés encontrar medicamentos consigan tratar pacientes efectos secundarios forma rápida abarcando extensión moléculas vismodegib imiquimod diclofenacola terapia fotodinámica ingenol mebutato confirma carlos guillén jefe dermatología instituto valenciano oncología ivo presentada congreso anual sociedad americana oncología clínica asco labrolizumab capaz respuestas claras personas melanoma metastásico suerte mayoría melanomas detectan precoces curan problema extirpaciónen información filtros solares curvas cáncer piel melanoma melanoma dejado crecer señala joseph malvehy coordinador unidad melanoma hospital clínic barcelona década problema triplica estimamos españoles melanoma vida mayores años desarrolla carcinoma tipo cáncer piel melanomamalvehy liderado puesta marcha encuesta nacional hábitos solares presentado resultados definitivos especialista adelanta datos obtenidos parecen confirmar hipótesis españoles conscientes efectos exceso exposición solar cambian hábitos siguen saliendo centrales aplicándose crema protectora insuficiente playa minutos etc fallando encuestados asumían lunares iba dermatólogo población riesgo desarrollar melanoma acuden especialistatan importante investigación prevención reglas sencillas razón cumplen deseable aficiones expuestos radiaciones solares año deberían ropa adecuada gorros sombreros manga larga crema protección solar olvidar rayos ultravioleta tipo altos inviernolas personas oficinas necesitan filtro año basta protejan piel expuesta recomienda malvehy ideal extender capa miligramos centímetro cuadrado piel seca media hora exposición solar bañoen fotoprotectores orales remarca doctor refuerzan sustituyen protección solar componentes sumplementos alimenticios antioxidantes vitaminas carotenoides realmente protegen quemaduras complemento habituales recomendaciones aconsejamos pacientes riesgo</t>
+          <t>pspv eupv compromís pedido domingo alcaldesa valencia rita barberá dé explicaciones supuestos regalos valorados euros recibidos feria valencia aclare razón presentesasí solicitado grupos oposición raíz información publicada diario mundo fiscalía investiga marco diligencias gestión feria valencia regalos presuntamente entregados dirigentes pp alcaldesa fuentes recibido distintos complementos marcas lujoel portavoz socialista ayuntamiento joan calabuig advertido barberá fiscalía deja excusas seguir eludiendo asumir responsabilidad gestión feria valencia calidad recibía regalos institución ferial preguntado edil considerado inadmisible barberá pretenda eludir responsabilidades gestión entidades relacionadas consistorio aflorado presuntos casos corrupciónha incidido negativa pp aprobar pleno moción retirar cargos imputados cobra información aparece publicada miedo acaben imputados casos salpican ayuntamientoasí incidido regalos investiga fiscalía euros únicos procedencia dudosa recibe alcaldesa señalada reiteradas ocasiones receptora regalos lujo empresas entidades públicas emarsa investigada agujero contable millones eurosregalos álvaro pérez bigotes cabecilla trama gürtel valencia alcaldesa conversación telefónica interceptada policía curso investigación año aseguraba tienda louis vuitton comprándole bolso alcaldesa agregado calabuigcómplice necesariaen caso joan calabuig apuntado deriva feria valencia lamentable vuelto exigir barberá asuma responsabilidad política preside patronato nombra miembros comité ejecutivo miembros patronato visto ocupa cargo únicamente recibir regalos lujo criticadocon actitud barberá cómplice necesaria hundiendo feria valencia incapaz vigilar gestión evitar escándalo presuntos sobrecostes millonarios despilfarro agregadopor diputado eupv cortes víctor tormo señalado pp arruinado saqueado arcas generalitat feria valencia caso gobierno sale luz atraco arcas públicas regalos lujo alcaldesa regalos aceptó gustosamente valencianos engrosaban lista desempleados viendo peligrar casa dificultades llegar mes indicado tormo barberá debería dimitir inmediatamente obstante precisado esperamos decencia personajes esperamos justiciaasimismo compromís portavoz ayuntamiento joan ribó exigido explicaciones rita barberá presuntos regalos recibidos años dirección presidencia feria cometieron irregularidades investiga fiscalía anticorrupción informe elaborado intervención generalitat valencianaribó recordado barberá preside patronato feria valencia alcaldesa valencia figura estatutos entidad derecho público estatutos recogen operación comercial financiera supere euros aprobada patronatotodos conocemos predilección barberá firmas lujo desplazarse coche oficial rodeada escoltas vacaciones particulares gerencia feria valencia conocía gustos agasajaron bolsos pañuelos complementos comprados milla oro entregaban coche oficial pagado valencianos apuntadopor compromís exige barberá explique razón regalos preguntado barberá servirían patronato preside aprobará operaciones comerciales crédito euros</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Politica_27.txt</t>
+        </is>
       </c>
     </row>
     <row r="89">
@@ -1582,11 +2022,16 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>año vuelto demostrar oncología española envidiar países entorno mirar ojos estadounidense congreso cáncer mundo celebrado semana chicago resumir participación española pieza imposible abundante individual cooperación grupos internacionalesla sesión plenaria recoge estudios importantes presentados congreso contó participación española estudio estadounidense evaluó positivamente beneficio añadir bevacizumab quimioterapia aumentar supervivencia global cáncer cuello útero avanzado españa único país europeo aportó pacientes estudio estadounidense cambia práctica clínica entrada estudio envergadura pone relieve duda alta calidad investigación clínica española subrayó principal investigadora nacional oncóloga hospital vall dhebron ana oakninmás allá hall fama asco presencia española fructífera variada grupo español investigación cáncer mama geicam presentado trabajos conclusiones interesantes explica elmundoes miguel martín coordinador trabajos concluido sobrepeso extremo factor pronóstico cáncer mama efecto tratamiento apunta oncólogo mujeres obesas diagnosticadas enfermedad priorizar perder peso rápido posibleotro geicam basado multitudinario proyecto álamo analiza pacientes cáncer mama concluye afectadas enfermedad pariente grado sufrido datos conocían apunta martínla conjunción investigación básica clínica cabo españa protagonismo chicago mano director programa investigación traslacional centro nacional investigaciones oncológicas cnio manuel hidalgo investigadora equipo elena garralda presentado estudio pacientes secuenciado completamente exoma genes decidir tratamientos funcionar acorde mutaciones observadas acotadas posibles terapias utilizaron llamados ratones avatar introducen muestras tumor humano probar fármacos pacientes reduciendo posibilidades fracaso toxicidades pacientes españoles hospital madrid conseguido supervivencias importantes tipo tumores hablando resume hidalgo periódico descanso congreso participantes benefició ratones dispuestos probar fármaco enviado publicación revista alto impactorafael rosell espada oncología española desplazado chicago experto cáncer pulmón presentado diversos estudios quimioterapia seleccionada mutaciones tumor vía eficaz aumentar supervivencia cánceres letales comunicación oral presentada congreso oncólogo catalán demostrado pacientes hora empezar tratamiento responden independencia estadio tumor trabajos grupo investigación cáncer pulmón logrado aumentar supervivencia meses grupo enfermospor colaboración cancer therapeutics innovation group ctig rosell caído bondades secuenciación genómica completa hallazgos positivos demuestran reajusta tumor poquísimo inicio tratamiento personalizado desvelar alteraciones genómicas conocidas mutación egfr</t>
+          <t>centroderecha triunfa elecciones locales celebradas domingo ayuntamientos italia gracias impulso liga movimiento estrellas conquista ciudad prepara vuelta municipios examen recién estrenado gobierno giuseppe conte nacido pacto ultraderechista liga confirma aumento consenso favor liga ciudades presentaba coalición forza italia silvio berlusconi postfascistas hermanos italiaestoy contento alcaldes ciudadanos óptimos alcaldes exultante matteo salvini ministro interior líder liga resultados afluencia baja superó frente anteriores elecciones millones italianos llamados urnas confirmaron tendencia elecciones políticas marzo confianza liga alza líder indiscutible centroderechael movimiento estrellas presentaba ayuntamientos sufre frenazo perder alcaldía ragusa sicilia única capital provincia votó gobernaba actual alcalde grillino antonio tringali consiguió votos afrontar vuelta electoral municipios mil habitantes candidato supera sicilia celebra vuelta prevista junio mil habitantes suficiente alcanzar mayoría sufragiosel centroderecha presentará partido vuelta capitales provincia centroizquierda hará votabanlos resultados mejores esperados partido democrático pd perdedor elecciones generales marzo logró acceder vuelta bastiones históricos ciudades toscanas siena pisa única ciudad participación aumentó precedentes elecciones respiro partido atravesando grave crisis interna supera pelos examen gracias presentó coalición partidos izquierda pd cambiar abajo noticia muerte fuertemente exagerada ministro paolo gentiloni necesaria alternativa gobierno guiado salvini</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Politica_50.txt</t>
+        </is>
       </c>
     </row>
     <row r="90">
@@ -1595,11 +2040,16 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>congreso sociedad americana oncologia clínica asco congreso esperanza año oncólogos mundo comparten escenario avances torno lucha cáncer queda oncología especialidad viva avances tipos cáncer continuos casos brillan ausencia tumores cerebrales pertenecen categoríael único estudio presentado sesión plenaria selecciona trabajos importantes tumor cerebral alternativa afectados glioblastoma tumores cerebrales utiliza éxito línea cáncer recurrido funciona matando hambre vasos sanguíneos utiliza tumor alimentarse conoce angiogénesisel polémico coincidido presentación estudio importante participación española concluye contrariamente añadir fármaco antiangiogénico bevacizumab radio quimioterapia aumentaba supervivencia libre progresión mesesasí rueda prensa presentaron resultados preguntas relativas diferencia estudios potencial encontramos pacientes correctos estudio encontrado mark gilbert md anderson cancer center autor trabajoel neuroncólogo español juan manuel sepúlveda participado estudios valora diferencia trabajos cuestión diseño estudios rtog llama estadounidense excluyó pacientes inoperables constituyen administración antiangiogénico tardía avaglio nombre estudio europeo positivo estudio estadounidense permitía conoce crossover pacientes recurrían daba opción recibir fármaco mayoría pacientes tratado medicamentomás allá polémica siquiera estudio positivo permitía hablar reducción global mortalidad presentado asco sepúlveda defiende avances despacioeste especialista destaca cabo grupo español investigación neuroncología geino combina investigación básica puntera clínica señala cambiado radicalmente años asistido mejora radioterapia introducción quimioterapia bevacizumab tumor reproduce pequeñas noticias subraya especialistael problema tumores cerebrales activan alteraciones moleculares parecido pasa cáncer páncreas continuamente buscando punto débil apunta expertoesos presumibles puntos débiles frutos molécula dirigida proteína juega papel esencial tumores cerebrales tgf beta presentado resultados seguridad congreso equipo sepúlveda participando ensayos clínicos hospitales españolesno único fármaco estudio geino analiza eficacia inhibidor familia receptores her pacientes glioblastoma recurrente amplificaciones gen egfr destaca neuroncólogo español equipo biólogos instituto salud carlos iii dirigidos pilar sánchez acaban describir diana terapéutica glioblastomas proteína dyrkaquizás congresos noticias torno tumor cerebral</t>
+          <t>centroamérica enfrentando epidemia dengue vive constatado organización panamericana salud ops señalado presencia cepa agresiva virus costado vida centenar personas contagiado regióntal informaba conferencia prensa socorro gross representante ops nicaragua serotipo agresivo virus propagó rápidamente américa central actual temporada lluviassegún cifras oficiales dengue cobrado vidas centroamérica honduras nicaragua guatemala salvador costa rica fallecido informa personas contagiadas cifra alta país años elevada centroaméricapor presidente nicaragua daniel ortega muertes registrado afectados enero decretado alerta roja sanitaria contener epidemiaa autoridades honduras sanitarias san pedro sula ciudad importante honduras elevado nivel alarma umbral emergencia médica registrado casos periodo año contabilizan enfermos denguese variante peligrosa enfermedad indicado médicos fronteras msf comunicado ong prestando servicios hondureños afectadosla epidemia dengue representa amenaza población hondureña empezamos visto flujo constante pacientes incluyendo casos graves niños explicado coordinador médico msf doctor luis neirasegún podido constatar ong agosto subida casos sospechosos dengue fecha año pasadonicaragua medidas implantar urgente realizará jornadas fumigación mosquito aedes aegyti vector transmite infección movilizarán miles brigadistas salud mañana país brigadistas llevarán instrucciones correspondientes detectar casos sospechosos dengue visitas casa casa remitirlos inmediato unidades salud evaluación clínicalos síntomas enfermedad fiebre dolor cabeza cuerpo casos graves deshidratación grave hemorragias internas conducen muerteexiste situación desastre calamidad país señala rosa murillo dama portavoz oficial centros salud hospitales públicos encuentran atestados enfermosel mosquito transmisor dengue incuba larvas depósitos agua limpia cáscaras huevo macetas vacías llantas automóvil patios jardines viviendas negocios oficinas</t>
         </is>
       </c>
       <c r="C90" t="n">
         <v>1</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Salud_16.txt</t>
+        </is>
       </c>
     </row>
     <row r="91">
@@ -1608,11 +2058,16 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>vitaminas lociones champús tratamientos cosméticos utilizados tratar alopecia efectividad médica frenan caída cabello asegurado coordinador unidad tricología hospital ramón cajal madrid sergio vañó jornada trastornose problema médico necesita valoración adecuado tratamiento combatirlo cien causas origina pérdida pelo terapia frene definitivamente problema métodos técnicas médicas ayudan retrasar tipos alopecia tratamientos factores crecimiento farmacológicos asegurado especialista demostrado efectivos perfil seguridadahora múltiples factores originan alopecia vañó recordado comunes hormonales provocan alopecia androgenética producidos cambios ritmo vida originan alopecia efluvio telógena autoinmunes ocasionan conocida alopecia areataéstas formas frecuentes causas caída pelo trastornos alimentarios déficit hierro alteraciones tiroides provocadas determinados medicamentos enfermedades sistémicas señalado vañótodos proseguido factores afectan importante calidad vida pacientes demostrado alopecia enfermedades cutáneas procesos afecta calidad vida personasademás experto informado mujeres padecen cáncer plantean someterse tratamientos quimioterapia evitar caída pelo darle nivel médico institucional importancia proceso pacientes pasan apostilladodicho vañó explicado principales líneas investigación médica enfermedad centrado medicina regenerativa factores crecimiento células madre obstante reconocido diez años marcha aplicación prácticapor dermatólogo participado curso actualización tricología organizado hospital ramón cajal insistido importancia personas sufren caídas severas cabello acudan especialista farmacéutico centro cosmético médicos capaces retrasar eficazmente alopecialos pacientes problema médico piensan cosmético acuden centros belleza realidad alopecia enfermedad hipertensión diabetes requiere valoración adecuado tratamiento médico zanjado</t>
+          <t>pedro sánchez juega elecciones domingo celebran meses victoria primarias psoe autoridad partido fase construcción resistiría precario liderazgo debacle histórica urnas socialistas superados cómputo global votos fuerza hegemónica izquierda incapaces recuperar feudos históricos arrebató pp extremadura castillala mancha probablemente psoe cosechó elecciones municipales celebradas años resultado historia votos sánchez siquiera soñar rozar listón irrupción fuerza ciudadanos partidos cuño existían salvando distancias elecciones generales locales autonómicas suelen primar rostros siglas barómetro centro investigaciones sociológicas cis daba psoe intención voto comicios legislativos salvar cara sáncheznecesitaría arrebatar pp extremadura castillala mancha comunidades autónomas manos socialistas única excepción estaúltima legislaturay conservar principado asturias único territorio andalucía gobierna psoe escenario –es perder asturias josé antonio monago maría dolores cospedal siguieran mando extremadura castillala mancha respectivamente–sería sinónimo cataclismo situación castillala mancha resulta especialmente endiablada cospedal sondeo cis perdería mayoría absoluta comunidad obtendría escaños socialista emiliano garcíapage lograría décimas populares intención voto tomaría iniciativa formar gobierno comunidad cospedal investida presidenta apoyo ciudadanos escaños partido albert riverarespaldaría pp inclinaría psoe aire futuro político extremadura gobernada años pp apoyo natura iu cis otorga socialistas guillermo fernández vara horquilla escaños alejados marcan umbral mayoría absoluta psoe alcanzar cota apoyo cis lograría diputados populares quedarían puertas objetivo voto parlamentarios barómetro concede ciudadanospedro sánchez miedo quede rajoy asturias dibuja igualmente complejo mosaico apoyos cruzados determinante papel ciudadanos psoe gobierna principado volvería ganar elecciones gobernar respaldo formación lidera pablo iglesias –el presidente asturiano javier fernández ve simpatía podemos– pp hacerse ejecutivo autonómico lograra respaldo ciudadanos foro asturias partido creado exministro popular francisco álvarez cascos recientes elecciones andaluzas mérito pírrica victoria socialista susana díaz protagonizó deliberadamente campaña medida injerencias ferraz domingo miradas clavadas sánchez mérito psoe salva muebles reforzando precario liderazgo secretario partido losresultados calamitosos dudan tardarían alzarse voces reclamaran cabeza caso primarias convocadas julio contar probablemente aspirante</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Politica_22.txt</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>